<commit_message>
E-gradanin sheet sortiraj pls
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Desktop\Karlo\FER\Semestar_5\Projekt R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\projektRrepo\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3A6246-FF6F-47A0-8F43-70B3E03878DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE47E41-1904-44BA-9FB6-346050C2476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="7" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Umrli" sheetId="3" r:id="rId6"/>
     <sheet name="Brakovi" sheetId="8" r:id="rId7"/>
     <sheet name="Razvodi" sheetId="5" r:id="rId8"/>
+    <sheet name="E-građani" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="147">
   <si>
     <t>2001.</t>
   </si>
@@ -673,16 +674,90 @@
       <t>3)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Naziv županije </t>
+  </si>
+  <si>
+    <t>Broj jedinstvenih korisnika</t>
+  </si>
+  <si>
+    <t>Udjel (%)</t>
+  </si>
+  <si>
+    <t>Bjelovarsko-Bilogorska Županija</t>
+  </si>
+  <si>
+    <t>Brodsko-Posavska Županija</t>
+  </si>
+  <si>
+    <t>Dubrovačko-Neretvanska Županija</t>
+  </si>
+  <si>
+    <t>Istarska Županija</t>
+  </si>
+  <si>
+    <t>Karlovačka Županija</t>
+  </si>
+  <si>
+    <t>Koprivničko-Križevačka Županija</t>
+  </si>
+  <si>
+    <t>Krapinsko-Zagorska Županija</t>
+  </si>
+  <si>
+    <t>Ličko-Senjska Županija</t>
+  </si>
+  <si>
+    <t>Međimurska Županija</t>
+  </si>
+  <si>
+    <t>Osječko-Baranjska Županija</t>
+  </si>
+  <si>
+    <t>Požeško-Slavonska Županija</t>
+  </si>
+  <si>
+    <t>Primorsko-Goranska Županija</t>
+  </si>
+  <si>
+    <t>Sisačko-Moslavačka Županija</t>
+  </si>
+  <si>
+    <t>Splitsko-Dalmatinska Županija</t>
+  </si>
+  <si>
+    <t>Šibensko-Kninska Županija</t>
+  </si>
+  <si>
+    <t>Varaždinska Županija</t>
+  </si>
+  <si>
+    <t>Virovitičko-Podravska Županija</t>
+  </si>
+  <si>
+    <t>Vukovarsko-Srijemska Županija</t>
+  </si>
+  <si>
+    <t>Zadarska Županija</t>
+  </si>
+  <si>
+    <t>Zagrebačka Županija</t>
+  </si>
+  <si>
+    <t>UKUPNO</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="166" formatCode="[$-1041A]0.00%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -747,8 +822,34 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -773,8 +874,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8064A2"/>
+        <bgColor rgb="FF8064A2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0DA"/>
+        <bgColor rgb="FFCCC0DA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4DFEC"/>
+        <bgColor rgb="FFE4DFEC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -836,6 +955,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD3D3D3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -844,7 +1015,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -899,6 +1070,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1210,7 +1438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1224,7 +1452,7 @@
       <selection activeCell="A3" sqref="A3:V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="7" customWidth="1"/>
     <col min="2" max="17" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
@@ -1233,7 +1461,7 @@
     <col min="23" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>31</v>
       </c>
@@ -1301,7 +1529,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
@@ -1369,7 +1597,7 @@
         <v>3878981</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" s="20" t="s">
         <v>73</v>
       </c>
@@ -1437,7 +1665,7 @@
         <v>768054</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" s="20" t="s">
         <v>72</v>
       </c>
@@ -1505,7 +1733,7 @@
         <v>105393</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" s="20" t="s">
         <v>54</v>
       </c>
@@ -1573,7 +1801,7 @@
         <v>120670</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" s="20" t="s">
         <v>57</v>
       </c>
@@ -1641,7 +1869,7 @@
         <v>159747</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
@@ -1709,7 +1937,7 @@
         <v>70648</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8" s="20" t="s">
         <v>63</v>
       </c>
@@ -1777,7 +2005,7 @@
         <v>64384</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9" s="20" t="s">
         <v>58</v>
       </c>
@@ -1845,7 +2073,7 @@
         <v>101358</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="A10" s="20" t="s">
         <v>59</v>
       </c>
@@ -1913,7 +2141,7 @@
         <v>102205</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="A11" s="20" t="s">
         <v>68</v>
       </c>
@@ -1981,7 +2209,7 @@
         <v>143678</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="A12" s="20" t="s">
         <v>64</v>
       </c>
@@ -2049,7 +2277,7 @@
         <v>130844</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="A13" s="20" t="s">
         <v>56</v>
       </c>
@@ -2117,7 +2345,7 @@
         <v>112357</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22">
       <c r="A14" s="20" t="s">
         <v>66</v>
       </c>
@@ -2185,7 +2413,7 @@
         <v>258719</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22">
       <c r="A15" s="20" t="s">
         <v>55</v>
       </c>
@@ -2253,7 +2481,7 @@
         <v>140131</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22">
       <c r="A16" s="20" t="s">
         <v>61</v>
       </c>
@@ -2321,7 +2549,7 @@
         <v>42931</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22">
       <c r="A17" s="20" t="s">
         <v>70</v>
       </c>
@@ -2389,7 +2617,7 @@
         <v>195326</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22">
       <c r="A18" s="20" t="s">
         <v>53</v>
       </c>
@@ -2457,7 +2685,7 @@
         <v>299983</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22">
       <c r="A19" s="20" t="s">
         <v>67</v>
       </c>
@@ -2525,7 +2753,7 @@
         <v>96722</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22">
       <c r="A20" s="20" t="s">
         <v>71</v>
       </c>
@@ -2593,7 +2821,7 @@
         <v>115714</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22">
       <c r="A21" s="20" t="s">
         <v>69</v>
       </c>
@@ -2661,7 +2889,7 @@
         <v>423849</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22">
       <c r="A22" s="20" t="s">
         <v>60</v>
       </c>
@@ -2729,7 +2957,7 @@
         <v>266183</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22">
       <c r="A23" s="20" t="s">
         <v>65</v>
       </c>
@@ -2797,11 +3025,11 @@
         <v>160085</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1"/>
+    <row r="25" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1"/>
+    <row r="26" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1"/>
+    <row r="27" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1"/>
+    <row r="28" spans="1:22" s="22" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
@@ -2825,14 +3053,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2843,7 +3071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2860,7 +3088,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2874,7 +3102,7 @@
         <v>3547614</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2888,7 +3116,7 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2902,7 +3130,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2916,7 +3144,7 @@
         <v>24131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2930,7 +3158,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -2944,7 +3172,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +3186,7 @@
         <v>7862</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2972,7 +3200,7 @@
         <v>10315</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2986,7 +3214,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -3000,7 +3228,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -3014,7 +3242,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3028,7 +3256,7 @@
         <v>17980</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -3042,7 +3270,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3056,7 +3284,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -3070,7 +3298,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -3084,7 +3312,7 @@
         <v>3688</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -3098,7 +3326,7 @@
         <v>7729</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -3112,7 +3340,7 @@
         <v>123892</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -3126,7 +3354,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -3140,7 +3368,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3154,7 +3382,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -3168,7 +3396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -3182,7 +3410,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -3196,7 +3424,7 @@
         <v>22178</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -3210,7 +3438,7 @@
         <v>12712</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -3224,7 +3452,7 @@
         <v>22388</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3249,13 +3477,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="4" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -3275,7 +3503,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -3298,7 +3526,7 @@
         <v>0.52676872898244653</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -3321,7 +3549,7 @@
         <v>0.52251222204699577</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>99</v>
       </c>
@@ -3344,7 +3572,7 @@
         <v>0.51673267105280107</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>100</v>
       </c>
@@ -3367,7 +3595,7 @@
         <v>0.51604802727129095</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>101</v>
       </c>
@@ -3390,7 +3618,7 @@
         <v>0.51536484705592189</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -3413,7 +3641,7 @@
         <v>0.51866608375061407</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3436,7 +3664,7 @@
         <v>0.51776230376096088</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3472,14 +3700,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="7" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.2" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -3541,7 +3769,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -3604,7 +3832,7 @@
         <v>91851</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -3666,7 +3894,7 @@
         <v>17364</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
@@ -3728,7 +3956,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -3791,7 +4019,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -3853,7 +4081,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -3915,7 +4143,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -3977,7 +4205,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -4039,7 +4267,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -4101,7 +4329,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -4163,7 +4391,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -4225,7 +4453,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -4287,7 +4515,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -4349,7 +4577,7 @@
         <v>5137</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="8" t="s">
         <v>55</v>
       </c>
@@ -4411,7 +4639,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
@@ -4473,7 +4701,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
@@ -4535,7 +4763,7 @@
         <v>5419</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
@@ -4598,7 +4826,7 @@
         <v>5996</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -4660,7 +4888,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
@@ -4722,7 +4950,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="8" t="s">
         <v>69</v>
       </c>
@@ -4784,7 +5012,7 @@
         <v>10018</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -4846,7 +5074,7 @@
         <v>7470</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="8" t="s">
         <v>65</v>
       </c>
@@ -4925,7 +5153,7 @@
       <selection activeCell="A3" sqref="A3:Y23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="7" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="7" customWidth="1"/>
@@ -4939,7 +5167,7 @@
     <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -5016,7 +5244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -5093,7 +5321,7 @@
         <v>36508</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -5170,7 +5398,7 @@
         <v>8030</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
@@ -5247,7 +5475,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -5324,7 +5552,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -5401,7 +5629,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -5478,7 +5706,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -5555,7 +5783,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -5632,7 +5860,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -5709,7 +5937,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -5786,7 +6014,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -5863,7 +6091,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -5940,7 +6168,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -6017,7 +6245,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="8" t="s">
         <v>55</v>
       </c>
@@ -6094,7 +6322,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
@@ -6171,7 +6399,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
@@ -6248,7 +6476,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
@@ -6325,7 +6553,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -6402,7 +6630,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
@@ -6479,7 +6707,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="8" t="s">
         <v>69</v>
       </c>
@@ -6556,7 +6784,7 @@
         <v>4211</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -6633,7 +6861,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="8" t="s">
         <v>65</v>
       </c>
@@ -6735,7 +6963,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="7" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="7" customWidth="1"/>
@@ -6749,7 +6977,7 @@
     <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -6826,7 +7054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -6903,7 +7131,7 @@
         <v>62712</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -6980,7 +7208,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
@@ -7057,7 +7285,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -7134,7 +7362,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -7211,7 +7439,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -7288,7 +7516,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -7365,7 +7593,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -7442,7 +7670,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -7519,7 +7747,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -7596,7 +7824,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -7673,7 +7901,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -7750,7 +7978,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -7827,7 +8055,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="8" t="s">
         <v>55</v>
       </c>
@@ -7904,7 +8132,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
@@ -7981,7 +8209,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
@@ -8058,7 +8286,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
@@ -8135,7 +8363,7 @@
         <v>4428</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -8212,7 +8440,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
@@ -8289,7 +8517,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="8" t="s">
         <v>69</v>
       </c>
@@ -8366,7 +8594,7 @@
         <v>6005</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -8443,7 +8671,7 @@
         <v>4588</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="8" t="s">
         <v>65</v>
       </c>
@@ -8547,7 +8775,7 @@
       <selection activeCell="A3" sqref="A3:Y23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="7" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="7" customWidth="1"/>
@@ -8561,7 +8789,7 @@
     <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -8638,7 +8866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -8715,7 +8943,7 @@
         <v>18203</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -8792,7 +9020,7 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
@@ -8869,7 +9097,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -8946,7 +9174,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -9023,7 +9251,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -9100,7 +9328,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -9177,7 +9405,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -9254,7 +9482,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -9331,7 +9559,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -9408,7 +9636,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -9485,7 +9713,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -9562,7 +9790,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -9639,7 +9867,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="8" t="s">
         <v>55</v>
       </c>
@@ -9716,7 +9944,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
@@ -9793,7 +10021,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
@@ -9870,7 +10098,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
@@ -9947,7 +10175,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -10024,7 +10252,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
@@ -10101,7 +10329,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="8" t="s">
         <v>69</v>
       </c>
@@ -10178,7 +10406,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -10255,7 +10483,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="8" t="s">
         <v>65</v>
       </c>
@@ -10352,9 +10580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5010BC67-7950-4090-BE5A-0AABB8636ABD}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="7" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="7" customWidth="1"/>
@@ -10368,7 +10596,7 @@
     <col min="26" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>31</v>
       </c>
@@ -10445,7 +10673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -10522,7 +10750,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
@@ -10599,7 +10827,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
@@ -10676,7 +10904,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
@@ -10753,7 +10981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="8" t="s">
         <v>57</v>
       </c>
@@ -10830,7 +11058,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="8" t="s">
         <v>62</v>
       </c>
@@ -10907,7 +11135,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="8" t="s">
         <v>63</v>
       </c>
@@ -10984,7 +11212,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -11061,7 +11289,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="8" t="s">
         <v>59</v>
       </c>
@@ -11138,7 +11366,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="8" t="s">
         <v>68</v>
       </c>
@@ -11215,7 +11443,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="8" t="s">
         <v>64</v>
       </c>
@@ -11292,7 +11520,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="8" t="s">
         <v>56</v>
       </c>
@@ -11369,7 +11597,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="8" t="s">
         <v>66</v>
       </c>
@@ -11446,7 +11674,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="8" t="s">
         <v>55</v>
       </c>
@@ -11523,7 +11751,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="8" t="s">
         <v>61</v>
       </c>
@@ -11600,7 +11828,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="8" t="s">
         <v>70</v>
       </c>
@@ -11677,7 +11905,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="8" t="s">
         <v>53</v>
       </c>
@@ -11754,7 +11982,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="8" t="s">
         <v>67</v>
       </c>
@@ -11831,7 +12059,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="8" t="s">
         <v>71</v>
       </c>
@@ -11908,7 +12136,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="8" t="s">
         <v>69</v>
       </c>
@@ -11985,7 +12213,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="8" t="s">
         <v>60</v>
       </c>
@@ -12062,7 +12290,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="8" t="s">
         <v>65</v>
       </c>
@@ -12153,4 +12381,429 @@
 Ažurirano/ Updated: 26.7.2022.</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AAEE19-D059-4936-963D-F2F96734F6BC}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="57.6">
+      <c r="A1" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="25"/>
+    </row>
+    <row r="2" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A2" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="29">
+        <v>12742</v>
+      </c>
+      <c r="F2" s="37">
+        <v>1.7770624775112799E-2</v>
+      </c>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.4">
+      <c r="A3" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="32">
+        <v>17932</v>
+      </c>
+      <c r="F3" s="33">
+        <v>2.5008856024746701E-2</v>
+      </c>
+      <c r="G3" s="25"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.4">
+      <c r="A4" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="29">
+        <v>17568</v>
+      </c>
+      <c r="F4" s="30">
+        <v>2.4501203582575799E-2</v>
+      </c>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.4">
+      <c r="A5" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="32">
+        <v>194034</v>
+      </c>
+      <c r="F5" s="33">
+        <v>0.27060943396752701</v>
+      </c>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" ht="14.4">
+      <c r="A6" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="29">
+        <v>40350</v>
+      </c>
+      <c r="F6" s="30">
+        <v>5.6274110004379201E-2</v>
+      </c>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.4">
+      <c r="A7" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="32">
+        <v>18760</v>
+      </c>
+      <c r="F7" s="33">
+        <v>2.61636258657287E-2</v>
+      </c>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.4">
+      <c r="A8" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="29">
+        <v>17884</v>
+      </c>
+      <c r="F8" s="30">
+        <v>2.49419128455593E-2</v>
+      </c>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.4">
+      <c r="A9" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="32">
+        <v>16629</v>
+      </c>
+      <c r="F9" s="33">
+        <v>2.3191627639723E-2</v>
+      </c>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.4">
+      <c r="A10" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="29">
+        <v>6664</v>
+      </c>
+      <c r="F10" s="30">
+        <v>9.2939447105125899E-3</v>
+      </c>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" ht="14.4">
+      <c r="A11" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="32">
+        <v>19532</v>
+      </c>
+      <c r="F11" s="33">
+        <v>2.72402953309922E-2</v>
+      </c>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" ht="14.4">
+      <c r="A12" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="29">
+        <v>44641</v>
+      </c>
+      <c r="F12" s="30">
+        <v>6.2258551293816397E-2</v>
+      </c>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" ht="14.4">
+      <c r="A13" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="32">
+        <v>9128</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1.27303612421307E-2</v>
+      </c>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.4">
+      <c r="A14" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="29">
+        <v>62650</v>
+      </c>
+      <c r="F14" s="30">
+        <v>8.73747953351761E-2</v>
+      </c>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" ht="14.4">
+      <c r="A15" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="32">
+        <v>22907</v>
+      </c>
+      <c r="F15" s="33">
+        <v>3.1947237617603798E-2</v>
+      </c>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:7" ht="14.4">
+      <c r="A16" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="29">
+        <v>65260</v>
+      </c>
+      <c r="F16" s="30">
+        <v>9.1014830703489105E-2</v>
+      </c>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="1:7" ht="14.4">
+      <c r="A17" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="32">
+        <v>13268</v>
+      </c>
+      <c r="F17" s="33">
+        <v>1.8504210447041002E-2</v>
+      </c>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.4">
+      <c r="A18" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="29">
+        <v>26286</v>
+      </c>
+      <c r="F18" s="30">
+        <v>3.6659758502481099E-2</v>
+      </c>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" ht="14.4">
+      <c r="A19" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="32">
+        <v>10163</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1.41738235433583E-2</v>
+      </c>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" ht="14.4">
+      <c r="A20" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="29">
+        <v>22098</v>
+      </c>
+      <c r="F20" s="30">
+        <v>3.08189661183834E-2</v>
+      </c>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" ht="14.4">
+      <c r="A21" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="32">
+        <v>25266</v>
+      </c>
+      <c r="F21" s="33">
+        <v>3.52372159447496E-2</v>
+      </c>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.4">
+      <c r="A22" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="29">
+        <v>47346</v>
+      </c>
+      <c r="F22" s="30">
+        <v>6.6031078370937704E-2</v>
+      </c>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.4">
+      <c r="A23" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="32">
+        <v>5918</v>
+      </c>
+      <c r="F23" s="33">
+        <v>8.2535361339756193E-3</v>
+      </c>
+      <c r="G23" s="25"/>
+    </row>
+    <row r="24" spans="1:7" ht="14.4">
+      <c r="A24" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="35">
+        <v>717026</v>
+      </c>
+      <c r="F24" s="36">
+        <v>1</v>
+      </c>
+      <c r="G24" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Sretan Bozic u fileu grafoviZaPrikaz.Rmd su brakoiRazvodi
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\ProjektR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9516558F-639C-418C-A588-669C7EA076A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AE5082-AE3C-4AE6-9BAB-6AB702A96B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -281,7 +281,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -484,7 +484,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -540,23 +540,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -869,7 +868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -883,7 +882,7 @@
       <selection activeCell="A23" sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="17" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
@@ -892,7 +891,7 @@
     <col min="23" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -960,7 +959,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1028,7 +1027,7 @@
         <v>3878981</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>768054</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>105393</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>120670</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -1300,7 +1299,7 @@
         <v>159747</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -1368,7 +1367,7 @@
         <v>70648</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -1436,7 +1435,7 @@
         <v>64384</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -1504,7 +1503,7 @@
         <v>101358</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -1572,7 +1571,7 @@
         <v>102205</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -1640,7 +1639,7 @@
         <v>143678</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>130844</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -1776,7 +1775,7 @@
         <v>112357</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>258719</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -1912,7 +1911,7 @@
         <v>140131</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>42931</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>195326</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -2116,7 +2115,7 @@
         <v>299983</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>96722</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>115714</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -2320,7 +2319,7 @@
         <v>423849</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -2388,7 +2387,7 @@
         <v>266183</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -2456,11 +2455,11 @@
         <v>160085</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
@@ -2482,29 +2481,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF10406A-7DA4-4C95-BD29-6EE4B84A0747}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1">
         <v>2001</v>
       </c>
       <c r="C1">
         <v>2011</v>
       </c>
-      <c r="D1" s="21">
+      <c r="D1">
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2520,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2535,7 +2534,7 @@
         <v>3547614</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2563,7 +2562,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>24131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2604,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>7862</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2633,7 +2632,7 @@
         <v>10315</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2661,7 +2660,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2675,7 +2674,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>17980</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2745,7 +2744,7 @@
         <v>3688</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2759,7 +2758,7 @@
         <v>7729</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2773,7 +2772,7 @@
         <v>123892</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2787,7 +2786,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2801,7 +2800,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2815,7 +2814,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2829,7 +2828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -2843,7 +2842,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2857,7 +2856,7 @@
         <v>22178</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2871,7 +2870,7 @@
         <v>12712</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>22388</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2912,14 +2911,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -2948,44 +2947,44 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="11">
-        <f>B3+B4</f>
+        <f t="shared" ref="B2:I2" si="0">B3+B4</f>
         <v>3933022</v>
       </c>
       <c r="C2" s="11">
-        <f>C3+C4</f>
+        <f t="shared" si="0"/>
         <v>4159696</v>
       </c>
       <c r="D2" s="11">
-        <f>D3+D4</f>
+        <f t="shared" si="0"/>
         <v>4426221</v>
       </c>
       <c r="E2" s="11">
-        <f>E3+E4</f>
+        <f t="shared" si="0"/>
         <v>4601469</v>
       </c>
       <c r="F2" s="11">
-        <f>F3+F4</f>
+        <f t="shared" si="0"/>
         <v>4784265</v>
       </c>
       <c r="G2" s="11">
-        <f>G3+G4</f>
+        <f t="shared" si="0"/>
         <v>4437460</v>
       </c>
       <c r="H2" s="11">
-        <f>H3+H4</f>
+        <f t="shared" si="0"/>
         <v>4284889</v>
       </c>
       <c r="I2" s="11">
-        <f>I3+I4</f>
+        <f t="shared" si="0"/>
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -3014,7 +3013,7 @@
         <v>1865129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3056,14 +3055,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.2" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3187,7 @@
         <v>91851</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -3250,7 +3249,7 @@
         <v>17364</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -3375,7 +3374,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -3499,7 +3498,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -3561,7 +3560,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -3623,7 +3622,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -3685,7 +3684,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -3747,7 +3746,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -3809,7 +3808,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -3933,7 +3932,7 @@
         <v>5137</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -4057,7 +4056,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>5419</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -4182,7 +4181,7 @@
         <v>5996</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -4306,7 +4305,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -4368,7 +4367,7 @@
         <v>10018</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -4430,7 +4429,7 @@
         <v>7470</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -4509,7 +4508,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -4523,7 +4522,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -4600,7 +4599,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -4677,7 +4676,7 @@
         <v>36508</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -4754,7 +4753,7 @@
         <v>8030</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -4908,7 +4907,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -4985,7 +4984,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -5062,7 +5061,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -5216,7 +5215,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -5293,7 +5292,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -5370,7 +5369,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -5447,7 +5446,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -5524,7 +5523,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -5601,7 +5600,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -5755,7 +5754,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -5832,7 +5831,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -5909,7 +5908,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -5986,7 +5985,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -6063,7 +6062,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -6140,7 +6139,7 @@
         <v>4211</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -6217,7 +6216,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -6321,7 +6320,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -6335,7 +6334,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -6412,7 +6411,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -6489,7 +6488,7 @@
         <v>62712</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -6566,7 +6565,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -6720,7 +6719,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -6797,7 +6796,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -6874,7 +6873,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -6951,7 +6950,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -7105,7 +7104,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -7182,7 +7181,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -7259,7 +7258,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -7336,7 +7335,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -7413,7 +7412,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -7490,7 +7489,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -7567,7 +7566,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -7644,7 +7643,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -7721,7 +7720,7 @@
         <v>4428</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -7798,7 +7797,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -7875,7 +7874,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -7952,7 +7951,7 @@
         <v>6005</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -8029,7 +8028,7 @@
         <v>4588</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -8133,7 +8132,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -8147,7 +8146,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -8224,7 +8223,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -8301,7 +8300,7 @@
         <v>18203</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -8378,7 +8377,7 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -8455,7 +8454,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -8532,7 +8531,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -8609,7 +8608,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -8763,7 +8762,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -8840,7 +8839,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -8917,7 +8916,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -8994,7 +8993,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -9071,7 +9070,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -9148,7 +9147,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -9225,7 +9224,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -9302,7 +9301,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -9379,7 +9378,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -9456,7 +9455,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -9533,7 +9532,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -9610,7 +9609,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -9687,7 +9686,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -9764,7 +9763,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -9841,7 +9840,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -9942,7 +9941,7 @@
       <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -9956,7 +9955,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -10033,7 +10032,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -10110,7 +10109,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -10187,7 +10186,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -10264,7 +10263,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -10341,7 +10340,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -10418,7 +10417,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -10495,7 +10494,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -10572,7 +10571,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -10649,7 +10648,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -10726,7 +10725,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -10803,7 +10802,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -10880,7 +10879,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -10957,7 +10956,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -11034,7 +11033,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -11111,7 +11110,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -11188,7 +11187,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -11265,7 +11264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -11342,7 +11341,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -11419,7 +11418,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -11496,7 +11495,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -11573,7 +11572,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -11650,7 +11649,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -11747,233 +11746,233 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9AAEE19-D059-4936-963D-F2F96734F6BC}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:3" ht="14.4">
+      <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:3" ht="14.4">
+      <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <f>SUM(B3:B24)</f>
         <v>717026</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A3" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>194034</v>
       </c>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>19532</v>
       </c>
       <c r="C4" s="20"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="22">
         <v>16629</v>
       </c>
       <c r="C5" s="20"/>
     </row>
-    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>26286</v>
       </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>10163</v>
       </c>
       <c r="C7" s="20"/>
     </row>
-    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A8" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>9128</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+    <row r="9" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A9" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>17884</v>
       </c>
       <c r="C9" s="20"/>
     </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>12742</v>
       </c>
       <c r="C10" s="20"/>
     </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>22098</v>
       </c>
       <c r="C11" s="20"/>
     </row>
-    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+    <row r="12" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>17932</v>
       </c>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="23">
+      <c r="B13" s="22">
         <v>18760</v>
       </c>
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+    <row r="14" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="22">
         <v>44641</v>
       </c>
       <c r="C14" s="20"/>
     </row>
-    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+    <row r="15" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A15" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="22">
         <v>22907</v>
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+    <row r="16" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A16" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="22">
         <v>6664</v>
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="22">
         <v>40350</v>
       </c>
       <c r="C17" s="20"/>
     </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A18" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="22">
         <v>47346</v>
       </c>
       <c r="C18" s="20"/>
     </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A19" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="23">
+      <c r="B19" s="22">
         <v>13268</v>
       </c>
       <c r="C19" s="20"/>
     </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A20" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="22">
         <v>17568</v>
       </c>
       <c r="C20" s="20"/>
     </row>
-    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+    <row r="21" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="22">
         <v>65260</v>
       </c>
       <c r="C21" s="20"/>
     </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="22">
         <v>62650</v>
       </c>
       <c r="C22" s="20"/>
     </row>
-    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+    <row r="23" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A23" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="22">
         <v>25266</v>
       </c>
       <c r="C23" s="20"/>
     </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:3" ht="14.4" customHeight="1">
+      <c r="A24" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="22">
         <v>5918</v>
       </c>
       <c r="C24" s="20"/>
     </row>
-    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.4">
       <c r="C25" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add migrations in population
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\ProjektR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AE5082-AE3C-4AE6-9BAB-6AB702A96B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64CC767-895B-42EC-A5A5-E9BC35D55973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Brakovi" sheetId="8" r:id="rId7"/>
     <sheet name="Razvodi" sheetId="5" r:id="rId8"/>
     <sheet name="E-gradani" sheetId="9" r:id="rId9"/>
+    <sheet name="Migracije" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="98">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -271,6 +272,81 @@
   <si>
     <t>85+</t>
   </si>
+  <si>
+    <t>Zupanije</t>
+  </si>
+  <si>
+    <t>Broj_stanovnika_2011</t>
+  </si>
+  <si>
+    <t>Broj_stanovnika_2021</t>
+  </si>
+  <si>
+    <t>Doseljeni_2011</t>
+  </si>
+  <si>
+    <t>Odseljeni_2011</t>
+  </si>
+  <si>
+    <t>Doseljeni_2012</t>
+  </si>
+  <si>
+    <t>Odseljeni_2012</t>
+  </si>
+  <si>
+    <t>Doseljeni_2013</t>
+  </si>
+  <si>
+    <t>Odseljeni_2013</t>
+  </si>
+  <si>
+    <t>Doseljeni_2014</t>
+  </si>
+  <si>
+    <t>Odseljeni_2014</t>
+  </si>
+  <si>
+    <t>Doseljeni_2015</t>
+  </si>
+  <si>
+    <t>Odseljeni_2015</t>
+  </si>
+  <si>
+    <t>Doseljeni_2016</t>
+  </si>
+  <si>
+    <t>Odseljeni_2016</t>
+  </si>
+  <si>
+    <t>Doseljeni_2017</t>
+  </si>
+  <si>
+    <t>Odseljeni_2017</t>
+  </si>
+  <si>
+    <t>Doseljeni_2018</t>
+  </si>
+  <si>
+    <t>Odseljeni_2018</t>
+  </si>
+  <si>
+    <t>Doseljeni_2019</t>
+  </si>
+  <si>
+    <t>Odseljeni_2019</t>
+  </si>
+  <si>
+    <t>Doseljeni_2020</t>
+  </si>
+  <si>
+    <t>Odseljeni_2020</t>
+  </si>
+  <si>
+    <t>Doseljeni_2021</t>
+  </si>
+  <si>
+    <t>Odseljeni_2021</t>
+  </si>
 </sst>
 </file>
 
@@ -281,7 +357,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -868,7 +944,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -882,7 +958,7 @@
       <selection activeCell="A23" sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="17" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
@@ -891,7 +967,7 @@
     <col min="23" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -959,7 +1035,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1103,7 @@
         <v>3878981</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -1095,7 +1171,7 @@
         <v>768054</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -1163,7 +1239,7 @@
         <v>105393</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -1231,7 +1307,7 @@
         <v>120670</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -1299,7 +1375,7 @@
         <v>159747</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -1367,7 +1443,7 @@
         <v>70648</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -1435,7 +1511,7 @@
         <v>64384</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -1503,7 +1579,7 @@
         <v>101358</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -1571,7 +1647,7 @@
         <v>102205</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -1639,7 +1715,7 @@
         <v>143678</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1707,7 +1783,7 @@
         <v>130844</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -1775,7 +1851,7 @@
         <v>112357</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -1843,7 +1919,7 @@
         <v>258719</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -1911,7 +1987,7 @@
         <v>140131</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -1979,7 +2055,7 @@
         <v>42931</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -2047,7 +2123,7 @@
         <v>195326</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -2115,7 +2191,7 @@
         <v>299983</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -2183,7 +2259,7 @@
         <v>96722</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -2251,7 +2327,7 @@
         <v>115714</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -2319,7 +2395,7 @@
         <v>423849</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -2387,7 +2463,7 @@
         <v>266183</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -2455,11 +2531,11 @@
         <v>160085</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
-    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
-    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
-    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
-    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
@@ -2477,22 +2553,1736 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0FD2C1-80AD-4861-A1E7-BB4C1BEC8857}">
+  <dimension ref="A1:Y22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="25" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" t="s">
+        <v>93</v>
+      </c>
+      <c r="V1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>790017</v>
+      </c>
+      <c r="C2">
+        <v>767131</v>
+      </c>
+      <c r="D2">
+        <v>14304</v>
+      </c>
+      <c r="E2">
+        <v>12165</v>
+      </c>
+      <c r="F2">
+        <v>13194</v>
+      </c>
+      <c r="G2">
+        <v>11042</v>
+      </c>
+      <c r="H2">
+        <v>14715</v>
+      </c>
+      <c r="I2">
+        <v>11844</v>
+      </c>
+      <c r="J2">
+        <v>16061</v>
+      </c>
+      <c r="K2">
+        <v>13021</v>
+      </c>
+      <c r="L2">
+        <v>16513</v>
+      </c>
+      <c r="M2">
+        <v>14381</v>
+      </c>
+      <c r="N2">
+        <v>16492</v>
+      </c>
+      <c r="O2">
+        <v>13786</v>
+      </c>
+      <c r="P2">
+        <v>16253</v>
+      </c>
+      <c r="Q2">
+        <v>15250</v>
+      </c>
+      <c r="R2">
+        <v>18787</v>
+      </c>
+      <c r="S2">
+        <v>15545</v>
+      </c>
+      <c r="T2">
+        <v>20338</v>
+      </c>
+      <c r="U2">
+        <v>16641</v>
+      </c>
+      <c r="V2">
+        <v>16569</v>
+      </c>
+      <c r="W2">
+        <v>14946</v>
+      </c>
+      <c r="X2">
+        <v>19412</v>
+      </c>
+      <c r="Y2">
+        <v>18549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>113804</v>
+      </c>
+      <c r="C3">
+        <v>105250</v>
+      </c>
+      <c r="D3">
+        <v>2046</v>
+      </c>
+      <c r="E3">
+        <v>2194</v>
+      </c>
+      <c r="F3">
+        <v>1608</v>
+      </c>
+      <c r="G3">
+        <v>1772</v>
+      </c>
+      <c r="H3">
+        <v>1851</v>
+      </c>
+      <c r="I3">
+        <v>2086</v>
+      </c>
+      <c r="J3">
+        <v>2172</v>
+      </c>
+      <c r="K3">
+        <v>2604</v>
+      </c>
+      <c r="L3">
+        <v>2094</v>
+      </c>
+      <c r="M3">
+        <v>2516</v>
+      </c>
+      <c r="N3">
+        <v>2130</v>
+      </c>
+      <c r="O3">
+        <v>2847</v>
+      </c>
+      <c r="P3">
+        <v>2163</v>
+      </c>
+      <c r="Q3">
+        <v>3249</v>
+      </c>
+      <c r="R3">
+        <v>2506</v>
+      </c>
+      <c r="S3">
+        <v>3396</v>
+      </c>
+      <c r="T3">
+        <v>2902</v>
+      </c>
+      <c r="U3">
+        <v>3210</v>
+      </c>
+      <c r="V3">
+        <v>2754</v>
+      </c>
+      <c r="W3">
+        <v>3017</v>
+      </c>
+      <c r="X3">
+        <v>3120</v>
+      </c>
+      <c r="Y3">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>132892</v>
+      </c>
+      <c r="C4">
+        <v>120702</v>
+      </c>
+      <c r="D4">
+        <v>1717</v>
+      </c>
+      <c r="E4">
+        <v>1837</v>
+      </c>
+      <c r="F4">
+        <v>1707</v>
+      </c>
+      <c r="G4">
+        <v>1876</v>
+      </c>
+      <c r="H4">
+        <v>2024</v>
+      </c>
+      <c r="I4">
+        <v>2176</v>
+      </c>
+      <c r="J4">
+        <v>2081</v>
+      </c>
+      <c r="K4">
+        <v>2329</v>
+      </c>
+      <c r="L4">
+        <v>2223</v>
+      </c>
+      <c r="M4">
+        <v>2494</v>
+      </c>
+      <c r="N4">
+        <v>2025</v>
+      </c>
+      <c r="O4">
+        <v>2651</v>
+      </c>
+      <c r="P4">
+        <v>2174</v>
+      </c>
+      <c r="Q4">
+        <v>2608</v>
+      </c>
+      <c r="R4">
+        <v>2508</v>
+      </c>
+      <c r="S4">
+        <v>2775</v>
+      </c>
+      <c r="T4">
+        <v>3059</v>
+      </c>
+      <c r="U4">
+        <v>2748</v>
+      </c>
+      <c r="V4">
+        <v>2856</v>
+      </c>
+      <c r="W4">
+        <v>2541</v>
+      </c>
+      <c r="X4">
+        <v>3410</v>
+      </c>
+      <c r="Y4">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>175951</v>
+      </c>
+      <c r="C5">
+        <v>159487</v>
+      </c>
+      <c r="D5">
+        <v>2490</v>
+      </c>
+      <c r="E5">
+        <v>2424</v>
+      </c>
+      <c r="F5">
+        <v>2432</v>
+      </c>
+      <c r="G5">
+        <v>2556</v>
+      </c>
+      <c r="H5">
+        <v>2508</v>
+      </c>
+      <c r="I5">
+        <v>2753</v>
+      </c>
+      <c r="J5">
+        <v>2865</v>
+      </c>
+      <c r="K5">
+        <v>3429</v>
+      </c>
+      <c r="L5">
+        <v>3035</v>
+      </c>
+      <c r="M5">
+        <v>3579</v>
+      </c>
+      <c r="N5">
+        <v>2891</v>
+      </c>
+      <c r="O5">
+        <v>3725</v>
+      </c>
+      <c r="P5">
+        <v>2824</v>
+      </c>
+      <c r="Q5">
+        <v>4007</v>
+      </c>
+      <c r="R5">
+        <v>3580</v>
+      </c>
+      <c r="S5">
+        <v>3946</v>
+      </c>
+      <c r="T5">
+        <v>4183</v>
+      </c>
+      <c r="U5">
+        <v>4165</v>
+      </c>
+      <c r="V5">
+        <v>3701</v>
+      </c>
+      <c r="W5">
+        <v>3662</v>
+      </c>
+      <c r="X5">
+        <v>3954</v>
+      </c>
+      <c r="Y5">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>84836</v>
+      </c>
+      <c r="C6">
+        <v>70368</v>
+      </c>
+      <c r="D6">
+        <v>1315</v>
+      </c>
+      <c r="E6">
+        <v>1641</v>
+      </c>
+      <c r="F6">
+        <v>1268</v>
+      </c>
+      <c r="G6">
+        <v>1715</v>
+      </c>
+      <c r="H6">
+        <v>1387</v>
+      </c>
+      <c r="I6">
+        <v>1830</v>
+      </c>
+      <c r="J6">
+        <v>1514</v>
+      </c>
+      <c r="K6">
+        <v>2220</v>
+      </c>
+      <c r="L6">
+        <v>1377</v>
+      </c>
+      <c r="M6">
+        <v>2549</v>
+      </c>
+      <c r="N6">
+        <v>1413</v>
+      </c>
+      <c r="O6">
+        <v>2637</v>
+      </c>
+      <c r="P6">
+        <v>1276</v>
+      </c>
+      <c r="Q6">
+        <v>2866</v>
+      </c>
+      <c r="R6">
+        <v>1441</v>
+      </c>
+      <c r="S6">
+        <v>2662</v>
+      </c>
+      <c r="T6">
+        <v>1494</v>
+      </c>
+      <c r="U6">
+        <v>2660</v>
+      </c>
+      <c r="V6">
+        <v>1482</v>
+      </c>
+      <c r="W6">
+        <v>2018</v>
+      </c>
+      <c r="X6">
+        <v>1435</v>
+      </c>
+      <c r="Y6">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>78034</v>
+      </c>
+      <c r="C7">
+        <v>64084</v>
+      </c>
+      <c r="D7">
+        <v>1304</v>
+      </c>
+      <c r="E7">
+        <v>1989</v>
+      </c>
+      <c r="F7">
+        <v>1173</v>
+      </c>
+      <c r="G7">
+        <v>1983</v>
+      </c>
+      <c r="H7">
+        <v>1361</v>
+      </c>
+      <c r="I7">
+        <v>1778</v>
+      </c>
+      <c r="J7">
+        <v>1613</v>
+      </c>
+      <c r="K7">
+        <v>2313</v>
+      </c>
+      <c r="L7">
+        <v>1708</v>
+      </c>
+      <c r="M7">
+        <v>2951</v>
+      </c>
+      <c r="N7">
+        <v>1520</v>
+      </c>
+      <c r="O7">
+        <v>2982</v>
+      </c>
+      <c r="P7">
+        <v>1554</v>
+      </c>
+      <c r="Q7">
+        <v>3389</v>
+      </c>
+      <c r="R7">
+        <v>1746</v>
+      </c>
+      <c r="S7">
+        <v>3010</v>
+      </c>
+      <c r="T7">
+        <v>1743</v>
+      </c>
+      <c r="U7">
+        <v>2715</v>
+      </c>
+      <c r="V7">
+        <v>1516</v>
+      </c>
+      <c r="W7">
+        <v>1992</v>
+      </c>
+      <c r="X7">
+        <v>1737</v>
+      </c>
+      <c r="Y7">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>115584</v>
+      </c>
+      <c r="C8">
+        <v>101221</v>
+      </c>
+      <c r="D8">
+        <v>1610</v>
+      </c>
+      <c r="E8">
+        <v>1755</v>
+      </c>
+      <c r="F8">
+        <v>1633</v>
+      </c>
+      <c r="G8">
+        <v>1718</v>
+      </c>
+      <c r="H8">
+        <v>1841</v>
+      </c>
+      <c r="I8">
+        <v>1989</v>
+      </c>
+      <c r="J8">
+        <v>1832</v>
+      </c>
+      <c r="K8">
+        <v>2388</v>
+      </c>
+      <c r="L8">
+        <v>1763</v>
+      </c>
+      <c r="M8">
+        <v>2384</v>
+      </c>
+      <c r="N8">
+        <v>1793</v>
+      </c>
+      <c r="O8">
+        <v>2794</v>
+      </c>
+      <c r="P8">
+        <v>1756</v>
+      </c>
+      <c r="Q8">
+        <v>2784</v>
+      </c>
+      <c r="R8">
+        <v>1995</v>
+      </c>
+      <c r="S8">
+        <v>2833</v>
+      </c>
+      <c r="T8">
+        <v>2161</v>
+      </c>
+      <c r="U8">
+        <v>2813</v>
+      </c>
+      <c r="V8">
+        <v>2032</v>
+      </c>
+      <c r="W8">
+        <v>2235</v>
+      </c>
+      <c r="X8">
+        <v>2525</v>
+      </c>
+      <c r="Y8">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>119764</v>
+      </c>
+      <c r="C9">
+        <v>101879</v>
+      </c>
+      <c r="D9">
+        <v>1931</v>
+      </c>
+      <c r="E9">
+        <v>2702</v>
+      </c>
+      <c r="F9">
+        <v>2017</v>
+      </c>
+      <c r="G9">
+        <v>2591</v>
+      </c>
+      <c r="H9">
+        <v>2276</v>
+      </c>
+      <c r="I9">
+        <v>2991</v>
+      </c>
+      <c r="J9">
+        <v>2434</v>
+      </c>
+      <c r="K9">
+        <v>3181</v>
+      </c>
+      <c r="L9">
+        <v>2064</v>
+      </c>
+      <c r="M9">
+        <v>3179</v>
+      </c>
+      <c r="N9">
+        <v>2200</v>
+      </c>
+      <c r="O9">
+        <v>3508</v>
+      </c>
+      <c r="P9">
+        <v>2238</v>
+      </c>
+      <c r="Q9">
+        <v>3472</v>
+      </c>
+      <c r="R9">
+        <v>2450</v>
+      </c>
+      <c r="S9">
+        <v>3438</v>
+      </c>
+      <c r="T9">
+        <v>2432</v>
+      </c>
+      <c r="U9">
+        <v>3458</v>
+      </c>
+      <c r="V9">
+        <v>2369</v>
+      </c>
+      <c r="W9">
+        <v>2874</v>
+      </c>
+      <c r="X9">
+        <v>2486</v>
+      </c>
+      <c r="Y9">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>179521</v>
+      </c>
+      <c r="C10">
+        <v>143113</v>
+      </c>
+      <c r="D10">
+        <v>2711</v>
+      </c>
+      <c r="E10">
+        <v>3950</v>
+      </c>
+      <c r="F10">
+        <v>2558</v>
+      </c>
+      <c r="G10">
+        <v>3429</v>
+      </c>
+      <c r="H10">
+        <v>2703</v>
+      </c>
+      <c r="I10">
+        <v>4327</v>
+      </c>
+      <c r="J10">
+        <v>2800</v>
+      </c>
+      <c r="K10">
+        <v>5379</v>
+      </c>
+      <c r="L10">
+        <v>2959</v>
+      </c>
+      <c r="M10">
+        <v>5671</v>
+      </c>
+      <c r="N10">
+        <v>2820</v>
+      </c>
+      <c r="O10">
+        <v>6346</v>
+      </c>
+      <c r="P10">
+        <v>2904</v>
+      </c>
+      <c r="Q10">
+        <v>8569</v>
+      </c>
+      <c r="R10">
+        <v>3055</v>
+      </c>
+      <c r="S10">
+        <v>6156</v>
+      </c>
+      <c r="T10">
+        <v>3293</v>
+      </c>
+      <c r="U10">
+        <v>5398</v>
+      </c>
+      <c r="V10">
+        <v>3016</v>
+      </c>
+      <c r="W10">
+        <v>4340</v>
+      </c>
+      <c r="X10">
+        <v>3307</v>
+      </c>
+      <c r="Y10">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>158575</v>
+      </c>
+      <c r="C11">
+        <v>130267</v>
+      </c>
+      <c r="D11">
+        <v>2271</v>
+      </c>
+      <c r="E11">
+        <v>2960</v>
+      </c>
+      <c r="F11">
+        <v>2139</v>
+      </c>
+      <c r="G11">
+        <v>2838</v>
+      </c>
+      <c r="H11">
+        <v>2360</v>
+      </c>
+      <c r="I11">
+        <v>3649</v>
+      </c>
+      <c r="J11">
+        <v>2470</v>
+      </c>
+      <c r="K11">
+        <v>4078</v>
+      </c>
+      <c r="L11">
+        <v>2257</v>
+      </c>
+      <c r="M11">
+        <v>4511</v>
+      </c>
+      <c r="N11">
+        <v>2414</v>
+      </c>
+      <c r="O11">
+        <v>5165</v>
+      </c>
+      <c r="P11">
+        <v>2137</v>
+      </c>
+      <c r="Q11">
+        <v>5838</v>
+      </c>
+      <c r="R11">
+        <v>2549</v>
+      </c>
+      <c r="S11">
+        <v>4787</v>
+      </c>
+      <c r="T11">
+        <v>3049</v>
+      </c>
+      <c r="U11">
+        <v>4626</v>
+      </c>
+      <c r="V11">
+        <v>2747</v>
+      </c>
+      <c r="W11">
+        <v>3618</v>
+      </c>
+      <c r="X11">
+        <v>2976</v>
+      </c>
+      <c r="Y11">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>128899</v>
+      </c>
+      <c r="C12">
+        <v>112195</v>
+      </c>
+      <c r="D12">
+        <v>2082</v>
+      </c>
+      <c r="E12">
+        <v>2668</v>
+      </c>
+      <c r="F12">
+        <v>2127</v>
+      </c>
+      <c r="G12">
+        <v>2631</v>
+      </c>
+      <c r="H12">
+        <v>2362</v>
+      </c>
+      <c r="I12">
+        <v>3040</v>
+      </c>
+      <c r="J12">
+        <v>2176</v>
+      </c>
+      <c r="K12">
+        <v>3006</v>
+      </c>
+      <c r="L12">
+        <v>2416</v>
+      </c>
+      <c r="M12">
+        <v>3080</v>
+      </c>
+      <c r="N12">
+        <v>2333</v>
+      </c>
+      <c r="O12">
+        <v>3328</v>
+      </c>
+      <c r="P12">
+        <v>2140</v>
+      </c>
+      <c r="Q12">
+        <v>3227</v>
+      </c>
+      <c r="R12">
+        <v>2645</v>
+      </c>
+      <c r="S12">
+        <v>2961</v>
+      </c>
+      <c r="T12">
+        <v>2912</v>
+      </c>
+      <c r="U12">
+        <v>3374</v>
+      </c>
+      <c r="V12">
+        <v>2819</v>
+      </c>
+      <c r="W12">
+        <v>2707</v>
+      </c>
+      <c r="X12">
+        <v>2879</v>
+      </c>
+      <c r="Y12">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>305032</v>
+      </c>
+      <c r="C13">
+        <v>258026</v>
+      </c>
+      <c r="D13">
+        <v>4993</v>
+      </c>
+      <c r="E13">
+        <v>5547</v>
+      </c>
+      <c r="F13">
+        <v>4779</v>
+      </c>
+      <c r="G13">
+        <v>5545</v>
+      </c>
+      <c r="H13">
+        <v>4976</v>
+      </c>
+      <c r="I13">
+        <v>6183</v>
+      </c>
+      <c r="J13">
+        <v>5490</v>
+      </c>
+      <c r="K13">
+        <v>7260</v>
+      </c>
+      <c r="L13">
+        <v>5198</v>
+      </c>
+      <c r="M13">
+        <v>7832</v>
+      </c>
+      <c r="N13">
+        <v>5274</v>
+      </c>
+      <c r="O13">
+        <v>9226</v>
+      </c>
+      <c r="P13">
+        <v>5231</v>
+      </c>
+      <c r="Q13">
+        <v>10691</v>
+      </c>
+      <c r="R13">
+        <v>5585</v>
+      </c>
+      <c r="S13">
+        <v>9127</v>
+      </c>
+      <c r="T13">
+        <v>6016</v>
+      </c>
+      <c r="U13">
+        <v>8573</v>
+      </c>
+      <c r="V13">
+        <v>5890</v>
+      </c>
+      <c r="W13">
+        <v>6838</v>
+      </c>
+      <c r="X13">
+        <v>5961</v>
+      </c>
+      <c r="Y13">
+        <v>7183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>172439</v>
+      </c>
+      <c r="C14">
+        <v>139603</v>
+      </c>
+      <c r="D14">
+        <v>2845</v>
+      </c>
+      <c r="E14">
+        <v>4396</v>
+      </c>
+      <c r="F14">
+        <v>2709</v>
+      </c>
+      <c r="G14">
+        <v>4238</v>
+      </c>
+      <c r="H14">
+        <v>2920</v>
+      </c>
+      <c r="I14">
+        <v>4867</v>
+      </c>
+      <c r="J14">
+        <v>2990</v>
+      </c>
+      <c r="K14">
+        <v>4739</v>
+      </c>
+      <c r="L14">
+        <v>2986</v>
+      </c>
+      <c r="M14">
+        <v>5172</v>
+      </c>
+      <c r="N14">
+        <v>3108</v>
+      </c>
+      <c r="O14">
+        <v>5643</v>
+      </c>
+      <c r="P14">
+        <v>3048</v>
+      </c>
+      <c r="Q14">
+        <v>6644</v>
+      </c>
+      <c r="R14">
+        <v>3602</v>
+      </c>
+      <c r="S14">
+        <v>5527</v>
+      </c>
+      <c r="T14">
+        <v>3785</v>
+      </c>
+      <c r="U14">
+        <v>5184</v>
+      </c>
+      <c r="V14">
+        <v>3187</v>
+      </c>
+      <c r="W14">
+        <v>3800</v>
+      </c>
+      <c r="X14">
+        <v>3743</v>
+      </c>
+      <c r="Y14">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>50927</v>
+      </c>
+      <c r="C15">
+        <v>42748</v>
+      </c>
+      <c r="D15">
+        <v>1150</v>
+      </c>
+      <c r="E15">
+        <v>1447</v>
+      </c>
+      <c r="F15">
+        <v>1056</v>
+      </c>
+      <c r="G15">
+        <v>1391</v>
+      </c>
+      <c r="H15">
+        <v>1279</v>
+      </c>
+      <c r="I15">
+        <v>1362</v>
+      </c>
+      <c r="J15">
+        <v>1436</v>
+      </c>
+      <c r="K15">
+        <v>1740</v>
+      </c>
+      <c r="L15">
+        <v>1184</v>
+      </c>
+      <c r="M15">
+        <v>1588</v>
+      </c>
+      <c r="N15">
+        <v>1244</v>
+      </c>
+      <c r="O15">
+        <v>1503</v>
+      </c>
+      <c r="P15">
+        <v>1193</v>
+      </c>
+      <c r="Q15">
+        <v>1750</v>
+      </c>
+      <c r="R15">
+        <v>1313</v>
+      </c>
+      <c r="S15">
+        <v>1444</v>
+      </c>
+      <c r="T15">
+        <v>1429</v>
+      </c>
+      <c r="U15">
+        <v>1418</v>
+      </c>
+      <c r="V15">
+        <v>1082</v>
+      </c>
+      <c r="W15">
+        <v>1142</v>
+      </c>
+      <c r="X15">
+        <v>1315</v>
+      </c>
+      <c r="Y15">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>208055</v>
+      </c>
+      <c r="C16">
+        <v>195237</v>
+      </c>
+      <c r="D16">
+        <v>4559</v>
+      </c>
+      <c r="E16">
+        <v>4648</v>
+      </c>
+      <c r="F16">
+        <v>4708</v>
+      </c>
+      <c r="G16">
+        <v>4494</v>
+      </c>
+      <c r="H16">
+        <v>5124</v>
+      </c>
+      <c r="I16">
+        <v>4474</v>
+      </c>
+      <c r="J16">
+        <v>5721</v>
+      </c>
+      <c r="K16">
+        <v>4938</v>
+      </c>
+      <c r="L16">
+        <v>5432</v>
+      </c>
+      <c r="M16">
+        <v>5042</v>
+      </c>
+      <c r="N16">
+        <v>6163</v>
+      </c>
+      <c r="O16">
+        <v>5308</v>
+      </c>
+      <c r="P16">
+        <v>6639</v>
+      </c>
+      <c r="Q16">
+        <v>5640</v>
+      </c>
+      <c r="R16">
+        <v>7142</v>
+      </c>
+      <c r="S16">
+        <v>5743</v>
+      </c>
+      <c r="T16">
+        <v>8412</v>
+      </c>
+      <c r="U16">
+        <v>6655</v>
+      </c>
+      <c r="V16">
+        <v>7801</v>
+      </c>
+      <c r="W16">
+        <v>6339</v>
+      </c>
+      <c r="X16">
+        <v>7540</v>
+      </c>
+      <c r="Y16">
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>317606</v>
+      </c>
+      <c r="C17">
+        <v>299985</v>
+      </c>
+      <c r="D17">
+        <v>7496</v>
+      </c>
+      <c r="E17">
+        <v>6631</v>
+      </c>
+      <c r="F17">
+        <v>7033</v>
+      </c>
+      <c r="G17">
+        <v>6319</v>
+      </c>
+      <c r="H17">
+        <v>7454</v>
+      </c>
+      <c r="I17">
+        <v>7049</v>
+      </c>
+      <c r="J17">
+        <v>7461</v>
+      </c>
+      <c r="K17">
+        <v>7783</v>
+      </c>
+      <c r="L17">
+        <v>7021</v>
+      </c>
+      <c r="M17">
+        <v>8387</v>
+      </c>
+      <c r="N17">
+        <v>7229</v>
+      </c>
+      <c r="O17">
+        <v>9023</v>
+      </c>
+      <c r="P17">
+        <v>7294</v>
+      </c>
+      <c r="Q17">
+        <v>8934</v>
+      </c>
+      <c r="R17">
+        <v>8184</v>
+      </c>
+      <c r="S17">
+        <v>8603</v>
+      </c>
+      <c r="T17">
+        <v>9763</v>
+      </c>
+      <c r="U17">
+        <v>8723</v>
+      </c>
+      <c r="V17">
+        <v>8985</v>
+      </c>
+      <c r="W17">
+        <v>7646</v>
+      </c>
+      <c r="X17">
+        <v>10759</v>
+      </c>
+      <c r="Y17">
+        <v>9013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>109375</v>
+      </c>
+      <c r="C18">
+        <v>96381</v>
+      </c>
+      <c r="D18">
+        <v>2064</v>
+      </c>
+      <c r="E18">
+        <v>2964</v>
+      </c>
+      <c r="F18">
+        <v>2217</v>
+      </c>
+      <c r="G18">
+        <v>3074</v>
+      </c>
+      <c r="H18">
+        <v>2593</v>
+      </c>
+      <c r="I18">
+        <v>3122</v>
+      </c>
+      <c r="J18">
+        <v>2777</v>
+      </c>
+      <c r="K18">
+        <v>3005</v>
+      </c>
+      <c r="L18">
+        <v>2275</v>
+      </c>
+      <c r="M18">
+        <v>2933</v>
+      </c>
+      <c r="N18">
+        <v>2323</v>
+      </c>
+      <c r="O18">
+        <v>2935</v>
+      </c>
+      <c r="P18">
+        <v>2523</v>
+      </c>
+      <c r="Q18">
+        <v>3300</v>
+      </c>
+      <c r="R18">
+        <v>2549</v>
+      </c>
+      <c r="S18">
+        <v>2935</v>
+      </c>
+      <c r="T18">
+        <v>2802</v>
+      </c>
+      <c r="U18">
+        <v>2884</v>
+      </c>
+      <c r="V18">
+        <v>2561</v>
+      </c>
+      <c r="W18">
+        <v>2805</v>
+      </c>
+      <c r="X18">
+        <v>2823</v>
+      </c>
+      <c r="Y18">
+        <v>2962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>122568</v>
+      </c>
+      <c r="C19">
+        <v>115564</v>
+      </c>
+      <c r="D19">
+        <v>2708</v>
+      </c>
+      <c r="E19">
+        <v>2866</v>
+      </c>
+      <c r="F19">
+        <v>2707</v>
+      </c>
+      <c r="G19">
+        <v>2697</v>
+      </c>
+      <c r="H19">
+        <v>3825</v>
+      </c>
+      <c r="I19">
+        <v>3985</v>
+      </c>
+      <c r="J19">
+        <v>3559</v>
+      </c>
+      <c r="K19">
+        <v>3445</v>
+      </c>
+      <c r="L19">
+        <v>3325</v>
+      </c>
+      <c r="M19">
+        <v>3409</v>
+      </c>
+      <c r="N19">
+        <v>3125</v>
+      </c>
+      <c r="O19">
+        <v>3623</v>
+      </c>
+      <c r="P19">
+        <v>3134</v>
+      </c>
+      <c r="Q19">
+        <v>3309</v>
+      </c>
+      <c r="R19">
+        <v>3382</v>
+      </c>
+      <c r="S19">
+        <v>3153</v>
+      </c>
+      <c r="T19">
+        <v>4337</v>
+      </c>
+      <c r="U19">
+        <v>3221</v>
+      </c>
+      <c r="V19">
+        <v>3728</v>
+      </c>
+      <c r="W19">
+        <v>3365</v>
+      </c>
+      <c r="X19">
+        <v>3370</v>
+      </c>
+      <c r="Y19">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>454798</v>
+      </c>
+      <c r="C20">
+        <v>423407</v>
+      </c>
+      <c r="D20">
+        <v>9636</v>
+      </c>
+      <c r="E20">
+        <v>9604</v>
+      </c>
+      <c r="F20">
+        <v>9499</v>
+      </c>
+      <c r="G20">
+        <v>9668</v>
+      </c>
+      <c r="H20">
+        <v>11748</v>
+      </c>
+      <c r="I20">
+        <v>11292</v>
+      </c>
+      <c r="J20">
+        <v>11229</v>
+      </c>
+      <c r="K20">
+        <v>11712</v>
+      </c>
+      <c r="L20">
+        <v>9974</v>
+      </c>
+      <c r="M20">
+        <v>10320</v>
+      </c>
+      <c r="N20">
+        <v>10066</v>
+      </c>
+      <c r="O20">
+        <v>10894</v>
+      </c>
+      <c r="P20">
+        <v>9176</v>
+      </c>
+      <c r="Q20">
+        <v>10450</v>
+      </c>
+      <c r="R20">
+        <v>9921</v>
+      </c>
+      <c r="S20">
+        <v>10180</v>
+      </c>
+      <c r="T20">
+        <v>11263</v>
+      </c>
+      <c r="U20">
+        <v>9977</v>
+      </c>
+      <c r="V20">
+        <v>9766</v>
+      </c>
+      <c r="W20">
+        <v>10123</v>
+      </c>
+      <c r="X20">
+        <v>11116</v>
+      </c>
+      <c r="Y20">
+        <v>11201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>296195</v>
+      </c>
+      <c r="C21">
+        <v>265419</v>
+      </c>
+      <c r="D21">
+        <v>6662</v>
+      </c>
+      <c r="E21">
+        <v>6413</v>
+      </c>
+      <c r="F21">
+        <v>7059</v>
+      </c>
+      <c r="G21">
+        <v>6691</v>
+      </c>
+      <c r="H21">
+        <v>7567</v>
+      </c>
+      <c r="I21">
+        <v>7322</v>
+      </c>
+      <c r="J21">
+        <v>8258</v>
+      </c>
+      <c r="K21">
+        <v>8220</v>
+      </c>
+      <c r="L21">
+        <v>7867</v>
+      </c>
+      <c r="M21">
+        <v>9020</v>
+      </c>
+      <c r="N21">
+        <v>8127</v>
+      </c>
+      <c r="O21">
+        <v>9049</v>
+      </c>
+      <c r="P21">
+        <v>7631</v>
+      </c>
+      <c r="Q21">
+        <v>8733</v>
+      </c>
+      <c r="R21">
+        <v>8553</v>
+      </c>
+      <c r="S21">
+        <v>8934</v>
+      </c>
+      <c r="T21">
+        <v>9042</v>
+      </c>
+      <c r="U21">
+        <v>8813</v>
+      </c>
+      <c r="V21">
+        <v>8256</v>
+      </c>
+      <c r="W21">
+        <v>8220</v>
+      </c>
+      <c r="X21">
+        <v>8828</v>
+      </c>
+      <c r="Y21">
+        <v>9360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>170017</v>
+      </c>
+      <c r="C22">
+        <v>159766</v>
+      </c>
+      <c r="D22">
+        <v>4043</v>
+      </c>
+      <c r="E22">
+        <v>3301</v>
+      </c>
+      <c r="F22">
+        <v>4175</v>
+      </c>
+      <c r="G22">
+        <v>3448</v>
+      </c>
+      <c r="H22">
+        <v>4344</v>
+      </c>
+      <c r="I22">
+        <v>3983</v>
+      </c>
+      <c r="J22">
+        <v>4435</v>
+      </c>
+      <c r="K22">
+        <v>4804</v>
+      </c>
+      <c r="L22">
+        <v>3962</v>
+      </c>
+      <c r="M22">
+        <v>4580</v>
+      </c>
+      <c r="N22">
+        <v>4047</v>
+      </c>
+      <c r="O22">
+        <v>4215</v>
+      </c>
+      <c r="P22">
+        <v>3845</v>
+      </c>
+      <c r="Q22">
+        <v>4222</v>
+      </c>
+      <c r="R22">
+        <v>4239</v>
+      </c>
+      <c r="S22">
+        <v>4063</v>
+      </c>
+      <c r="T22">
+        <v>5101</v>
+      </c>
+      <c r="U22">
+        <v>4682</v>
+      </c>
+      <c r="V22">
+        <v>4452</v>
+      </c>
+      <c r="W22">
+        <v>3973</v>
+      </c>
+      <c r="X22">
+        <v>5080</v>
+      </c>
+      <c r="Y22">
+        <v>4830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF10406A-7DA4-4C95-BD29-6EE4B84A0747}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>2001</v>
       </c>
@@ -2503,7 +4293,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2520,7 +4310,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2534,7 +4324,7 @@
         <v>3547614</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2548,7 +4338,7 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2562,7 +4352,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2576,7 +4366,7 @@
         <v>24131</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2590,7 +4380,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2604,7 +4394,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2618,7 +4408,7 @@
         <v>7862</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2632,7 +4422,7 @@
         <v>10315</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2646,7 +4436,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2660,7 +4450,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2674,7 +4464,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2688,7 +4478,7 @@
         <v>17980</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2702,7 +4492,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2716,7 +4506,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2730,7 +4520,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -2744,7 +4534,7 @@
         <v>3688</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2758,7 +4548,7 @@
         <v>7729</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2772,7 +4562,7 @@
         <v>123892</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2786,7 +4576,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +4590,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2814,7 +4604,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2828,7 +4618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -2842,7 +4632,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2856,7 +4646,7 @@
         <v>22178</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2870,7 +4660,7 @@
         <v>12712</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2884,7 +4674,7 @@
         <v>22388</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2911,14 +4701,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -2947,7 +4737,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -2984,7 +4774,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -3013,7 +4803,7 @@
         <v>1865129</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -3055,14 +4845,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.2" customHeight="1">
+    <row r="1" spans="1:20" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -3124,7 +4914,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -3187,7 +4977,7 @@
         <v>91851</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -3249,7 +5039,7 @@
         <v>17364</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -3311,7 +5101,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -3374,7 +5164,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -3436,7 +5226,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -3498,7 +5288,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -3560,7 +5350,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -3622,7 +5412,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -3684,7 +5474,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -3746,7 +5536,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -3808,7 +5598,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -3870,7 +5660,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -3932,7 +5722,7 @@
         <v>5137</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -3994,7 +5784,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -4056,7 +5846,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -4118,7 +5908,7 @@
         <v>5419</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -4181,7 +5971,7 @@
         <v>5996</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -4243,7 +6033,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -4305,7 +6095,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -4367,7 +6157,7 @@
         <v>10018</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -4429,7 +6219,7 @@
         <v>7470</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -4508,7 +6298,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -4522,7 +6312,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -4599,7 +6389,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -4676,7 +6466,7 @@
         <v>36508</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -4753,7 +6543,7 @@
         <v>8030</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -4830,7 +6620,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -4907,7 +6697,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -4984,7 +6774,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -5061,7 +6851,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -5138,7 +6928,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -5215,7 +7005,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -5292,7 +7082,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -5369,7 +7159,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -5446,7 +7236,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -5523,7 +7313,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -5600,7 +7390,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -5677,7 +7467,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -5754,7 +7544,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -5831,7 +7621,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -5908,7 +7698,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -5985,7 +7775,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -6062,7 +7852,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -6139,7 +7929,7 @@
         <v>4211</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -6216,7 +8006,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -6320,7 +8110,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -6334,7 +8124,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -6411,7 +8201,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -6488,7 +8278,7 @@
         <v>62712</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -6565,7 +8355,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -6642,7 +8432,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -6719,7 +8509,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -6796,7 +8586,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -6873,7 +8663,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -6950,7 +8740,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -7027,7 +8817,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -7104,7 +8894,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -7181,7 +8971,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -7258,7 +9048,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -7335,7 +9125,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -7412,7 +9202,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -7489,7 +9279,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -7566,7 +9356,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -7643,7 +9433,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -7720,7 +9510,7 @@
         <v>4428</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -7797,7 +9587,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -7874,7 +9664,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -7951,7 +9741,7 @@
         <v>6005</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -8028,7 +9818,7 @@
         <v>4588</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -8132,7 +9922,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -8146,7 +9936,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -8223,7 +10013,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -8300,7 +10090,7 @@
         <v>18203</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -8377,7 +10167,7 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -8454,7 +10244,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -8531,7 +10321,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -8608,7 +10398,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -8685,7 +10475,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -8762,7 +10552,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -8839,7 +10629,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -8916,7 +10706,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -8993,7 +10783,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -9070,7 +10860,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -9147,7 +10937,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -9224,7 +11014,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -9301,7 +11091,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -9378,7 +11168,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -9455,7 +11245,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -9532,7 +11322,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -9609,7 +11399,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -9686,7 +11476,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -9763,7 +11553,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -9840,7 +11630,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -9941,7 +11731,7 @@
       <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -9955,7 +11745,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -10032,7 +11822,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -10109,7 +11899,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -10186,7 +11976,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -10263,7 +12053,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -10340,7 +12130,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -10417,7 +12207,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -10494,7 +12284,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -10571,7 +12361,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -10648,7 +12438,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -10725,7 +12515,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -10802,7 +12592,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -10879,7 +12669,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -10956,7 +12746,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -11033,7 +12823,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -11110,7 +12900,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -11187,7 +12977,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -11264,7 +13054,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -11341,7 +13131,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -11418,7 +13208,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -11495,7 +13285,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -11572,7 +13362,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -11649,7 +13439,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -11750,13 +13540,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4">
+    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
@@ -11765,7 +13555,7 @@
       </c>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="14.4">
+    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -11774,7 +13564,7 @@
         <v>717026</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" customHeight="1">
+    <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>31</v>
       </c>
@@ -11783,7 +13573,7 @@
       </c>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1">
+    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
@@ -11792,7 +13582,7 @@
       </c>
       <c r="C4" s="20"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1">
+    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>23</v>
       </c>
@@ -11801,7 +13591,7 @@
       </c>
       <c r="C5" s="20"/>
     </row>
-    <row r="6" spans="1:3" ht="14.4" customHeight="1">
+    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>56</v>
       </c>
@@ -11810,7 +13600,7 @@
       </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="14.4" customHeight="1">
+    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>57</v>
       </c>
@@ -11819,7 +13609,7 @@
       </c>
       <c r="C7" s="20"/>
     </row>
-    <row r="8" spans="1:3" ht="14.4" customHeight="1">
+    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>58</v>
       </c>
@@ -11828,7 +13618,7 @@
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:3" ht="14.4" customHeight="1">
+    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>59</v>
       </c>
@@ -11837,7 +13627,7 @@
       </c>
       <c r="C9" s="20"/>
     </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1">
+    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>24</v>
       </c>
@@ -11846,7 +13636,7 @@
       </c>
       <c r="C10" s="20"/>
     </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1">
+    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>28</v>
       </c>
@@ -11855,7 +13645,7 @@
       </c>
       <c r="C11" s="20"/>
     </row>
-    <row r="12" spans="1:3" ht="14.4" customHeight="1">
+    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>26</v>
       </c>
@@ -11864,7 +13654,7 @@
       </c>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1">
+    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
@@ -11873,7 +13663,7 @@
       </c>
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1">
+    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
@@ -11882,7 +13672,7 @@
       </c>
       <c r="C14" s="20"/>
     </row>
-    <row r="15" spans="1:3" ht="14.4" customHeight="1">
+    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>62</v>
       </c>
@@ -11891,7 +13681,7 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:3" ht="14.4" customHeight="1">
+    <row r="16" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>63</v>
       </c>
@@ -11900,7 +13690,7 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1">
+    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
@@ -11909,7 +13699,7 @@
       </c>
       <c r="C17" s="20"/>
     </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1">
+    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>64</v>
       </c>
@@ -11918,7 +13708,7 @@
       </c>
       <c r="C18" s="20"/>
     </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1">
+    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>65</v>
       </c>
@@ -11927,7 +13717,7 @@
       </c>
       <c r="C19" s="20"/>
     </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1">
+    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>66</v>
       </c>
@@ -11936,7 +13726,7 @@
       </c>
       <c r="C20" s="20"/>
     </row>
-    <row r="21" spans="1:3" ht="14.4" customHeight="1">
+    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>29</v>
       </c>
@@ -11945,7 +13735,7 @@
       </c>
       <c r="C21" s="20"/>
     </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1">
+    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>25</v>
       </c>
@@ -11954,7 +13744,7 @@
       </c>
       <c r="C22" s="20"/>
     </row>
-    <row r="23" spans="1:3" ht="14.4" customHeight="1">
+    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>27</v>
       </c>
@@ -11963,7 +13753,7 @@
       </c>
       <c r="C23" s="20"/>
     </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1">
+    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>22</v>
       </c>
@@ -11972,7 +13762,7 @@
       </c>
       <c r="C24" s="20"/>
     </row>
-    <row r="25" spans="1:3" ht="14.4">
+    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="C25" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split table migration into movedIn and movedOut
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64CC767-895B-42EC-A5A5-E9BC35D55973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E32EF8-958E-4F72-B83D-B6C57B65C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Brakovi" sheetId="8" r:id="rId7"/>
     <sheet name="Razvodi" sheetId="5" r:id="rId8"/>
     <sheet name="E-gradani" sheetId="9" r:id="rId9"/>
-    <sheet name="Migracije" sheetId="10" r:id="rId10"/>
+    <sheet name="Doseljeni" sheetId="10" r:id="rId10"/>
+    <sheet name="Odseljeni" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -280,72 +281,6 @@
   </si>
   <si>
     <t>Broj_stanovnika_2021</t>
-  </si>
-  <si>
-    <t>Doseljeni_2011</t>
-  </si>
-  <si>
-    <t>Odseljeni_2011</t>
-  </si>
-  <si>
-    <t>Doseljeni_2012</t>
-  </si>
-  <si>
-    <t>Odseljeni_2012</t>
-  </si>
-  <si>
-    <t>Doseljeni_2013</t>
-  </si>
-  <si>
-    <t>Odseljeni_2013</t>
-  </si>
-  <si>
-    <t>Doseljeni_2014</t>
-  </si>
-  <si>
-    <t>Odseljeni_2014</t>
-  </si>
-  <si>
-    <t>Doseljeni_2015</t>
-  </si>
-  <si>
-    <t>Odseljeni_2015</t>
-  </si>
-  <si>
-    <t>Doseljeni_2016</t>
-  </si>
-  <si>
-    <t>Odseljeni_2016</t>
-  </si>
-  <si>
-    <t>Doseljeni_2017</t>
-  </si>
-  <si>
-    <t>Odseljeni_2017</t>
-  </si>
-  <si>
-    <t>Doseljeni_2018</t>
-  </si>
-  <si>
-    <t>Odseljeni_2018</t>
-  </si>
-  <si>
-    <t>Doseljeni_2019</t>
-  </si>
-  <si>
-    <t>Odseljeni_2019</t>
-  </si>
-  <si>
-    <t>Doseljeni_2020</t>
-  </si>
-  <si>
-    <t>Odseljeni_2020</t>
-  </si>
-  <si>
-    <t>Doseljeni_2021</t>
-  </si>
-  <si>
-    <t>Odseljeni_2021</t>
   </si>
 </sst>
 </file>
@@ -2555,20 +2490,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0FD2C1-80AD-4861-A1E7-BB4C1BEC8857}">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="25" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2578,74 +2513,41 @@
       <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" t="s">
-        <v>81</v>
-      </c>
-      <c r="J1" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O1" t="s">
-        <v>87</v>
-      </c>
-      <c r="P1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>89</v>
-      </c>
-      <c r="R1" t="s">
-        <v>90</v>
-      </c>
-      <c r="S1" t="s">
-        <v>91</v>
-      </c>
-      <c r="T1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U1" t="s">
-        <v>93</v>
-      </c>
-      <c r="V1" t="s">
-        <v>94</v>
-      </c>
-      <c r="W1" t="s">
-        <v>95</v>
-      </c>
-      <c r="X1" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+      <c r="K1">
+        <v>2018</v>
+      </c>
+      <c r="L1">
+        <v>2019</v>
+      </c>
+      <c r="M1">
+        <v>2020</v>
+      </c>
+      <c r="N1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2659,70 +2561,37 @@
         <v>14304</v>
       </c>
       <c r="E2">
-        <v>12165</v>
+        <v>13194</v>
       </c>
       <c r="F2">
-        <v>13194</v>
+        <v>14715</v>
       </c>
       <c r="G2">
-        <v>11042</v>
+        <v>16061</v>
       </c>
       <c r="H2">
-        <v>14715</v>
+        <v>16513</v>
       </c>
       <c r="I2">
-        <v>11844</v>
+        <v>16492</v>
       </c>
       <c r="J2">
-        <v>16061</v>
+        <v>16253</v>
       </c>
       <c r="K2">
-        <v>13021</v>
+        <v>18787</v>
       </c>
       <c r="L2">
-        <v>16513</v>
+        <v>20338</v>
       </c>
       <c r="M2">
-        <v>14381</v>
+        <v>16569</v>
       </c>
       <c r="N2">
-        <v>16492</v>
-      </c>
-      <c r="O2">
-        <v>13786</v>
-      </c>
-      <c r="P2">
-        <v>16253</v>
-      </c>
-      <c r="Q2">
-        <v>15250</v>
-      </c>
-      <c r="R2">
-        <v>18787</v>
-      </c>
-      <c r="S2">
-        <v>15545</v>
-      </c>
-      <c r="T2">
-        <v>20338</v>
-      </c>
-      <c r="U2">
-        <v>16641</v>
-      </c>
-      <c r="V2">
-        <v>16569</v>
-      </c>
-      <c r="W2">
-        <v>14946</v>
-      </c>
-      <c r="X2">
         <v>19412</v>
       </c>
-      <c r="Y2">
-        <v>18549</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2736,70 +2605,37 @@
         <v>2046</v>
       </c>
       <c r="E3">
-        <v>2194</v>
+        <v>1608</v>
       </c>
       <c r="F3">
-        <v>1608</v>
+        <v>1851</v>
       </c>
       <c r="G3">
-        <v>1772</v>
+        <v>2172</v>
       </c>
       <c r="H3">
-        <v>1851</v>
+        <v>2094</v>
       </c>
       <c r="I3">
-        <v>2086</v>
+        <v>2130</v>
       </c>
       <c r="J3">
-        <v>2172</v>
+        <v>2163</v>
       </c>
       <c r="K3">
-        <v>2604</v>
+        <v>2506</v>
       </c>
       <c r="L3">
-        <v>2094</v>
+        <v>2902</v>
       </c>
       <c r="M3">
-        <v>2516</v>
+        <v>2754</v>
       </c>
       <c r="N3">
-        <v>2130</v>
-      </c>
-      <c r="O3">
-        <v>2847</v>
-      </c>
-      <c r="P3">
-        <v>2163</v>
-      </c>
-      <c r="Q3">
-        <v>3249</v>
-      </c>
-      <c r="R3">
-        <v>2506</v>
-      </c>
-      <c r="S3">
-        <v>3396</v>
-      </c>
-      <c r="T3">
-        <v>2902</v>
-      </c>
-      <c r="U3">
-        <v>3210</v>
-      </c>
-      <c r="V3">
-        <v>2754</v>
-      </c>
-      <c r="W3">
-        <v>3017</v>
-      </c>
-      <c r="X3">
         <v>3120</v>
       </c>
-      <c r="Y3">
-        <v>3277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2813,70 +2649,37 @@
         <v>1717</v>
       </c>
       <c r="E4">
-        <v>1837</v>
+        <v>1707</v>
       </c>
       <c r="F4">
-        <v>1707</v>
+        <v>2024</v>
       </c>
       <c r="G4">
-        <v>1876</v>
+        <v>2081</v>
       </c>
       <c r="H4">
-        <v>2024</v>
+        <v>2223</v>
       </c>
       <c r="I4">
-        <v>2176</v>
+        <v>2025</v>
       </c>
       <c r="J4">
-        <v>2081</v>
+        <v>2174</v>
       </c>
       <c r="K4">
-        <v>2329</v>
+        <v>2508</v>
       </c>
       <c r="L4">
-        <v>2223</v>
+        <v>3059</v>
       </c>
       <c r="M4">
-        <v>2494</v>
+        <v>2856</v>
       </c>
       <c r="N4">
-        <v>2025</v>
-      </c>
-      <c r="O4">
-        <v>2651</v>
-      </c>
-      <c r="P4">
-        <v>2174</v>
-      </c>
-      <c r="Q4">
-        <v>2608</v>
-      </c>
-      <c r="R4">
-        <v>2508</v>
-      </c>
-      <c r="S4">
-        <v>2775</v>
-      </c>
-      <c r="T4">
-        <v>3059</v>
-      </c>
-      <c r="U4">
-        <v>2748</v>
-      </c>
-      <c r="V4">
-        <v>2856</v>
-      </c>
-      <c r="W4">
-        <v>2541</v>
-      </c>
-      <c r="X4">
         <v>3410</v>
       </c>
-      <c r="Y4">
-        <v>3175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2890,70 +2693,37 @@
         <v>2490</v>
       </c>
       <c r="E5">
-        <v>2424</v>
+        <v>2432</v>
       </c>
       <c r="F5">
-        <v>2432</v>
+        <v>2508</v>
       </c>
       <c r="G5">
-        <v>2556</v>
+        <v>2865</v>
       </c>
       <c r="H5">
-        <v>2508</v>
+        <v>3035</v>
       </c>
       <c r="I5">
-        <v>2753</v>
+        <v>2891</v>
       </c>
       <c r="J5">
-        <v>2865</v>
+        <v>2824</v>
       </c>
       <c r="K5">
-        <v>3429</v>
+        <v>3580</v>
       </c>
       <c r="L5">
-        <v>3035</v>
+        <v>4183</v>
       </c>
       <c r="M5">
-        <v>3579</v>
+        <v>3701</v>
       </c>
       <c r="N5">
-        <v>2891</v>
-      </c>
-      <c r="O5">
-        <v>3725</v>
-      </c>
-      <c r="P5">
-        <v>2824</v>
-      </c>
-      <c r="Q5">
-        <v>4007</v>
-      </c>
-      <c r="R5">
-        <v>3580</v>
-      </c>
-      <c r="S5">
-        <v>3946</v>
-      </c>
-      <c r="T5">
-        <v>4183</v>
-      </c>
-      <c r="U5">
-        <v>4165</v>
-      </c>
-      <c r="V5">
-        <v>3701</v>
-      </c>
-      <c r="W5">
-        <v>3662</v>
-      </c>
-      <c r="X5">
         <v>3954</v>
       </c>
-      <c r="Y5">
-        <v>4112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -2967,70 +2737,37 @@
         <v>1315</v>
       </c>
       <c r="E6">
-        <v>1641</v>
+        <v>1268</v>
       </c>
       <c r="F6">
-        <v>1268</v>
+        <v>1387</v>
       </c>
       <c r="G6">
-        <v>1715</v>
+        <v>1514</v>
       </c>
       <c r="H6">
-        <v>1387</v>
+        <v>1377</v>
       </c>
       <c r="I6">
-        <v>1830</v>
+        <v>1413</v>
       </c>
       <c r="J6">
-        <v>1514</v>
+        <v>1276</v>
       </c>
       <c r="K6">
-        <v>2220</v>
+        <v>1441</v>
       </c>
       <c r="L6">
-        <v>1377</v>
+        <v>1494</v>
       </c>
       <c r="M6">
-        <v>2549</v>
+        <v>1482</v>
       </c>
       <c r="N6">
-        <v>1413</v>
-      </c>
-      <c r="O6">
-        <v>2637</v>
-      </c>
-      <c r="P6">
-        <v>1276</v>
-      </c>
-      <c r="Q6">
-        <v>2866</v>
-      </c>
-      <c r="R6">
-        <v>1441</v>
-      </c>
-      <c r="S6">
-        <v>2662</v>
-      </c>
-      <c r="T6">
-        <v>1494</v>
-      </c>
-      <c r="U6">
-        <v>2660</v>
-      </c>
-      <c r="V6">
-        <v>1482</v>
-      </c>
-      <c r="W6">
-        <v>2018</v>
-      </c>
-      <c r="X6">
         <v>1435</v>
       </c>
-      <c r="Y6">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -3044,70 +2781,37 @@
         <v>1304</v>
       </c>
       <c r="E7">
-        <v>1989</v>
+        <v>1173</v>
       </c>
       <c r="F7">
-        <v>1173</v>
+        <v>1361</v>
       </c>
       <c r="G7">
-        <v>1983</v>
+        <v>1613</v>
       </c>
       <c r="H7">
-        <v>1361</v>
+        <v>1708</v>
       </c>
       <c r="I7">
-        <v>1778</v>
+        <v>1520</v>
       </c>
       <c r="J7">
-        <v>1613</v>
+        <v>1554</v>
       </c>
       <c r="K7">
-        <v>2313</v>
+        <v>1746</v>
       </c>
       <c r="L7">
-        <v>1708</v>
+        <v>1743</v>
       </c>
       <c r="M7">
-        <v>2951</v>
+        <v>1516</v>
       </c>
       <c r="N7">
-        <v>1520</v>
-      </c>
-      <c r="O7">
-        <v>2982</v>
-      </c>
-      <c r="P7">
-        <v>1554</v>
-      </c>
-      <c r="Q7">
-        <v>3389</v>
-      </c>
-      <c r="R7">
-        <v>1746</v>
-      </c>
-      <c r="S7">
-        <v>3010</v>
-      </c>
-      <c r="T7">
-        <v>1743</v>
-      </c>
-      <c r="U7">
-        <v>2715</v>
-      </c>
-      <c r="V7">
-        <v>1516</v>
-      </c>
-      <c r="W7">
-        <v>1992</v>
-      </c>
-      <c r="X7">
         <v>1737</v>
       </c>
-      <c r="Y7">
-        <v>2319</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3121,70 +2825,37 @@
         <v>1610</v>
       </c>
       <c r="E8">
-        <v>1755</v>
+        <v>1633</v>
       </c>
       <c r="F8">
-        <v>1633</v>
+        <v>1841</v>
       </c>
       <c r="G8">
-        <v>1718</v>
+        <v>1832</v>
       </c>
       <c r="H8">
-        <v>1841</v>
+        <v>1763</v>
       </c>
       <c r="I8">
-        <v>1989</v>
+        <v>1793</v>
       </c>
       <c r="J8">
-        <v>1832</v>
+        <v>1756</v>
       </c>
       <c r="K8">
-        <v>2388</v>
+        <v>1995</v>
       </c>
       <c r="L8">
-        <v>1763</v>
+        <v>2161</v>
       </c>
       <c r="M8">
-        <v>2384</v>
+        <v>2032</v>
       </c>
       <c r="N8">
-        <v>1793</v>
-      </c>
-      <c r="O8">
-        <v>2794</v>
-      </c>
-      <c r="P8">
-        <v>1756</v>
-      </c>
-      <c r="Q8">
-        <v>2784</v>
-      </c>
-      <c r="R8">
-        <v>1995</v>
-      </c>
-      <c r="S8">
-        <v>2833</v>
-      </c>
-      <c r="T8">
-        <v>2161</v>
-      </c>
-      <c r="U8">
-        <v>2813</v>
-      </c>
-      <c r="V8">
-        <v>2032</v>
-      </c>
-      <c r="W8">
-        <v>2235</v>
-      </c>
-      <c r="X8">
         <v>2525</v>
       </c>
-      <c r="Y8">
-        <v>2491</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3198,70 +2869,37 @@
         <v>1931</v>
       </c>
       <c r="E9">
-        <v>2702</v>
+        <v>2017</v>
       </c>
       <c r="F9">
-        <v>2017</v>
+        <v>2276</v>
       </c>
       <c r="G9">
-        <v>2591</v>
+        <v>2434</v>
       </c>
       <c r="H9">
-        <v>2276</v>
+        <v>2064</v>
       </c>
       <c r="I9">
-        <v>2991</v>
+        <v>2200</v>
       </c>
       <c r="J9">
-        <v>2434</v>
+        <v>2238</v>
       </c>
       <c r="K9">
-        <v>3181</v>
+        <v>2450</v>
       </c>
       <c r="L9">
-        <v>2064</v>
+        <v>2432</v>
       </c>
       <c r="M9">
-        <v>3179</v>
+        <v>2369</v>
       </c>
       <c r="N9">
-        <v>2200</v>
-      </c>
-      <c r="O9">
-        <v>3508</v>
-      </c>
-      <c r="P9">
-        <v>2238</v>
-      </c>
-      <c r="Q9">
-        <v>3472</v>
-      </c>
-      <c r="R9">
-        <v>2450</v>
-      </c>
-      <c r="S9">
-        <v>3438</v>
-      </c>
-      <c r="T9">
-        <v>2432</v>
-      </c>
-      <c r="U9">
-        <v>3458</v>
-      </c>
-      <c r="V9">
-        <v>2369</v>
-      </c>
-      <c r="W9">
-        <v>2874</v>
-      </c>
-      <c r="X9">
         <v>2486</v>
       </c>
-      <c r="Y9">
-        <v>3225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3275,70 +2913,37 @@
         <v>2711</v>
       </c>
       <c r="E10">
-        <v>3950</v>
+        <v>2558</v>
       </c>
       <c r="F10">
-        <v>2558</v>
+        <v>2703</v>
       </c>
       <c r="G10">
-        <v>3429</v>
+        <v>2800</v>
       </c>
       <c r="H10">
-        <v>2703</v>
+        <v>2959</v>
       </c>
       <c r="I10">
-        <v>4327</v>
+        <v>2820</v>
       </c>
       <c r="J10">
-        <v>2800</v>
+        <v>2904</v>
       </c>
       <c r="K10">
-        <v>5379</v>
+        <v>3055</v>
       </c>
       <c r="L10">
-        <v>2959</v>
+        <v>3293</v>
       </c>
       <c r="M10">
-        <v>5671</v>
+        <v>3016</v>
       </c>
       <c r="N10">
-        <v>2820</v>
-      </c>
-      <c r="O10">
-        <v>6346</v>
-      </c>
-      <c r="P10">
-        <v>2904</v>
-      </c>
-      <c r="Q10">
-        <v>8569</v>
-      </c>
-      <c r="R10">
-        <v>3055</v>
-      </c>
-      <c r="S10">
-        <v>6156</v>
-      </c>
-      <c r="T10">
-        <v>3293</v>
-      </c>
-      <c r="U10">
-        <v>5398</v>
-      </c>
-      <c r="V10">
-        <v>3016</v>
-      </c>
-      <c r="W10">
-        <v>4340</v>
-      </c>
-      <c r="X10">
         <v>3307</v>
       </c>
-      <c r="Y10">
-        <v>4568</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3352,70 +2957,37 @@
         <v>2271</v>
       </c>
       <c r="E11">
-        <v>2960</v>
+        <v>2139</v>
       </c>
       <c r="F11">
-        <v>2139</v>
+        <v>2360</v>
       </c>
       <c r="G11">
-        <v>2838</v>
+        <v>2470</v>
       </c>
       <c r="H11">
-        <v>2360</v>
+        <v>2257</v>
       </c>
       <c r="I11">
-        <v>3649</v>
+        <v>2414</v>
       </c>
       <c r="J11">
-        <v>2470</v>
+        <v>2137</v>
       </c>
       <c r="K11">
-        <v>4078</v>
+        <v>2549</v>
       </c>
       <c r="L11">
-        <v>2257</v>
+        <v>3049</v>
       </c>
       <c r="M11">
-        <v>4511</v>
+        <v>2747</v>
       </c>
       <c r="N11">
-        <v>2414</v>
-      </c>
-      <c r="O11">
-        <v>5165</v>
-      </c>
-      <c r="P11">
-        <v>2137</v>
-      </c>
-      <c r="Q11">
-        <v>5838</v>
-      </c>
-      <c r="R11">
-        <v>2549</v>
-      </c>
-      <c r="S11">
-        <v>4787</v>
-      </c>
-      <c r="T11">
-        <v>3049</v>
-      </c>
-      <c r="U11">
-        <v>4626</v>
-      </c>
-      <c r="V11">
-        <v>2747</v>
-      </c>
-      <c r="W11">
-        <v>3618</v>
-      </c>
-      <c r="X11">
         <v>2976</v>
       </c>
-      <c r="Y11">
-        <v>4244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3429,70 +3001,37 @@
         <v>2082</v>
       </c>
       <c r="E12">
-        <v>2668</v>
+        <v>2127</v>
       </c>
       <c r="F12">
-        <v>2127</v>
+        <v>2362</v>
       </c>
       <c r="G12">
-        <v>2631</v>
+        <v>2176</v>
       </c>
       <c r="H12">
-        <v>2362</v>
+        <v>2416</v>
       </c>
       <c r="I12">
-        <v>3040</v>
+        <v>2333</v>
       </c>
       <c r="J12">
-        <v>2176</v>
+        <v>2140</v>
       </c>
       <c r="K12">
-        <v>3006</v>
+        <v>2645</v>
       </c>
       <c r="L12">
-        <v>2416</v>
+        <v>2912</v>
       </c>
       <c r="M12">
-        <v>3080</v>
+        <v>2819</v>
       </c>
       <c r="N12">
-        <v>2333</v>
-      </c>
-      <c r="O12">
-        <v>3328</v>
-      </c>
-      <c r="P12">
-        <v>2140</v>
-      </c>
-      <c r="Q12">
-        <v>3227</v>
-      </c>
-      <c r="R12">
-        <v>2645</v>
-      </c>
-      <c r="S12">
-        <v>2961</v>
-      </c>
-      <c r="T12">
-        <v>2912</v>
-      </c>
-      <c r="U12">
-        <v>3374</v>
-      </c>
-      <c r="V12">
-        <v>2819</v>
-      </c>
-      <c r="W12">
-        <v>2707</v>
-      </c>
-      <c r="X12">
         <v>2879</v>
       </c>
-      <c r="Y12">
-        <v>3030</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -3506,70 +3045,37 @@
         <v>4993</v>
       </c>
       <c r="E13">
-        <v>5547</v>
+        <v>4779</v>
       </c>
       <c r="F13">
-        <v>4779</v>
+        <v>4976</v>
       </c>
       <c r="G13">
-        <v>5545</v>
+        <v>5490</v>
       </c>
       <c r="H13">
-        <v>4976</v>
+        <v>5198</v>
       </c>
       <c r="I13">
-        <v>6183</v>
+        <v>5274</v>
       </c>
       <c r="J13">
-        <v>5490</v>
+        <v>5231</v>
       </c>
       <c r="K13">
-        <v>7260</v>
+        <v>5585</v>
       </c>
       <c r="L13">
-        <v>5198</v>
+        <v>6016</v>
       </c>
       <c r="M13">
-        <v>7832</v>
+        <v>5890</v>
       </c>
       <c r="N13">
-        <v>5274</v>
-      </c>
-      <c r="O13">
-        <v>9226</v>
-      </c>
-      <c r="P13">
-        <v>5231</v>
-      </c>
-      <c r="Q13">
-        <v>10691</v>
-      </c>
-      <c r="R13">
-        <v>5585</v>
-      </c>
-      <c r="S13">
-        <v>9127</v>
-      </c>
-      <c r="T13">
-        <v>6016</v>
-      </c>
-      <c r="U13">
-        <v>8573</v>
-      </c>
-      <c r="V13">
-        <v>5890</v>
-      </c>
-      <c r="W13">
-        <v>6838</v>
-      </c>
-      <c r="X13">
         <v>5961</v>
       </c>
-      <c r="Y13">
-        <v>7183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3583,70 +3089,37 @@
         <v>2845</v>
       </c>
       <c r="E14">
-        <v>4396</v>
+        <v>2709</v>
       </c>
       <c r="F14">
-        <v>2709</v>
+        <v>2920</v>
       </c>
       <c r="G14">
-        <v>4238</v>
+        <v>2990</v>
       </c>
       <c r="H14">
-        <v>2920</v>
+        <v>2986</v>
       </c>
       <c r="I14">
-        <v>4867</v>
+        <v>3108</v>
       </c>
       <c r="J14">
-        <v>2990</v>
+        <v>3048</v>
       </c>
       <c r="K14">
-        <v>4739</v>
+        <v>3602</v>
       </c>
       <c r="L14">
-        <v>2986</v>
+        <v>3785</v>
       </c>
       <c r="M14">
-        <v>5172</v>
+        <v>3187</v>
       </c>
       <c r="N14">
-        <v>3108</v>
-      </c>
-      <c r="O14">
-        <v>5643</v>
-      </c>
-      <c r="P14">
-        <v>3048</v>
-      </c>
-      <c r="Q14">
-        <v>6644</v>
-      </c>
-      <c r="R14">
-        <v>3602</v>
-      </c>
-      <c r="S14">
-        <v>5527</v>
-      </c>
-      <c r="T14">
-        <v>3785</v>
-      </c>
-      <c r="U14">
-        <v>5184</v>
-      </c>
-      <c r="V14">
-        <v>3187</v>
-      </c>
-      <c r="W14">
-        <v>3800</v>
-      </c>
-      <c r="X14">
         <v>3743</v>
       </c>
-      <c r="Y14">
-        <v>4670</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -3660,70 +3133,37 @@
         <v>1150</v>
       </c>
       <c r="E15">
-        <v>1447</v>
+        <v>1056</v>
       </c>
       <c r="F15">
-        <v>1056</v>
+        <v>1279</v>
       </c>
       <c r="G15">
-        <v>1391</v>
+        <v>1436</v>
       </c>
       <c r="H15">
-        <v>1279</v>
+        <v>1184</v>
       </c>
       <c r="I15">
-        <v>1362</v>
+        <v>1244</v>
       </c>
       <c r="J15">
-        <v>1436</v>
+        <v>1193</v>
       </c>
       <c r="K15">
-        <v>1740</v>
+        <v>1313</v>
       </c>
       <c r="L15">
-        <v>1184</v>
+        <v>1429</v>
       </c>
       <c r="M15">
-        <v>1588</v>
+        <v>1082</v>
       </c>
       <c r="N15">
-        <v>1244</v>
-      </c>
-      <c r="O15">
-        <v>1503</v>
-      </c>
-      <c r="P15">
-        <v>1193</v>
-      </c>
-      <c r="Q15">
-        <v>1750</v>
-      </c>
-      <c r="R15">
-        <v>1313</v>
-      </c>
-      <c r="S15">
-        <v>1444</v>
-      </c>
-      <c r="T15">
-        <v>1429</v>
-      </c>
-      <c r="U15">
-        <v>1418</v>
-      </c>
-      <c r="V15">
-        <v>1082</v>
-      </c>
-      <c r="W15">
-        <v>1142</v>
-      </c>
-      <c r="X15">
         <v>1315</v>
       </c>
-      <c r="Y15">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3737,70 +3177,37 @@
         <v>4559</v>
       </c>
       <c r="E16">
-        <v>4648</v>
+        <v>4708</v>
       </c>
       <c r="F16">
-        <v>4708</v>
+        <v>5124</v>
       </c>
       <c r="G16">
-        <v>4494</v>
+        <v>5721</v>
       </c>
       <c r="H16">
-        <v>5124</v>
+        <v>5432</v>
       </c>
       <c r="I16">
-        <v>4474</v>
+        <v>6163</v>
       </c>
       <c r="J16">
-        <v>5721</v>
+        <v>6639</v>
       </c>
       <c r="K16">
-        <v>4938</v>
+        <v>7142</v>
       </c>
       <c r="L16">
-        <v>5432</v>
+        <v>8412</v>
       </c>
       <c r="M16">
-        <v>5042</v>
+        <v>7801</v>
       </c>
       <c r="N16">
-        <v>6163</v>
-      </c>
-      <c r="O16">
-        <v>5308</v>
-      </c>
-      <c r="P16">
-        <v>6639</v>
-      </c>
-      <c r="Q16">
-        <v>5640</v>
-      </c>
-      <c r="R16">
-        <v>7142</v>
-      </c>
-      <c r="S16">
-        <v>5743</v>
-      </c>
-      <c r="T16">
-        <v>8412</v>
-      </c>
-      <c r="U16">
-        <v>6655</v>
-      </c>
-      <c r="V16">
-        <v>7801</v>
-      </c>
-      <c r="W16">
-        <v>6339</v>
-      </c>
-      <c r="X16">
         <v>7540</v>
       </c>
-      <c r="Y16">
-        <v>6729</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -3814,70 +3221,37 @@
         <v>7496</v>
       </c>
       <c r="E17">
-        <v>6631</v>
+        <v>7033</v>
       </c>
       <c r="F17">
-        <v>7033</v>
+        <v>7454</v>
       </c>
       <c r="G17">
-        <v>6319</v>
+        <v>7461</v>
       </c>
       <c r="H17">
-        <v>7454</v>
+        <v>7021</v>
       </c>
       <c r="I17">
-        <v>7049</v>
+        <v>7229</v>
       </c>
       <c r="J17">
-        <v>7461</v>
+        <v>7294</v>
       </c>
       <c r="K17">
-        <v>7783</v>
+        <v>8184</v>
       </c>
       <c r="L17">
-        <v>7021</v>
+        <v>9763</v>
       </c>
       <c r="M17">
-        <v>8387</v>
+        <v>8985</v>
       </c>
       <c r="N17">
-        <v>7229</v>
-      </c>
-      <c r="O17">
-        <v>9023</v>
-      </c>
-      <c r="P17">
-        <v>7294</v>
-      </c>
-      <c r="Q17">
-        <v>8934</v>
-      </c>
-      <c r="R17">
-        <v>8184</v>
-      </c>
-      <c r="S17">
-        <v>8603</v>
-      </c>
-      <c r="T17">
-        <v>9763</v>
-      </c>
-      <c r="U17">
-        <v>8723</v>
-      </c>
-      <c r="V17">
-        <v>8985</v>
-      </c>
-      <c r="W17">
-        <v>7646</v>
-      </c>
-      <c r="X17">
         <v>10759</v>
       </c>
-      <c r="Y17">
-        <v>9013</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -3891,70 +3265,37 @@
         <v>2064</v>
       </c>
       <c r="E18">
-        <v>2964</v>
+        <v>2217</v>
       </c>
       <c r="F18">
-        <v>2217</v>
+        <v>2593</v>
       </c>
       <c r="G18">
-        <v>3074</v>
+        <v>2777</v>
       </c>
       <c r="H18">
-        <v>2593</v>
+        <v>2275</v>
       </c>
       <c r="I18">
-        <v>3122</v>
+        <v>2323</v>
       </c>
       <c r="J18">
-        <v>2777</v>
+        <v>2523</v>
       </c>
       <c r="K18">
-        <v>3005</v>
+        <v>2549</v>
       </c>
       <c r="L18">
-        <v>2275</v>
+        <v>2802</v>
       </c>
       <c r="M18">
-        <v>2933</v>
+        <v>2561</v>
       </c>
       <c r="N18">
-        <v>2323</v>
-      </c>
-      <c r="O18">
-        <v>2935</v>
-      </c>
-      <c r="P18">
-        <v>2523</v>
-      </c>
-      <c r="Q18">
-        <v>3300</v>
-      </c>
-      <c r="R18">
-        <v>2549</v>
-      </c>
-      <c r="S18">
-        <v>2935</v>
-      </c>
-      <c r="T18">
-        <v>2802</v>
-      </c>
-      <c r="U18">
-        <v>2884</v>
-      </c>
-      <c r="V18">
-        <v>2561</v>
-      </c>
-      <c r="W18">
-        <v>2805</v>
-      </c>
-      <c r="X18">
         <v>2823</v>
       </c>
-      <c r="Y18">
-        <v>2962</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -3968,70 +3309,37 @@
         <v>2708</v>
       </c>
       <c r="E19">
-        <v>2866</v>
+        <v>2707</v>
       </c>
       <c r="F19">
-        <v>2707</v>
+        <v>3825</v>
       </c>
       <c r="G19">
-        <v>2697</v>
+        <v>3559</v>
       </c>
       <c r="H19">
-        <v>3825</v>
+        <v>3325</v>
       </c>
       <c r="I19">
-        <v>3985</v>
+        <v>3125</v>
       </c>
       <c r="J19">
-        <v>3559</v>
+        <v>3134</v>
       </c>
       <c r="K19">
-        <v>3445</v>
+        <v>3382</v>
       </c>
       <c r="L19">
-        <v>3325</v>
+        <v>4337</v>
       </c>
       <c r="M19">
-        <v>3409</v>
+        <v>3728</v>
       </c>
       <c r="N19">
-        <v>3125</v>
-      </c>
-      <c r="O19">
-        <v>3623</v>
-      </c>
-      <c r="P19">
-        <v>3134</v>
-      </c>
-      <c r="Q19">
-        <v>3309</v>
-      </c>
-      <c r="R19">
-        <v>3382</v>
-      </c>
-      <c r="S19">
-        <v>3153</v>
-      </c>
-      <c r="T19">
-        <v>4337</v>
-      </c>
-      <c r="U19">
-        <v>3221</v>
-      </c>
-      <c r="V19">
-        <v>3728</v>
-      </c>
-      <c r="W19">
-        <v>3365</v>
-      </c>
-      <c r="X19">
         <v>3370</v>
       </c>
-      <c r="Y19">
-        <v>4006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -4045,70 +3353,37 @@
         <v>9636</v>
       </c>
       <c r="E20">
-        <v>9604</v>
+        <v>9499</v>
       </c>
       <c r="F20">
-        <v>9499</v>
+        <v>11748</v>
       </c>
       <c r="G20">
-        <v>9668</v>
+        <v>11229</v>
       </c>
       <c r="H20">
-        <v>11748</v>
+        <v>9974</v>
       </c>
       <c r="I20">
-        <v>11292</v>
+        <v>10066</v>
       </c>
       <c r="J20">
-        <v>11229</v>
+        <v>9176</v>
       </c>
       <c r="K20">
-        <v>11712</v>
+        <v>9921</v>
       </c>
       <c r="L20">
-        <v>9974</v>
+        <v>11263</v>
       </c>
       <c r="M20">
-        <v>10320</v>
+        <v>9766</v>
       </c>
       <c r="N20">
-        <v>10066</v>
-      </c>
-      <c r="O20">
-        <v>10894</v>
-      </c>
-      <c r="P20">
-        <v>9176</v>
-      </c>
-      <c r="Q20">
-        <v>10450</v>
-      </c>
-      <c r="R20">
-        <v>9921</v>
-      </c>
-      <c r="S20">
-        <v>10180</v>
-      </c>
-      <c r="T20">
-        <v>11263</v>
-      </c>
-      <c r="U20">
-        <v>9977</v>
-      </c>
-      <c r="V20">
-        <v>9766</v>
-      </c>
-      <c r="W20">
-        <v>10123</v>
-      </c>
-      <c r="X20">
         <v>11116</v>
       </c>
-      <c r="Y20">
-        <v>11201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4122,70 +3397,37 @@
         <v>6662</v>
       </c>
       <c r="E21">
-        <v>6413</v>
+        <v>7059</v>
       </c>
       <c r="F21">
-        <v>7059</v>
+        <v>7567</v>
       </c>
       <c r="G21">
-        <v>6691</v>
+        <v>8258</v>
       </c>
       <c r="H21">
-        <v>7567</v>
+        <v>7867</v>
       </c>
       <c r="I21">
-        <v>7322</v>
+        <v>8127</v>
       </c>
       <c r="J21">
-        <v>8258</v>
+        <v>7631</v>
       </c>
       <c r="K21">
-        <v>8220</v>
+        <v>8553</v>
       </c>
       <c r="L21">
-        <v>7867</v>
+        <v>9042</v>
       </c>
       <c r="M21">
-        <v>9020</v>
+        <v>8256</v>
       </c>
       <c r="N21">
-        <v>8127</v>
-      </c>
-      <c r="O21">
-        <v>9049</v>
-      </c>
-      <c r="P21">
-        <v>7631</v>
-      </c>
-      <c r="Q21">
-        <v>8733</v>
-      </c>
-      <c r="R21">
-        <v>8553</v>
-      </c>
-      <c r="S21">
-        <v>8934</v>
-      </c>
-      <c r="T21">
-        <v>9042</v>
-      </c>
-      <c r="U21">
-        <v>8813</v>
-      </c>
-      <c r="V21">
-        <v>8256</v>
-      </c>
-      <c r="W21">
-        <v>8220</v>
-      </c>
-      <c r="X21">
         <v>8828</v>
       </c>
-      <c r="Y21">
-        <v>9360</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4199,66 +3441,1021 @@
         <v>4043</v>
       </c>
       <c r="E22">
+        <v>4175</v>
+      </c>
+      <c r="F22">
+        <v>4344</v>
+      </c>
+      <c r="G22">
+        <v>4435</v>
+      </c>
+      <c r="H22">
+        <v>3962</v>
+      </c>
+      <c r="I22">
+        <v>4047</v>
+      </c>
+      <c r="J22">
+        <v>3845</v>
+      </c>
+      <c r="K22">
+        <v>4239</v>
+      </c>
+      <c r="L22">
+        <v>5101</v>
+      </c>
+      <c r="M22">
+        <v>4452</v>
+      </c>
+      <c r="N22">
+        <v>5080</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F98E4D1-812A-43FC-A5E2-E0E4232BE4B7}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1">
+        <v>2011</v>
+      </c>
+      <c r="E1">
+        <v>2012</v>
+      </c>
+      <c r="F1">
+        <v>2013</v>
+      </c>
+      <c r="G1">
+        <v>2014</v>
+      </c>
+      <c r="H1">
+        <v>2015</v>
+      </c>
+      <c r="I1">
+        <v>2016</v>
+      </c>
+      <c r="J1">
+        <v>2017</v>
+      </c>
+      <c r="K1">
+        <v>2018</v>
+      </c>
+      <c r="L1">
+        <v>2019</v>
+      </c>
+      <c r="M1">
+        <v>2020</v>
+      </c>
+      <c r="N1">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>790017</v>
+      </c>
+      <c r="C2">
+        <v>767131</v>
+      </c>
+      <c r="D2">
+        <v>12165</v>
+      </c>
+      <c r="E2">
+        <v>11042</v>
+      </c>
+      <c r="F2">
+        <v>11844</v>
+      </c>
+      <c r="G2">
+        <v>13021</v>
+      </c>
+      <c r="H2">
+        <v>14381</v>
+      </c>
+      <c r="I2">
+        <v>13786</v>
+      </c>
+      <c r="J2">
+        <v>15250</v>
+      </c>
+      <c r="K2">
+        <v>15545</v>
+      </c>
+      <c r="L2">
+        <v>16641</v>
+      </c>
+      <c r="M2">
+        <v>14946</v>
+      </c>
+      <c r="N2">
+        <v>18549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3">
+        <v>113804</v>
+      </c>
+      <c r="C3">
+        <v>105250</v>
+      </c>
+      <c r="D3">
+        <v>2194</v>
+      </c>
+      <c r="E3">
+        <v>1772</v>
+      </c>
+      <c r="F3">
+        <v>2086</v>
+      </c>
+      <c r="G3">
+        <v>2604</v>
+      </c>
+      <c r="H3">
+        <v>2516</v>
+      </c>
+      <c r="I3">
+        <v>2847</v>
+      </c>
+      <c r="J3">
+        <v>3249</v>
+      </c>
+      <c r="K3">
+        <v>3396</v>
+      </c>
+      <c r="L3">
+        <v>3210</v>
+      </c>
+      <c r="M3">
+        <v>3017</v>
+      </c>
+      <c r="N3">
+        <v>3277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>132892</v>
+      </c>
+      <c r="C4">
+        <v>120702</v>
+      </c>
+      <c r="D4">
+        <v>1837</v>
+      </c>
+      <c r="E4">
+        <v>1876</v>
+      </c>
+      <c r="F4">
+        <v>2176</v>
+      </c>
+      <c r="G4">
+        <v>2329</v>
+      </c>
+      <c r="H4">
+        <v>2494</v>
+      </c>
+      <c r="I4">
+        <v>2651</v>
+      </c>
+      <c r="J4">
+        <v>2608</v>
+      </c>
+      <c r="K4">
+        <v>2775</v>
+      </c>
+      <c r="L4">
+        <v>2748</v>
+      </c>
+      <c r="M4">
+        <v>2541</v>
+      </c>
+      <c r="N4">
+        <v>3175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>175951</v>
+      </c>
+      <c r="C5">
+        <v>159487</v>
+      </c>
+      <c r="D5">
+        <v>2424</v>
+      </c>
+      <c r="E5">
+        <v>2556</v>
+      </c>
+      <c r="F5">
+        <v>2753</v>
+      </c>
+      <c r="G5">
+        <v>3429</v>
+      </c>
+      <c r="H5">
+        <v>3579</v>
+      </c>
+      <c r="I5">
+        <v>3725</v>
+      </c>
+      <c r="J5">
+        <v>4007</v>
+      </c>
+      <c r="K5">
+        <v>3946</v>
+      </c>
+      <c r="L5">
+        <v>4165</v>
+      </c>
+      <c r="M5">
+        <v>3662</v>
+      </c>
+      <c r="N5">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>84836</v>
+      </c>
+      <c r="C6">
+        <v>70368</v>
+      </c>
+      <c r="D6">
+        <v>1641</v>
+      </c>
+      <c r="E6">
+        <v>1715</v>
+      </c>
+      <c r="F6">
+        <v>1830</v>
+      </c>
+      <c r="G6">
+        <v>2220</v>
+      </c>
+      <c r="H6">
+        <v>2549</v>
+      </c>
+      <c r="I6">
+        <v>2637</v>
+      </c>
+      <c r="J6">
+        <v>2866</v>
+      </c>
+      <c r="K6">
+        <v>2662</v>
+      </c>
+      <c r="L6">
+        <v>2660</v>
+      </c>
+      <c r="M6">
+        <v>2018</v>
+      </c>
+      <c r="N6">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>78034</v>
+      </c>
+      <c r="C7">
+        <v>64084</v>
+      </c>
+      <c r="D7">
+        <v>1989</v>
+      </c>
+      <c r="E7">
+        <v>1983</v>
+      </c>
+      <c r="F7">
+        <v>1778</v>
+      </c>
+      <c r="G7">
+        <v>2313</v>
+      </c>
+      <c r="H7">
+        <v>2951</v>
+      </c>
+      <c r="I7">
+        <v>2982</v>
+      </c>
+      <c r="J7">
+        <v>3389</v>
+      </c>
+      <c r="K7">
+        <v>3010</v>
+      </c>
+      <c r="L7">
+        <v>2715</v>
+      </c>
+      <c r="M7">
+        <v>1992</v>
+      </c>
+      <c r="N7">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>115584</v>
+      </c>
+      <c r="C8">
+        <v>101221</v>
+      </c>
+      <c r="D8">
+        <v>1755</v>
+      </c>
+      <c r="E8">
+        <v>1718</v>
+      </c>
+      <c r="F8">
+        <v>1989</v>
+      </c>
+      <c r="G8">
+        <v>2388</v>
+      </c>
+      <c r="H8">
+        <v>2384</v>
+      </c>
+      <c r="I8">
+        <v>2794</v>
+      </c>
+      <c r="J8">
+        <v>2784</v>
+      </c>
+      <c r="K8">
+        <v>2833</v>
+      </c>
+      <c r="L8">
+        <v>2813</v>
+      </c>
+      <c r="M8">
+        <v>2235</v>
+      </c>
+      <c r="N8">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>119764</v>
+      </c>
+      <c r="C9">
+        <v>101879</v>
+      </c>
+      <c r="D9">
+        <v>2702</v>
+      </c>
+      <c r="E9">
+        <v>2591</v>
+      </c>
+      <c r="F9">
+        <v>2991</v>
+      </c>
+      <c r="G9">
+        <v>3181</v>
+      </c>
+      <c r="H9">
+        <v>3179</v>
+      </c>
+      <c r="I9">
+        <v>3508</v>
+      </c>
+      <c r="J9">
+        <v>3472</v>
+      </c>
+      <c r="K9">
+        <v>3438</v>
+      </c>
+      <c r="L9">
+        <v>3458</v>
+      </c>
+      <c r="M9">
+        <v>2874</v>
+      </c>
+      <c r="N9">
+        <v>3225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>179521</v>
+      </c>
+      <c r="C10">
+        <v>143113</v>
+      </c>
+      <c r="D10">
+        <v>3950</v>
+      </c>
+      <c r="E10">
+        <v>3429</v>
+      </c>
+      <c r="F10">
+        <v>4327</v>
+      </c>
+      <c r="G10">
+        <v>5379</v>
+      </c>
+      <c r="H10">
+        <v>5671</v>
+      </c>
+      <c r="I10">
+        <v>6346</v>
+      </c>
+      <c r="J10">
+        <v>8569</v>
+      </c>
+      <c r="K10">
+        <v>6156</v>
+      </c>
+      <c r="L10">
+        <v>5398</v>
+      </c>
+      <c r="M10">
+        <v>4340</v>
+      </c>
+      <c r="N10">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11">
+        <v>158575</v>
+      </c>
+      <c r="C11">
+        <v>130267</v>
+      </c>
+      <c r="D11">
+        <v>2960</v>
+      </c>
+      <c r="E11">
+        <v>2838</v>
+      </c>
+      <c r="F11">
+        <v>3649</v>
+      </c>
+      <c r="G11">
+        <v>4078</v>
+      </c>
+      <c r="H11">
+        <v>4511</v>
+      </c>
+      <c r="I11">
+        <v>5165</v>
+      </c>
+      <c r="J11">
+        <v>5838</v>
+      </c>
+      <c r="K11">
+        <v>4787</v>
+      </c>
+      <c r="L11">
+        <v>4626</v>
+      </c>
+      <c r="M11">
+        <v>3618</v>
+      </c>
+      <c r="N11">
+        <v>4244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12">
+        <v>128899</v>
+      </c>
+      <c r="C12">
+        <v>112195</v>
+      </c>
+      <c r="D12">
+        <v>2668</v>
+      </c>
+      <c r="E12">
+        <v>2631</v>
+      </c>
+      <c r="F12">
+        <v>3040</v>
+      </c>
+      <c r="G12">
+        <v>3006</v>
+      </c>
+      <c r="H12">
+        <v>3080</v>
+      </c>
+      <c r="I12">
+        <v>3328</v>
+      </c>
+      <c r="J12">
+        <v>3227</v>
+      </c>
+      <c r="K12">
+        <v>2961</v>
+      </c>
+      <c r="L12">
+        <v>3374</v>
+      </c>
+      <c r="M12">
+        <v>2707</v>
+      </c>
+      <c r="N12">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13">
+        <v>305032</v>
+      </c>
+      <c r="C13">
+        <v>258026</v>
+      </c>
+      <c r="D13">
+        <v>5547</v>
+      </c>
+      <c r="E13">
+        <v>5545</v>
+      </c>
+      <c r="F13">
+        <v>6183</v>
+      </c>
+      <c r="G13">
+        <v>7260</v>
+      </c>
+      <c r="H13">
+        <v>7832</v>
+      </c>
+      <c r="I13">
+        <v>9226</v>
+      </c>
+      <c r="J13">
+        <v>10691</v>
+      </c>
+      <c r="K13">
+        <v>9127</v>
+      </c>
+      <c r="L13">
+        <v>8573</v>
+      </c>
+      <c r="M13">
+        <v>6838</v>
+      </c>
+      <c r="N13">
+        <v>7183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>172439</v>
+      </c>
+      <c r="C14">
+        <v>139603</v>
+      </c>
+      <c r="D14">
+        <v>4396</v>
+      </c>
+      <c r="E14">
+        <v>4238</v>
+      </c>
+      <c r="F14">
+        <v>4867</v>
+      </c>
+      <c r="G14">
+        <v>4739</v>
+      </c>
+      <c r="H14">
+        <v>5172</v>
+      </c>
+      <c r="I14">
+        <v>5643</v>
+      </c>
+      <c r="J14">
+        <v>6644</v>
+      </c>
+      <c r="K14">
+        <v>5527</v>
+      </c>
+      <c r="L14">
+        <v>5184</v>
+      </c>
+      <c r="M14">
+        <v>3800</v>
+      </c>
+      <c r="N14">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>50927</v>
+      </c>
+      <c r="C15">
+        <v>42748</v>
+      </c>
+      <c r="D15">
+        <v>1447</v>
+      </c>
+      <c r="E15">
+        <v>1391</v>
+      </c>
+      <c r="F15">
+        <v>1362</v>
+      </c>
+      <c r="G15">
+        <v>1740</v>
+      </c>
+      <c r="H15">
+        <v>1588</v>
+      </c>
+      <c r="I15">
+        <v>1503</v>
+      </c>
+      <c r="J15">
+        <v>1750</v>
+      </c>
+      <c r="K15">
+        <v>1444</v>
+      </c>
+      <c r="L15">
+        <v>1418</v>
+      </c>
+      <c r="M15">
+        <v>1142</v>
+      </c>
+      <c r="N15">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>208055</v>
+      </c>
+      <c r="C16">
+        <v>195237</v>
+      </c>
+      <c r="D16">
+        <v>4648</v>
+      </c>
+      <c r="E16">
+        <v>4494</v>
+      </c>
+      <c r="F16">
+        <v>4474</v>
+      </c>
+      <c r="G16">
+        <v>4938</v>
+      </c>
+      <c r="H16">
+        <v>5042</v>
+      </c>
+      <c r="I16">
+        <v>5308</v>
+      </c>
+      <c r="J16">
+        <v>5640</v>
+      </c>
+      <c r="K16">
+        <v>5743</v>
+      </c>
+      <c r="L16">
+        <v>6655</v>
+      </c>
+      <c r="M16">
+        <v>6339</v>
+      </c>
+      <c r="N16">
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17">
+        <v>317606</v>
+      </c>
+      <c r="C17">
+        <v>299985</v>
+      </c>
+      <c r="D17">
+        <v>6631</v>
+      </c>
+      <c r="E17">
+        <v>6319</v>
+      </c>
+      <c r="F17">
+        <v>7049</v>
+      </c>
+      <c r="G17">
+        <v>7783</v>
+      </c>
+      <c r="H17">
+        <v>8387</v>
+      </c>
+      <c r="I17">
+        <v>9023</v>
+      </c>
+      <c r="J17">
+        <v>8934</v>
+      </c>
+      <c r="K17">
+        <v>8603</v>
+      </c>
+      <c r="L17">
+        <v>8723</v>
+      </c>
+      <c r="M17">
+        <v>7646</v>
+      </c>
+      <c r="N17">
+        <v>9013</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18">
+        <v>109375</v>
+      </c>
+      <c r="C18">
+        <v>96381</v>
+      </c>
+      <c r="D18">
+        <v>2964</v>
+      </c>
+      <c r="E18">
+        <v>3074</v>
+      </c>
+      <c r="F18">
+        <v>3122</v>
+      </c>
+      <c r="G18">
+        <v>3005</v>
+      </c>
+      <c r="H18">
+        <v>2933</v>
+      </c>
+      <c r="I18">
+        <v>2935</v>
+      </c>
+      <c r="J18">
+        <v>3300</v>
+      </c>
+      <c r="K18">
+        <v>2935</v>
+      </c>
+      <c r="L18">
+        <v>2884</v>
+      </c>
+      <c r="M18">
+        <v>2805</v>
+      </c>
+      <c r="N18">
+        <v>2962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>122568</v>
+      </c>
+      <c r="C19">
+        <v>115564</v>
+      </c>
+      <c r="D19">
+        <v>2866</v>
+      </c>
+      <c r="E19">
+        <v>2697</v>
+      </c>
+      <c r="F19">
+        <v>3985</v>
+      </c>
+      <c r="G19">
+        <v>3445</v>
+      </c>
+      <c r="H19">
+        <v>3409</v>
+      </c>
+      <c r="I19">
+        <v>3623</v>
+      </c>
+      <c r="J19">
+        <v>3309</v>
+      </c>
+      <c r="K19">
+        <v>3153</v>
+      </c>
+      <c r="L19">
+        <v>3221</v>
+      </c>
+      <c r="M19">
+        <v>3365</v>
+      </c>
+      <c r="N19">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>454798</v>
+      </c>
+      <c r="C20">
+        <v>423407</v>
+      </c>
+      <c r="D20">
+        <v>9604</v>
+      </c>
+      <c r="E20">
+        <v>9668</v>
+      </c>
+      <c r="F20">
+        <v>11292</v>
+      </c>
+      <c r="G20">
+        <v>11712</v>
+      </c>
+      <c r="H20">
+        <v>10320</v>
+      </c>
+      <c r="I20">
+        <v>10894</v>
+      </c>
+      <c r="J20">
+        <v>10450</v>
+      </c>
+      <c r="K20">
+        <v>10180</v>
+      </c>
+      <c r="L20">
+        <v>9977</v>
+      </c>
+      <c r="M20">
+        <v>10123</v>
+      </c>
+      <c r="N20">
+        <v>11201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>296195</v>
+      </c>
+      <c r="C21">
+        <v>265419</v>
+      </c>
+      <c r="D21">
+        <v>6413</v>
+      </c>
+      <c r="E21">
+        <v>6691</v>
+      </c>
+      <c r="F21">
+        <v>7322</v>
+      </c>
+      <c r="G21">
+        <v>8220</v>
+      </c>
+      <c r="H21">
+        <v>9020</v>
+      </c>
+      <c r="I21">
+        <v>9049</v>
+      </c>
+      <c r="J21">
+        <v>8733</v>
+      </c>
+      <c r="K21">
+        <v>8934</v>
+      </c>
+      <c r="L21">
+        <v>8813</v>
+      </c>
+      <c r="M21">
+        <v>8220</v>
+      </c>
+      <c r="N21">
+        <v>9360</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>170017</v>
+      </c>
+      <c r="C22">
+        <v>159766</v>
+      </c>
+      <c r="D22">
         <v>3301</v>
       </c>
+      <c r="E22">
+        <v>3448</v>
+      </c>
       <c r="F22">
-        <v>4175</v>
+        <v>3983</v>
       </c>
       <c r="G22">
-        <v>3448</v>
+        <v>4804</v>
       </c>
       <c r="H22">
-        <v>4344</v>
+        <v>4580</v>
       </c>
       <c r="I22">
-        <v>3983</v>
+        <v>4215</v>
       </c>
       <c r="J22">
-        <v>4435</v>
+        <v>4222</v>
       </c>
       <c r="K22">
-        <v>4804</v>
+        <v>4063</v>
       </c>
       <c r="L22">
-        <v>3962</v>
+        <v>4682</v>
       </c>
       <c r="M22">
-        <v>4580</v>
+        <v>3973</v>
       </c>
       <c r="N22">
-        <v>4047</v>
-      </c>
-      <c r="O22">
-        <v>4215</v>
-      </c>
-      <c r="P22">
-        <v>3845</v>
-      </c>
-      <c r="Q22">
-        <v>4222</v>
-      </c>
-      <c r="R22">
-        <v>4239</v>
-      </c>
-      <c r="S22">
-        <v>4063</v>
-      </c>
-      <c r="T22">
-        <v>5101</v>
-      </c>
-      <c r="U22">
-        <v>4682</v>
-      </c>
-      <c r="V22">
-        <v>4452</v>
-      </c>
-      <c r="W22">
-        <v>3973</v>
-      </c>
-      <c r="X22">
-        <v>5080</v>
-      </c>
-      <c r="Y22">
         <v>4830</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add statistical facts about counties
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E32EF8-958E-4F72-B83D-B6C57B65C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B5C8D-3513-4DF7-99EC-3C7C67B5DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="696" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="711" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -24,6 +24,8 @@
     <sheet name="E-gradani" sheetId="9" r:id="rId9"/>
     <sheet name="Doseljeni" sheetId="10" r:id="rId10"/>
     <sheet name="Odseljeni" sheetId="11" r:id="rId11"/>
+    <sheet name="Stat" sheetId="12" r:id="rId12"/>
+    <sheet name="FunFacts" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="116">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -282,6 +284,126 @@
   <si>
     <t>Broj_stanovnika_2021</t>
   </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>Grad Zagreb je svoj vrhunac stanovništva doživio 2020. godine, do te brojke je došao sporim i kontinuiranim rastom dok je već sljedeće godine izgubio više od 40 tisuća stanovnika i dosegao svoju najlošiju godinu 21. stoljeća.</t>
+  </si>
+  <si>
+    <t>Krapinsko-zagorska u zadnjih 20 godina ima kontinuirani pad i novim popisom je doživjela najnižu razinu sa malo iznad 120 tisuća stanovnika.</t>
+  </si>
+  <si>
+    <t>Međimurska županija 2006. godine ostvaruje svoj maksimum po broju stanovnika, a od tada je u padu i 2021. doživljava svoje najniže brojke.</t>
+  </si>
+  <si>
+    <t>Zadarska je jedna od samo dvije županije koja u prošloj godini nije doživjela najnižu brojku u zadnjih 20 godina.</t>
+  </si>
+  <si>
+    <t>Zagrebačka je jedna od samo dvije županije koja u prošloj godini nije doživjela najnižu brojku u zadnjih 20 godina.</t>
+  </si>
+  <si>
+    <t>Varaždinska županija od 2001. doživljava kontinuirani, ali svom srećom, blagi pad u broju stanovnika.</t>
+  </si>
+  <si>
+    <t>Naša najmanja županija, Ličko-senjska, svakom godinom postaje sve manja...</t>
+  </si>
+  <si>
+    <t>Požeško-slavonska je jedna od samo tri županije koja imaju manje od 100 tisuća stanovnika</t>
+  </si>
+  <si>
+    <t>Druga najveća županija naše države je ponos Dalmacije, Splitsko-dalmatinska!</t>
+  </si>
+  <si>
+    <t>Po prvi puta u zadnjih 20 godina, Istarska županija pala je ispod 200 tisuća stanovnika.</t>
+  </si>
+  <si>
+    <t>Dubrovačko-neretvanska županija krasi se jednom od najmanjih oscilacija u proteklih 20 godina.</t>
+  </si>
+  <si>
+    <t>U Vukovarsko-srijemskoj, najveći broj stanovnika bilježi između 60 i 64 godine.</t>
+  </si>
+  <si>
+    <t>U Varaždinskoj županiji, najveći broj stanovnika ima raspon godina 55-59 što je jedna od najstarijih skupina gledajući sve županije.</t>
+  </si>
+  <si>
+    <t>U Brodsko-posavskoj, najveći broj stanovnika bilježi između 60 i 64 godine.</t>
+  </si>
+  <si>
+    <t>U Šibensko-kninskoj, najveći broj stanovnika bilježi između 65 i 69 godina.</t>
+  </si>
+  <si>
+    <t>Grad Zagreb je najmanji broj rođenih bilježio 2001. i 2002. godine, upravo godine kada su rođeni kreatori ove stranice. :)</t>
+  </si>
+  <si>
+    <t>Ličko-senjska je županija sa najmanje rođenih, a brojka već dugo nije prešla 400.</t>
+  </si>
+  <si>
+    <t>Iako ima godišnji prosjek od preko 760 i maksimum sa više od 1000 rođenih, Požeško-slavonska je u 2021. godini imala samo 572 rođene djece.</t>
+  </si>
+  <si>
+    <t>Osječko-baranjska je jedna od rijetkih županija koja zadnjih godina doživljava rast po pitanju rođene djece.</t>
+  </si>
+  <si>
+    <t>Uz Grad Zagreb, Splitsko-dalmatinska je jedina županija sa više od 3000 rođenih.</t>
+  </si>
+  <si>
+    <t>Iako ima najmanje umrlih, Ličko-senjska broji dva puta više umrlih od rođenih.</t>
+  </si>
+  <si>
+    <t>Splitsko-dalmatinska ima duplo više umrlih od rođenih.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka ima jedan od najgorih odnosa rođenih i umrlih od svih županija.</t>
+  </si>
+  <si>
+    <t>Karlovačka županija ima jedan od najgorih odnosa rođenih i umrlih od svih županija.</t>
+  </si>
+  <si>
+    <t>Istarska županija ima najviše brakova na 1000 stanovnika u 2021. godini!</t>
+  </si>
+  <si>
+    <t>Virovitičko-podravska županija ima najmanji broj brakova na 1000 stanovnika u protekloj godini.</t>
+  </si>
+  <si>
+    <t>Virovitičko-podravska je jedna od samo tri županije koja imaju manje od 100 tisuća stanovnika</t>
+  </si>
+  <si>
+    <t>Karlovačka županija ima kontinuirani rast po broju razvoda na 1000 stanovnika i od jedne od najboljih županija je migrirala u najgoru!</t>
+  </si>
+  <si>
+    <t>U Primorsko-goranskoj županiji se ljudi vole! Županija sa najmanje razvoda na 1000 stanovnika u protekloj godini!</t>
+  </si>
+  <si>
+    <t>Međimurska županije ima najveću brojku rođenih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primorsko-goranska županija je, kao i ostale, doživjela veliki pad u broju stanovnika 2021. godine. </t>
+  </si>
+  <si>
+    <t>U proteklih 20 godina, Dubrovačko-neretvanska je rekorder po broju rođenih na 1000 stanovnika u jednoj godini, a vrhunac je doživjela 2008. godine.</t>
+  </si>
+  <si>
+    <t>Bjelovarsko-bilogorska županija zauzima mjesto u top 3 po najvećem broju umrlih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka županija zauzima mjesto u top 5 po najvećem broju umrlih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Požeško-slavonska županija osvaja 1. mjesto po broju odseljenih ljudi u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Druga po broju odseljenih na 1000 stanovnika u prošloj godini - Primorsko-goranska!</t>
+  </si>
+  <si>
+    <t>Istarska županija je rekorder po broju doseljenih na 1000 stanovnika!</t>
+  </si>
 </sst>
 </file>
 
@@ -292,11 +414,19 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -369,6 +499,14 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -490,85 +628,104 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -887,11 +1044,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B6D3D3-7E78-4A0B-9947-33E237049D29}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A1:A23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -899,10 +1054,12 @@
     <col min="2" max="17" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="8.88671875" style="6"/>
     <col min="22" max="22" width="8.88671875" style="6" customWidth="1"/>
-    <col min="23" max="16384" width="8.88671875" style="6"/>
+    <col min="23" max="25" width="8.88671875" style="6"/>
+    <col min="26" max="26" width="8.88671875" style="31"/>
+    <col min="27" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -969,8 +1126,9 @@
       <c r="V1" s="4">
         <v>2021</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Z1" s="6"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1037,8 +1195,12 @@
       <c r="V2" s="16">
         <v>3878981</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -1105,8 +1267,13 @@
       <c r="V3" s="16">
         <v>768054</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="27"/>
+      <c r="AB3" s="29"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -1173,8 +1340,13 @@
       <c r="V4" s="16">
         <v>105393</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="27"/>
+      <c r="AB4" s="29"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -1241,8 +1413,13 @@
       <c r="V5" s="16">
         <v>120670</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
+      <c r="Y5" s="28"/>
+      <c r="Z5" s="27"/>
+      <c r="AB5" s="29"/>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -1309,8 +1486,13 @@
       <c r="V6" s="16">
         <v>159747</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="27"/>
+      <c r="AB6" s="29"/>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -1377,8 +1559,13 @@
       <c r="V7" s="16">
         <v>70648</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="27"/>
+      <c r="AB7" s="29"/>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -1445,8 +1632,13 @@
       <c r="V8" s="16">
         <v>64384</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="27"/>
+      <c r="AB8" s="29"/>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -1513,8 +1705,12 @@
       <c r="V9" s="16">
         <v>101358</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="27"/>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -1581,8 +1777,12 @@
       <c r="V10" s="16">
         <v>102205</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="27"/>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -1649,8 +1849,12 @@
       <c r="V11" s="16">
         <v>143678</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="27"/>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1717,8 +1921,12 @@
       <c r="V12" s="16">
         <v>130844</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="27"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -1785,8 +1993,12 @@
       <c r="V13" s="16">
         <v>112357</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="27"/>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -1853,8 +2065,12 @@
       <c r="V14" s="16">
         <v>258719</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="27"/>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -1921,8 +2137,12 @@
       <c r="V15" s="16">
         <v>140131</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="27"/>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -1989,8 +2209,13 @@
       <c r="V16" s="16">
         <v>42931</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="27"/>
+      <c r="AB16" s="29"/>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -2057,8 +2282,13 @@
       <c r="V17" s="16">
         <v>195326</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="27"/>
+      <c r="AB17" s="29"/>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -2125,8 +2355,13 @@
       <c r="V18" s="16">
         <v>299983</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="27"/>
+      <c r="AB18" s="29"/>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -2193,8 +2428,12 @@
       <c r="V19" s="16">
         <v>96722</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W19" s="28"/>
+      <c r="X19" s="28"/>
+      <c r="Y19" s="28"/>
+      <c r="Z19" s="27"/>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -2261,8 +2500,13 @@
       <c r="V20" s="16">
         <v>115714</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W20" s="28"/>
+      <c r="X20" s="28"/>
+      <c r="Y20" s="28"/>
+      <c r="Z20" s="27"/>
+      <c r="AB20" s="29"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -2329,8 +2573,13 @@
       <c r="V21" s="16">
         <v>423849</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="27"/>
+      <c r="AB21" s="29"/>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -2397,8 +2646,13 @@
       <c r="V22" s="16">
         <v>266183</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="28"/>
+      <c r="Z22" s="27"/>
+      <c r="AB22" s="29"/>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -2465,12 +2719,27 @@
       <c r="V23" s="16">
         <v>160085</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="27"/>
+      <c r="AB23" s="29"/>
+    </row>
+    <row r="24" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z24" s="30"/>
+    </row>
+    <row r="25" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z25" s="30"/>
+    </row>
+    <row r="26" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="30"/>
+    </row>
+    <row r="27" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z27" s="30"/>
+    </row>
+    <row r="28" spans="1:28" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z28" s="30"/>
+    </row>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
@@ -3480,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F98E4D1-812A-43FC-A5E2-E0E4232BE4B7}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4457,6 +4726,908 @@
       </c>
       <c r="N22">
         <v>4830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34156728-7C93-420C-97DD-DA6B5A95B5FA}">
+  <dimension ref="A1:F63"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.88671875" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
+    </row>
+    <row r="4" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="34"/>
+      <c r="D4" s="35"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="35"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="33"/>
+    </row>
+    <row r="13" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
+    </row>
+    <row r="16" spans="1:5" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="33"/>
+    </row>
+    <row r="18" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+    </row>
+    <row r="23" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+    </row>
+    <row r="24" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+    </row>
+    <row r="25" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+    </row>
+    <row r="26" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+    </row>
+    <row r="28" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+    </row>
+    <row r="32" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+    </row>
+    <row r="33" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="33"/>
+    </row>
+    <row r="34" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="35"/>
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="35"/>
+      <c r="D36" s="34"/>
+      <c r="F36" s="33"/>
+    </row>
+    <row r="37" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="35"/>
+      <c r="D37" s="34"/>
+      <c r="F37" s="33"/>
+    </row>
+    <row r="38" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="34"/>
+      <c r="F38" s="33"/>
+    </row>
+    <row r="39" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="35"/>
+      <c r="D39" s="34"/>
+      <c r="F39" s="33"/>
+    </row>
+    <row r="40" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="D40" s="34"/>
+      <c r="F40" s="33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="35"/>
+      <c r="D41" s="34"/>
+    </row>
+    <row r="42" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="35"/>
+      <c r="D42" s="34"/>
+    </row>
+    <row r="43" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="35"/>
+      <c r="D43" s="34"/>
+    </row>
+    <row r="44" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="35"/>
+      <c r="D44" s="34"/>
+    </row>
+    <row r="45" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="37" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A55" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="37" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44DD792-A487-4A16-AC6D-C5624634E301}">
+  <dimension ref="A1:A63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B4" sqref="B4:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -5036,10 +6207,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2E0C36-09D8-4EB7-A499-252CB751FF76}">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U2" sqref="U2:X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5049,7 +6221,7 @@
     <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -5111,7 +6283,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -5173,8 +6345,11 @@
       <c r="T2" s="8">
         <v>91851</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -5235,8 +6410,11 @@
       <c r="T3" s="7">
         <v>17364</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -5297,8 +6475,11 @@
       <c r="T4" s="7">
         <v>2182</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -5360,8 +6541,11 @@
       <c r="T5" s="7">
         <v>2668</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -5422,8 +6606,12 @@
       <c r="T6" s="7">
         <v>3273</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="29"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -5484,8 +6672,11 @@
       <c r="T7" s="7">
         <v>1507</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -5546,8 +6737,11 @@
       <c r="T8" s="7">
         <v>1425</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -5608,8 +6802,11 @@
       <c r="T9" s="7">
         <v>2163</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -5670,8 +6867,11 @@
       <c r="T10" s="7">
         <v>2402</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -5732,8 +6932,12 @@
       <c r="T11" s="7">
         <v>3172</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="29"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -5794,8 +6998,12 @@
       <c r="T12" s="7">
         <v>3018</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="29"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -5856,8 +7064,11 @@
       <c r="T13" s="7">
         <v>3436</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -5918,8 +7129,11 @@
       <c r="T14" s="7">
         <v>5137</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -5980,8 +7194,11 @@
       <c r="T15" s="7">
         <v>3460</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -6042,8 +7259,11 @@
       <c r="T16" s="7">
         <v>1552</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -6104,8 +7324,11 @@
       <c r="T17" s="7">
         <v>5419</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -6167,8 +7390,11 @@
       <c r="T18" s="7">
         <v>5996</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -6229,8 +7455,12 @@
       <c r="T19" s="7">
         <v>3209</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U19" s="28"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="29"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -6291,8 +7521,11 @@
       <c r="T20" s="7">
         <v>3004</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U20" s="28"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="28"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -6353,8 +7586,11 @@
       <c r="T21" s="7">
         <v>10018</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U21" s="28"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -6415,8 +7651,11 @@
       <c r="T22" s="7">
         <v>7470</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -6477,6 +7716,9 @@
       <c r="T23" s="7">
         <v>3976</v>
       </c>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A24:T44">
@@ -6489,10 +7731,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5297FED2-5EBA-4D2B-8A6B-B31986E220AB}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6509,7 +7752,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -6586,7 +7829,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -6662,8 +7905,11 @@
       <c r="Y2" s="8">
         <v>36508</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -6739,8 +7985,12 @@
       <c r="Y3" s="8">
         <v>8030</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="29"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -6816,8 +8066,11 @@
       <c r="Y4" s="8">
         <v>1129</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -6893,8 +8146,11 @@
       <c r="Y5" s="8">
         <v>1080</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z5" s="28"/>
+      <c r="AA5" s="28"/>
+      <c r="AB5" s="28"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -6970,8 +8226,11 @@
       <c r="Y6" s="8">
         <v>1425</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -7047,8 +8306,11 @@
       <c r="Y7" s="8">
         <v>675</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -7124,8 +8386,12 @@
       <c r="Y8" s="8">
         <v>572</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="29"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -7201,8 +8467,11 @@
       <c r="Y9" s="8">
         <v>973</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -7278,8 +8547,11 @@
       <c r="Y10" s="8">
         <v>959</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -7355,8 +8627,11 @@
       <c r="Y11" s="8">
         <v>1266</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -7432,8 +8707,11 @@
       <c r="Y12" s="8">
         <v>1185</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -7509,8 +8787,11 @@
       <c r="Y13" s="8">
         <v>860</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -7586,8 +8867,12 @@
       <c r="Y14" s="8">
         <v>2352</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="29"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -7663,8 +8948,11 @@
       <c r="Y15" s="8">
         <v>1176</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -7740,8 +9028,12 @@
       <c r="Y16" s="8">
         <v>395</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="29"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -7817,8 +9109,11 @@
       <c r="Y17" s="8">
         <v>1657</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -7894,8 +9189,11 @@
       <c r="Y18" s="8">
         <v>2830</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -7971,8 +9269,11 @@
       <c r="Y19" s="8">
         <v>789</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -8048,8 +9349,11 @@
       <c r="Y20" s="8">
         <v>1199</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -8125,8 +9429,12 @@
       <c r="Y21" s="8">
         <v>4211</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="29"/>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -8202,8 +9510,11 @@
       <c r="Y22" s="8">
         <v>2154</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z22" s="28"/>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="28"/>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -8279,6 +9590,9 @@
       <c r="Y23" s="8">
         <v>1591</v>
       </c>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="28"/>
+      <c r="AB23" s="28"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Y23">
@@ -8301,10 +9615,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2911E758-2CF6-4B3F-A46B-43F4C13C86DC}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
+      <selection activeCell="Z13" sqref="Z13:Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8321,7 +9635,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -8398,7 +9712,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -8474,8 +9788,11 @@
       <c r="Y2" s="8">
         <v>62712</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -8551,8 +9868,11 @@
       <c r="Y3" s="8">
         <v>10962</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -8629,7 +9949,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -8706,7 +10026,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -8783,7 +10103,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -8860,7 +10180,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -8937,7 +10257,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -9014,7 +10334,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -9091,7 +10411,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -9168,7 +10488,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -9245,7 +10565,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -9322,7 +10642,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -9399,7 +10719,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -9476,7 +10796,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -10113,10 +11433,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1A7E52-2986-4975-BF52-05AC82283890}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
+      <selection activeCell="Z2" sqref="Z2:AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10133,7 +11453,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -10210,7 +11530,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -10286,8 +11606,17 @@
       <c r="Y2" s="8">
         <v>18203</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -10363,8 +11692,20 @@
       <c r="Y3" s="8">
         <v>3671</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="28" t="e">
+        <f>(MAX(#REF!))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA3" s="28" t="e">
+        <f>MIN(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AB3" s="28" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -10441,7 +11782,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -10518,7 +11859,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -10595,7 +11936,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -10672,7 +12013,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -10749,7 +12090,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -10826,7 +12167,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -10903,7 +12244,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -10980,7 +12321,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -11057,7 +12398,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -11134,7 +12475,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -11211,7 +12552,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -11288,7 +12629,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -11922,10 +13263,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5010BC67-7950-4090-BE5A-0AABB8636ABD}">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A23"/>
+      <selection activeCell="Z2" sqref="Z2:AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11942,7 +13283,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -12019,7 +13360,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -12095,8 +13436,17 @@
       <c r="Y2" s="8">
         <v>5100</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z2" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -12172,8 +13522,20 @@
       <c r="Y3" s="8">
         <v>1023</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="Z3" s="28" t="e">
+        <f>(MAX(#REF!))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AA3" s="28" t="e">
+        <f>MIN(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AB3" s="28" t="e">
+        <f>AVERAGE(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -12250,7 +13612,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -12327,7 +13689,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -12404,7 +13766,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -12481,7 +13843,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -12558,7 +13920,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -12635,7 +13997,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -12712,7 +14074,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -12789,7 +14151,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -12866,7 +14228,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -12943,7 +14305,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -13020,7 +14382,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -13097,7 +14459,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -13734,7 +15096,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add fun facts abou 10 counties
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58B5C8D-3513-4DF7-99EC-3C7C67B5DB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D307787-7964-4E68-91CF-EDFDEE437629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="711" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="711" firstSheet="8" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="147">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -403,6 +403,99 @@
   </si>
   <si>
     <t>Istarska županija je rekorder po broju doseljenih na 1000 stanovnika!</t>
+  </si>
+  <si>
+    <t>U Međimurskoj županiji nalazi se najsjevernija točka naše države.</t>
+  </si>
+  <si>
+    <t>Prvo nalazište nafte u Hrvatskoj pronađeno je upravo u Međimurju, u mjestu Peklenica.</t>
+  </si>
+  <si>
+    <t>Međimurci su ispleli najveću košaru od šibe koja je priznata u cijelome svijetu!</t>
+  </si>
+  <si>
+    <t>U Krapinskoj-zagorskoj županiji nalazi se Marija Bistrica, najveće hrvatsko svetište Majke Božje.</t>
+  </si>
+  <si>
+    <t>Na Hušnjakovu brijegu u Krapinsko-zagorskoj županiji nalazi se jedno od najstarijih nalazišta pračovjeka u Europi te ima i muzej posvećen tome.</t>
+  </si>
+  <si>
+    <t>Krapinsko-zagorska županija odlikuje se nejvećim brojem dvoraca po četvornom kilometru u Hrvatskoj.</t>
+  </si>
+  <si>
+    <t>Sjedište Varaždinske županije, Varaždin, je bivši hrvatski glavni grad!</t>
+  </si>
+  <si>
+    <t>U Varaždinskoj županiji nalazi se špilja Vindija u kojoj su otkriveni ostaci neandertalskog pračovjeka.</t>
+  </si>
+  <si>
+    <t>Dvorac Trakošćan jedan je od najljepših dvoraca u Hrvatskoj i nalazi se u Varaždinskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Slatini je proizveden prvi hrvatski pjenušac i na ponos je Virovitičko-podravske županije.</t>
+  </si>
+  <si>
+    <t>Park prirode Papuk odlično je mjesto za ljubitelje prirode, a nalazi se u Virovitičko-podravskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Virovitici je 1242. godine hrvatsko-ugarski kralj Bela IV. Izdao Zlatnu bulu kojem je Gradec (današnji Zagreb) stekao status grada!</t>
+  </si>
+  <si>
+    <t>Iako se dio njega nalazi u Virovitičko-podravskoj županiji, Park prirode Papuk prirodna je atrakcija i Požeško-slavonske županije.</t>
+  </si>
+  <si>
+    <t>U Požeško-slavonskoj županiji nalazi se Kutjevo, poznato pod Kutjevu d.d., jednom od naših najvećih proizvođača vina.</t>
+  </si>
+  <si>
+    <t>U Požegi se nalazi velebni Spomenik 123. brigadi Hrvatske vojske.</t>
+  </si>
+  <si>
+    <t>U Koprivnici se nalazi povijesni Franjevački samostan i crkva Sv. Antuna Padovanskog.</t>
+  </si>
+  <si>
+    <t>Gradska palača, izgrađena u 18. stoljeću, vrijedan je dio povijesti koji se isplati vidjeti, a nalazi se u sjedištu županije.</t>
+  </si>
+  <si>
+    <t>Koprivničko-križevačka županija ima sjedište najveće farmaceutske firme u hrvatskom vlasništvu - Belupo!</t>
+  </si>
+  <si>
+    <t>U Varaždinu će se 2023. godine održati svjetsko seniorsko kuglačko prvenstvo!</t>
+  </si>
+  <si>
+    <t>Bjelovarsko-bilogorska županija dom je mnogih poznatih manifestacija koje se rastežu kroz cijelu godinu i uvijek vrijedi otići.</t>
+  </si>
+  <si>
+    <t>Za ljude željne prirode, Bjelovarsko-bilogorska županija nudi opcije kao što su Moslavačka gora, Papuk i Bilogora!</t>
+  </si>
+  <si>
+    <t>Tko se odluči posjetiti Daruvar, može uživati u toplim kupeljima koje sežu još od rimskih vremena.</t>
+  </si>
+  <si>
+    <t>U Vukovarskoj-srijemskoj se nalazi Vučedol, jedan od najznačajnijih lokaliteta neolitika i Vučedolske kulture.</t>
+  </si>
+  <si>
+    <t>Vukovarski vodotoranj jedan je od najvećih spomenika i obilježava velik dio hrvatske povijesti!</t>
+  </si>
+  <si>
+    <t>Najistočnija županija Republike Hrvatske.</t>
+  </si>
+  <si>
+    <t>U Karlovačkoj županiji može se posjetiti Rastoke, poznate i kao "Plitvice u malom", predivan prirodni krajolik sa slapovima i adrenalinskim atrakcijama.</t>
+  </si>
+  <si>
+    <t>Karlovac, grad na 4 rijeke, povijesna je atrakcija koju vrijedi obići.</t>
+  </si>
+  <si>
+    <t>Tko voli stare zidine i dvorce, a nalazi se u Karlovačkoj županiji, ne smije zaobići Stari grad Dubovac.</t>
+  </si>
+  <si>
+    <t>U Đakovu se nalazi predivna katedrala, po kojoj je i grad poznat, a samim time i Osječko-baranjska županija.</t>
+  </si>
+  <si>
+    <t>U Osječko-baranjskoj županiji nalazi se najstariji park prirode u Hrvatskoj - Kopački rit.</t>
+  </si>
+  <si>
+    <t>Baranja je poznato vinsko središte Hrvatske i nezaobilazna postaja za sve vinoljupce!</t>
   </si>
 </sst>
 </file>
@@ -4737,7 +4830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34156728-7C93-420C-97DD-DA6B5A95B5FA}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:A63"/>
     </sheetView>
   </sheetViews>
@@ -5302,11 +5395,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44DD792-A487-4A16-AC6D-C5624634E301}">
-  <dimension ref="A1:A63"/>
+  <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B4" sqref="B4:B15"/>
+      <selection pane="topRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5315,249 +5408,342 @@
     <col min="2" max="2" width="119.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -5572,7 +5758,7 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
@@ -5587,7 +5773,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -5602,7 +5788,7 @@
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -5617,7 +5803,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -5627,6 +5813,11 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="32" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add fun facts about the rest of the counties
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D307787-7964-4E68-91CF-EDFDEE437629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CA34E2-3F39-4E78-BAF5-9EB9FE894AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="711" firstSheet="8" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="696" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="711" firstSheet="8" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="177">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -423,9 +423,6 @@
     <t>Krapinsko-zagorska županija odlikuje se nejvećim brojem dvoraca po četvornom kilometru u Hrvatskoj.</t>
   </si>
   <si>
-    <t>Sjedište Varaždinske županije, Varaždin, je bivši hrvatski glavni grad!</t>
-  </si>
-  <si>
     <t>U Varaždinskoj županiji nalazi se špilja Vindija u kojoj su otkriveni ostaci neandertalskog pračovjeka.</t>
   </si>
   <si>
@@ -496,6 +493,99 @@
   </si>
   <si>
     <t>Baranja je poznato vinsko središte Hrvatske i nezaobilazna postaja za sve vinoljupce!</t>
+  </si>
+  <si>
+    <t>Plitvička jezera su nezaobilazna atrakcija Ličko-senjske županije, kao i preostala dva nacionalna parka: Paklenica i Sjeverni Velebit!</t>
+  </si>
+  <si>
+    <t>Poznata Kula Nehaj simbol je grada Senja, najstarijeg grada na gornjem Jadranu i ponosa Ličko-senjske županije.</t>
+  </si>
+  <si>
+    <t>Mi Hrvati se ponosimo Nikolom Teslom, a u Ličko-senjskoj županiji možete posjetiti "Memorijalni centar Nikola Tesla"</t>
+  </si>
+  <si>
+    <t>Nacionalni park Brijuni jedan je od najljepših naših parkova, a nalazi se u Istarskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Istri se nalazi najmanji grad na svijetu - Hum!</t>
+  </si>
+  <si>
+    <t>Za gurmane, u Istri je pronađen najveći tartuf na svijetu.</t>
+  </si>
+  <si>
+    <t>U centru Zagreba nalazi se najmanja žičana željeznica na svijetu, a povezuje Donji i Gornji grad.</t>
+  </si>
+  <si>
+    <t>Lenucijeva potkova, kompleks od 7 trgova i parkova u centru Zagreba, prepuna je zelenila i može biti put za predivnu šetnju gradom!</t>
+  </si>
+  <si>
+    <t>Grad Zagreb dom je najvećeg i najuspješnijeg hrvatskog nogometnog kluba, Dinama.</t>
+  </si>
+  <si>
+    <t>Ljubitelji prirode mogu posjetiti Stari grad Samobor i Samoborsko gorje, uz predivnu prirodu može se vidjeti i dvorac iz 13. stoljeća.</t>
+  </si>
+  <si>
+    <t>Tradicionalne kremšnite potječu iz Samobora, delicija poznata diljem svijeta. Gdje bolje probati tako nešto, ako ne u gradu gdje je nastala.</t>
+  </si>
+  <si>
+    <t>U Zagrebačkoj županiji nalazi se najveća hrvatska zračna luka - Zračna luka doktora Franje Tuđmana.</t>
+  </si>
+  <si>
+    <t>Sisački stari grad dio je povijesti kojim se Sisak ponosi i isplati se posjetiti ga.</t>
+  </si>
+  <si>
+    <t>Lonjsko polje je park prirode Hrvatske i nalazi se u Sisačko-moslavačkoj županiji.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka županija bivše je industrijsko središte Hrvatske, sa sisačkom naftnom rafinerijom i željezarom te kutinskom petrokemijom kao njihovim najvećim pokretačima</t>
+  </si>
+  <si>
+    <t>Sjedište Varaždinske županije, Varaždin, je bivši hrvatski glavni grad, a Ludbreg je poznat kao centar svijeta!</t>
+  </si>
+  <si>
+    <t>Dubrovnik je prije bio republika za sebe i to zauzima velik dio njegove povijesti!</t>
+  </si>
+  <si>
+    <t>Dubrovačke zidine su velebna atrakcija i predivan dio povijesti. Na istim tim zidinama snimane su i scene jedne od najpoznatijih svjetskih serija - Game of Thrones.</t>
+  </si>
+  <si>
+    <t>Arboretum Trsteno u blizini Dubrovnika, osnovan je u 15. stoljeću i najstariji je arboretum na svijetu!</t>
+  </si>
+  <si>
+    <t>Sjedište Primorsko-goranske županije, Rijeka, predivan je grad na obali Jadranskog mora. Ako ju poželite posjetiti u proljetnim ili jesenskim mjesecima, ponesite kišobran!</t>
+  </si>
+  <si>
+    <t>Ljubitelji prirode, ako ste u Primorsko-goranskoj županiji, nemojte zaobići njihov nacionalni park Risnjak, nećete požaliti! U obilasku možete navratiti i do Bijelih i Samarskih stijena.</t>
+  </si>
+  <si>
+    <t>Na otoku Cresu nalazi se prirodni rezervat bjeloglavih supova, ugrožene životinjske vrste.</t>
+  </si>
+  <si>
+    <t>Šetnja obalom može postati posebna ako ste u Zadru! Uz melodične zvukove morskih orgulja i Pozdrav suncu, šetnja će postati lijepa uspomena.</t>
+  </si>
+  <si>
+    <t>Šibenik je prvi grad na svijetu koji je dobio javnu rasvjetu na izmjeničnu električnu struju.</t>
+  </si>
+  <si>
+    <t>Dražen Petrović ili "košarkaški Mozart", najveći i neprežaljeni talent hrvatske košarke, potječe iz Šibenika!</t>
+  </si>
+  <si>
+    <t>Četvrt Varoš u Šibeniku poznata je jer su u njoj stasali velikani hrvatske glazbene scene: Arsen Dedić, Vice Vukov i Mate Mišo Kovač.</t>
+  </si>
+  <si>
+    <t>Grijeh je otići u Split, a ne posjetiti Dioklecijanovu palaču - jednu od najbolje očuvanih rimskih građevina u svijetu!</t>
+  </si>
+  <si>
+    <t>Modra špilja kod mjesta Komiže svjetska je turistička atrakcija i vrijedna obilaska!</t>
+  </si>
+  <si>
+    <t>Na otoku Braču koji je smješten u Splitsko-dalmatinskoj županiji, nalazi se plaža Zlatni rat u mjestu Bol, koja spada u jedne od najljepših plaža na svijetu.</t>
+  </si>
+  <si>
+    <t>U zaleđu Zadra može se posjetiti park prirode Vransko jezero, koji spaja močvaru s raznovrsnim ekosustavom, razvedenu obalu Jadrana i ruralni ambijent Ravnih kotara!</t>
+  </si>
+  <si>
+    <t>Rijeka Zrmanja stvorila je poseban geomorfološki spomenik prirode koji se nalazi prije ušća Zrmanje u Novigradsko more.</t>
   </si>
 </sst>
 </file>
@@ -5397,9 +5487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44DD792-A487-4A16-AC6D-C5624634E301}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B38" sqref="B38"/>
+      <selection pane="topRight" activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5412,16 +5502,25 @@
       <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
+      <c r="B1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>31</v>
       </c>
+      <c r="B2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>31</v>
       </c>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -5476,7 +5575,7 @@
         <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5484,7 +5583,7 @@
         <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5492,7 +5591,7 @@
         <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5500,7 +5599,7 @@
         <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5508,7 +5607,7 @@
         <v>57</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -5516,7 +5615,7 @@
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5524,7 +5623,7 @@
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -5532,7 +5631,7 @@
         <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -5540,7 +5639,7 @@
         <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -5548,7 +5647,7 @@
         <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5556,7 +5655,7 @@
         <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -5564,7 +5663,7 @@
         <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5572,7 +5671,7 @@
         <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -5580,7 +5679,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -5588,7 +5687,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -5596,7 +5695,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -5604,7 +5703,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -5612,7 +5711,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -5620,7 +5719,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -5643,7 +5742,7 @@
         <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -5651,7 +5750,7 @@
         <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -5659,7 +5758,7 @@
         <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -5667,7 +5766,7 @@
         <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -5675,7 +5774,7 @@
         <v>61</v>
       </c>
       <c r="B36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -5683,142 +5782,223 @@
         <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="B38" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="B39" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="B40" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
         <v>63</v>
       </c>
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>63</v>
       </c>
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
         <v>63</v>
       </c>
+      <c r="B43" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>30</v>
       </c>
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
         <v>30</v>
       </c>
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>30</v>
       </c>
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>64</v>
       </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
         <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodana dobno spolna piramida i u excelici podatci za nju
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karlo\Documents\GitHub\crostats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\ProjektR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E32EF8-958E-4F72-B83D-B6C57B65C5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C075CE2-B76A-4670-99E9-FE02D06ED291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="10" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="11" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="E-gradani" sheetId="9" r:id="rId9"/>
     <sheet name="Doseljeni" sheetId="10" r:id="rId10"/>
     <sheet name="Odseljeni" sheetId="11" r:id="rId11"/>
+    <sheet name="dobno_spolna" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="112">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -282,6 +283,117 @@
   <si>
     <t>Broj_stanovnika_2021</t>
   </si>
+  <si>
+    <t>Županija</t>
+  </si>
+  <si>
+    <t>Jedinica lokalne samouprave</t>
+  </si>
+  <si>
+    <t>County of</t>
+  </si>
+  <si>
+    <t>Local self-government unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grad/općina  
+Town/Municipality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naselje
+Settlement </t>
+  </si>
+  <si>
+    <t>Spol</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Ukupno
+Total</t>
+  </si>
+  <si>
+    <t>0 – 4</t>
+  </si>
+  <si>
+    <t>5 – 9</t>
+  </si>
+  <si>
+    <t>10 – 14</t>
+  </si>
+  <si>
+    <t>15 – 19</t>
+  </si>
+  <si>
+    <t>20 – 24</t>
+  </si>
+  <si>
+    <t>25 – 29</t>
+  </si>
+  <si>
+    <t>30 – 34</t>
+  </si>
+  <si>
+    <t>35 – 39</t>
+  </si>
+  <si>
+    <t>40 – 44</t>
+  </si>
+  <si>
+    <t>45 – 49</t>
+  </si>
+  <si>
+    <t>50 – 54</t>
+  </si>
+  <si>
+    <t>55 – 59</t>
+  </si>
+  <si>
+    <t>60 – 64</t>
+  </si>
+  <si>
+    <t>65 – 69</t>
+  </si>
+  <si>
+    <t>70 – 74</t>
+  </si>
+  <si>
+    <t>75 – 79</t>
+  </si>
+  <si>
+    <t>80 – 84</t>
+  </si>
+  <si>
+    <t>85 – 89</t>
+  </si>
+  <si>
+    <t>90 – 94</t>
+  </si>
+  <si>
+    <t>Republic of Croatia</t>
+  </si>
+  <si>
+    <t>sv.</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ž</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
 </sst>
 </file>
 
@@ -292,7 +404,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -495,7 +607,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -569,6 +681,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -879,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -893,7 +1009,7 @@
       <selection activeCell="A23" sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="17" width="8.88671875" style="6" bestFit="1" customWidth="1"/>
@@ -902,7 +1018,7 @@
     <col min="23" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -970,7 +1086,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1154,7 @@
         <v>3878981</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -1106,7 +1222,7 @@
         <v>768054</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -1174,7 +1290,7 @@
         <v>105393</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -1242,7 +1358,7 @@
         <v>120670</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -1310,7 +1426,7 @@
         <v>159747</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -1378,7 +1494,7 @@
         <v>70648</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -1446,7 +1562,7 @@
         <v>64384</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -1514,7 +1630,7 @@
         <v>101358</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -1582,7 +1698,7 @@
         <v>102205</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -1650,7 +1766,7 @@
         <v>143678</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -1718,7 +1834,7 @@
         <v>130844</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -1786,7 +1902,7 @@
         <v>112357</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -1854,7 +1970,7 @@
         <v>258719</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -1922,7 +2038,7 @@
         <v>140131</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -1990,7 +2106,7 @@
         <v>42931</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -2058,7 +2174,7 @@
         <v>195326</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -2126,7 +2242,7 @@
         <v>299983</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -2194,7 +2310,7 @@
         <v>96722</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -2262,7 +2378,7 @@
         <v>115714</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -2330,7 +2446,7 @@
         <v>423849</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -2398,7 +2514,7 @@
         <v>266183</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -2466,11 +2582,11 @@
         <v>160085</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="25" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="26" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="27" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
+    <row r="28" spans="1:22" s="19" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.35433070866141736" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
@@ -2496,14 +2612,14 @@
       <selection activeCell="O1" sqref="O1:P1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -2547,7 +2663,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2591,7 +2707,7 @@
         <v>19412</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2635,7 +2751,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2679,7 +2795,7 @@
         <v>3410</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -2723,7 +2839,7 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -2767,7 +2883,7 @@
         <v>1435</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2811,7 +2927,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2855,7 +2971,7 @@
         <v>2525</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -2899,7 +3015,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2943,7 +3059,7 @@
         <v>3307</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2987,7 +3103,7 @@
         <v>2976</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -3031,7 +3147,7 @@
         <v>2879</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -3075,7 +3191,7 @@
         <v>5961</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -3119,7 +3235,7 @@
         <v>3743</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -3163,7 +3279,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3207,7 +3323,7 @@
         <v>7540</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -3251,7 +3367,7 @@
         <v>10759</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -3295,7 +3411,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -3339,7 +3455,7 @@
         <v>3370</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -3383,7 +3499,7 @@
         <v>11116</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -3427,7 +3543,7 @@
         <v>8828</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -3480,18 +3596,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F98E4D1-812A-43FC-A5E2-E0E4232BE4B7}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -3535,7 +3651,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3579,7 +3695,7 @@
         <v>18549</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -3623,7 +3739,7 @@
         <v>3277</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3667,7 +3783,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3711,7 +3827,7 @@
         <v>4112</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -3755,7 +3871,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -3799,7 +3915,7 @@
         <v>2319</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3843,7 +3959,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3887,7 +4003,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3931,7 +4047,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -3975,7 +4091,7 @@
         <v>4244</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -4019,7 +4135,7 @@
         <v>3030</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -4063,7 +4179,7 @@
         <v>7183</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -4107,7 +4223,7 @@
         <v>4670</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -4151,7 +4267,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -4195,7 +4311,7 @@
         <v>6729</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -4239,7 +4355,7 @@
         <v>9013</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>65</v>
       </c>
@@ -4283,7 +4399,7 @@
         <v>2962</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>66</v>
       </c>
@@ -4327,7 +4443,7 @@
         <v>4006</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -4371,7 +4487,7 @@
         <v>11201</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4415,7 +4531,7 @@
         <v>9360</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4457,6 +4573,341 @@
       </c>
       <c r="N22">
         <v>4830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9B41DD-50AF-44FF-9624-414E1786BABA}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:29" ht="52.8">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="28">
+        <v>3871833</v>
+      </c>
+      <c r="J2" s="28">
+        <v>175535</v>
+      </c>
+      <c r="K2" s="28">
+        <v>181445</v>
+      </c>
+      <c r="L2" s="28">
+        <v>195436</v>
+      </c>
+      <c r="M2" s="28">
+        <v>188729</v>
+      </c>
+      <c r="N2" s="28">
+        <v>208852</v>
+      </c>
+      <c r="O2" s="28">
+        <v>214023</v>
+      </c>
+      <c r="P2" s="28">
+        <v>227551</v>
+      </c>
+      <c r="Q2" s="28">
+        <v>255617</v>
+      </c>
+      <c r="R2" s="28">
+        <v>267349</v>
+      </c>
+      <c r="S2" s="28">
+        <v>260146</v>
+      </c>
+      <c r="T2" s="28">
+        <v>260056</v>
+      </c>
+      <c r="U2" s="28">
+        <v>279504</v>
+      </c>
+      <c r="V2" s="28">
+        <v>288351</v>
+      </c>
+      <c r="W2" s="28">
+        <v>279106</v>
+      </c>
+      <c r="X2" s="28">
+        <v>228612</v>
+      </c>
+      <c r="Y2" s="28">
+        <v>146855</v>
+      </c>
+      <c r="Z2" s="28">
+        <v>122719</v>
+      </c>
+      <c r="AA2" s="28">
+        <v>67249</v>
+      </c>
+      <c r="AB2" s="28">
+        <v>21019</v>
+      </c>
+      <c r="AC2" s="28">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="28">
+        <v>1865129</v>
+      </c>
+      <c r="J3" s="28">
+        <v>90245</v>
+      </c>
+      <c r="K3" s="28">
+        <v>93311</v>
+      </c>
+      <c r="L3" s="28">
+        <v>100216</v>
+      </c>
+      <c r="M3" s="28">
+        <v>97228</v>
+      </c>
+      <c r="N3" s="28">
+        <v>107102</v>
+      </c>
+      <c r="O3" s="28">
+        <v>109139</v>
+      </c>
+      <c r="P3" s="28">
+        <v>114778</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>128398</v>
+      </c>
+      <c r="R3" s="28">
+        <v>134213</v>
+      </c>
+      <c r="S3" s="28">
+        <v>130035</v>
+      </c>
+      <c r="T3" s="28">
+        <v>127953</v>
+      </c>
+      <c r="U3" s="28">
+        <v>134655</v>
+      </c>
+      <c r="V3" s="28">
+        <v>136338</v>
+      </c>
+      <c r="W3" s="28">
+        <v>129728</v>
+      </c>
+      <c r="X3" s="28">
+        <v>100506</v>
+      </c>
+      <c r="Y3" s="28">
+        <v>59065</v>
+      </c>
+      <c r="Z3" s="28">
+        <v>44672</v>
+      </c>
+      <c r="AA3" s="28">
+        <v>21206</v>
+      </c>
+      <c r="AB3" s="28">
+        <v>5604</v>
+      </c>
+      <c r="AC3">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="28">
+        <v>2006704</v>
+      </c>
+      <c r="J4" s="28">
+        <v>85290</v>
+      </c>
+      <c r="K4" s="28">
+        <v>88134</v>
+      </c>
+      <c r="L4" s="28">
+        <v>95220</v>
+      </c>
+      <c r="M4" s="28">
+        <v>91501</v>
+      </c>
+      <c r="N4" s="28">
+        <v>101750</v>
+      </c>
+      <c r="O4" s="28">
+        <v>104884</v>
+      </c>
+      <c r="P4" s="28">
+        <v>112773</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>127219</v>
+      </c>
+      <c r="R4" s="28">
+        <v>133136</v>
+      </c>
+      <c r="S4" s="28">
+        <v>130111</v>
+      </c>
+      <c r="T4" s="28">
+        <v>132103</v>
+      </c>
+      <c r="U4" s="28">
+        <v>144849</v>
+      </c>
+      <c r="V4" s="28">
+        <v>152013</v>
+      </c>
+      <c r="W4" s="28">
+        <v>149378</v>
+      </c>
+      <c r="X4" s="28">
+        <v>128106</v>
+      </c>
+      <c r="Y4" s="28">
+        <v>87790</v>
+      </c>
+      <c r="Z4" s="28">
+        <v>78047</v>
+      </c>
+      <c r="AA4" s="28">
+        <v>46043</v>
+      </c>
+      <c r="AB4" s="28">
+        <v>15415</v>
+      </c>
+      <c r="AC4" s="28">
+        <v>2942</v>
       </c>
     </row>
   </sheetData>
@@ -4472,14 +4923,14 @@
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1">
         <v>2001</v>
       </c>
@@ -4490,7 +4941,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4507,7 +4958,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4521,7 +4972,7 @@
         <v>3547614</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -4535,7 +4986,7 @@
         <v>13817</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4549,7 +5000,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4563,7 +5014,7 @@
         <v>24131</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4577,7 +5028,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4591,7 +5042,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -4605,7 +5056,7 @@
         <v>7862</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -4619,7 +5070,7 @@
         <v>10315</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -4633,7 +5084,7 @@
         <v>3555</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -4647,7 +5098,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -4661,7 +5112,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -4675,7 +5126,7 @@
         <v>17980</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -4689,7 +5140,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -4703,7 +5154,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -4717,7 +5168,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -4731,7 +5182,7 @@
         <v>3688</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -4745,7 +5196,7 @@
         <v>7729</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -4759,7 +5210,7 @@
         <v>123892</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -4773,7 +5224,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -4787,7 +5238,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -4801,7 +5252,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -4815,7 +5266,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -4829,7 +5280,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -4843,7 +5294,7 @@
         <v>22178</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -4857,7 +5308,7 @@
         <v>12712</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -4871,7 +5322,7 @@
         <v>22388</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -4898,14 +5349,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -4934,7 +5385,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -4971,7 +5422,7 @@
         <v>3871833</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -5000,7 +5451,7 @@
         <v>1865129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -5042,14 +5493,14 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="19.2" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -5111,7 +5562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -5174,7 +5625,7 @@
         <v>91851</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -5236,7 +5687,7 @@
         <v>17364</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -5298,7 +5749,7 @@
         <v>2182</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -5361,7 +5812,7 @@
         <v>2668</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -5423,7 +5874,7 @@
         <v>3273</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -5485,7 +5936,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -5547,7 +5998,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -5609,7 +6060,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -5671,7 +6122,7 @@
         <v>2402</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -5733,7 +6184,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -5795,7 +6246,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -5857,7 +6308,7 @@
         <v>3436</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -5919,7 +6370,7 @@
         <v>5137</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -5981,7 +6432,7 @@
         <v>3460</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -6043,7 +6494,7 @@
         <v>1552</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -6105,7 +6556,7 @@
         <v>5419</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -6168,7 +6619,7 @@
         <v>5996</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -6230,7 +6681,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -6292,7 +6743,7 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -6354,7 +6805,7 @@
         <v>10018</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -6416,7 +6867,7 @@
         <v>7470</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -6495,7 +6946,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -6509,7 +6960,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -6586,7 +7037,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -6663,7 +7114,7 @@
         <v>36508</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -6740,7 +7191,7 @@
         <v>8030</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -6817,7 +7268,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -6894,7 +7345,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -6971,7 +7422,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -7048,7 +7499,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -7125,7 +7576,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -7202,7 +7653,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -7279,7 +7730,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -7356,7 +7807,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -7433,7 +7884,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -7510,7 +7961,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -7587,7 +8038,7 @@
         <v>2352</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -7664,7 +8115,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -7741,7 +8192,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -7818,7 +8269,7 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -7895,7 +8346,7 @@
         <v>2830</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -7972,7 +8423,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -8049,7 +8500,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -8126,7 +8577,7 @@
         <v>4211</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -8203,7 +8654,7 @@
         <v>2154</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -8307,7 +8758,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -8321,7 +8772,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -8398,7 +8849,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -8475,7 +8926,7 @@
         <v>62712</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -8552,7 +9003,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -8629,7 +9080,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -8706,7 +9157,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -8783,7 +9234,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -8860,7 +9311,7 @@
         <v>1315</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -8937,7 +9388,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -9014,7 +9465,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -9091,7 +9542,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -9168,7 +9619,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -9245,7 +9696,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -9322,7 +9773,7 @@
         <v>2316</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -9399,7 +9850,7 @@
         <v>4619</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -9476,7 +9927,7 @@
         <v>2685</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -9553,7 +10004,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -9630,7 +10081,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -9707,7 +10158,7 @@
         <v>4428</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -9784,7 +10235,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -9861,7 +10312,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -9938,7 +10389,7 @@
         <v>6005</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -10015,7 +10466,7 @@
         <v>4588</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -10119,7 +10570,7 @@
       <selection activeCell="B1" sqref="B1:Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -10133,7 +10584,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -10210,7 +10661,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -10287,7 +10738,7 @@
         <v>18203</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -10364,7 +10815,7 @@
         <v>3671</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -10441,7 +10892,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -10518,7 +10969,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -10595,7 +11046,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -10672,7 +11123,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -10749,7 +11200,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -10826,7 +11277,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -10903,7 +11354,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -10980,7 +11431,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -11057,7 +11508,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -11134,7 +11585,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -11211,7 +11662,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -11288,7 +11739,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -11365,7 +11816,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -11442,7 +11893,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -11519,7 +11970,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -11596,7 +12047,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -11673,7 +12124,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -11750,7 +12201,7 @@
         <v>2158</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -11827,7 +12278,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -11928,7 +12379,7 @@
       <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="25.6640625" style="6" customWidth="1"/>
     <col min="2" max="4" width="6.44140625" style="6" customWidth="1"/>
@@ -11942,7 +12393,7 @@
     <col min="26" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -12019,7 +12470,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -12096,7 +12547,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25">
       <c r="A3" s="17" t="s">
         <v>31</v>
       </c>
@@ -12173,7 +12624,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -12250,7 +12701,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -12327,7 +12778,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25">
       <c r="A6" s="17" t="s">
         <v>56</v>
       </c>
@@ -12404,7 +12855,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25">
       <c r="A7" s="17" t="s">
         <v>57</v>
       </c>
@@ -12481,7 +12932,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25">
       <c r="A8" s="17" t="s">
         <v>58</v>
       </c>
@@ -12558,7 +13009,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25">
       <c r="A9" s="17" t="s">
         <v>59</v>
       </c>
@@ -12635,7 +13086,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -12712,7 +13163,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25">
       <c r="A11" s="17" t="s">
         <v>28</v>
       </c>
@@ -12789,7 +13240,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25">
       <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
@@ -12866,7 +13317,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25">
       <c r="A13" s="17" t="s">
         <v>60</v>
       </c>
@@ -12943,7 +13394,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25">
       <c r="A14" s="17" t="s">
         <v>61</v>
       </c>
@@ -13020,7 +13471,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25">
       <c r="A15" s="17" t="s">
         <v>62</v>
       </c>
@@ -13097,7 +13548,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25">
       <c r="A16" s="17" t="s">
         <v>63</v>
       </c>
@@ -13174,7 +13625,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -13251,7 +13702,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25">
       <c r="A18" s="17" t="s">
         <v>64</v>
       </c>
@@ -13328,7 +13779,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25">
       <c r="A19" s="17" t="s">
         <v>65</v>
       </c>
@@ -13405,7 +13856,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25">
       <c r="A20" s="17" t="s">
         <v>66</v>
       </c>
@@ -13482,7 +13933,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25">
       <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
@@ -13559,7 +14010,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25">
       <c r="A22" s="17" t="s">
         <v>25</v>
       </c>
@@ -13636,7 +14087,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25">
       <c r="A23" s="17" t="s">
         <v>27</v>
       </c>
@@ -13737,13 +14188,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="28.8">
       <c r="A1" s="26" t="s">
         <v>54</v>
       </c>
@@ -13752,7 +14203,7 @@
       </c>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.4">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -13761,7 +14212,7 @@
         <v>717026</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.4" customHeight="1">
       <c r="A3" s="23" t="s">
         <v>31</v>
       </c>
@@ -13770,7 +14221,7 @@
       </c>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.4" customHeight="1">
       <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
@@ -13779,7 +14230,7 @@
       </c>
       <c r="C4" s="20"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.4" customHeight="1">
       <c r="A5" s="23" t="s">
         <v>23</v>
       </c>
@@ -13788,7 +14239,7 @@
       </c>
       <c r="C5" s="20"/>
     </row>
-    <row r="6" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="14.4" customHeight="1">
       <c r="A6" s="23" t="s">
         <v>56</v>
       </c>
@@ -13797,7 +14248,7 @@
       </c>
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="14.4" customHeight="1">
       <c r="A7" s="23" t="s">
         <v>57</v>
       </c>
@@ -13806,7 +14257,7 @@
       </c>
       <c r="C7" s="20"/>
     </row>
-    <row r="8" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="14.4" customHeight="1">
       <c r="A8" s="23" t="s">
         <v>58</v>
       </c>
@@ -13815,7 +14266,7 @@
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="14.4" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>59</v>
       </c>
@@ -13824,7 +14275,7 @@
       </c>
       <c r="C9" s="20"/>
     </row>
-    <row r="10" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="14.4" customHeight="1">
       <c r="A10" s="23" t="s">
         <v>24</v>
       </c>
@@ -13833,7 +14284,7 @@
       </c>
       <c r="C10" s="20"/>
     </row>
-    <row r="11" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="14.4" customHeight="1">
       <c r="A11" s="23" t="s">
         <v>28</v>
       </c>
@@ -13842,7 +14293,7 @@
       </c>
       <c r="C11" s="20"/>
     </row>
-    <row r="12" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="14.4" customHeight="1">
       <c r="A12" s="23" t="s">
         <v>26</v>
       </c>
@@ -13851,7 +14302,7 @@
       </c>
       <c r="C12" s="20"/>
     </row>
-    <row r="13" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="14.4" customHeight="1">
       <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
@@ -13860,7 +14311,7 @@
       </c>
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="14.4" customHeight="1">
       <c r="A14" s="23" t="s">
         <v>61</v>
       </c>
@@ -13869,7 +14320,7 @@
       </c>
       <c r="C14" s="20"/>
     </row>
-    <row r="15" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="14.4" customHeight="1">
       <c r="A15" s="23" t="s">
         <v>62</v>
       </c>
@@ -13878,7 +14329,7 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="14.4" customHeight="1">
       <c r="A16" s="23" t="s">
         <v>63</v>
       </c>
@@ -13887,7 +14338,7 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="14.4" customHeight="1">
       <c r="A17" s="23" t="s">
         <v>30</v>
       </c>
@@ -13896,7 +14347,7 @@
       </c>
       <c r="C17" s="20"/>
     </row>
-    <row r="18" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="14.4" customHeight="1">
       <c r="A18" s="23" t="s">
         <v>64</v>
       </c>
@@ -13905,7 +14356,7 @@
       </c>
       <c r="C18" s="20"/>
     </row>
-    <row r="19" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="14.4" customHeight="1">
       <c r="A19" s="23" t="s">
         <v>65</v>
       </c>
@@ -13914,7 +14365,7 @@
       </c>
       <c r="C19" s="20"/>
     </row>
-    <row r="20" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="14.4" customHeight="1">
       <c r="A20" s="23" t="s">
         <v>66</v>
       </c>
@@ -13923,7 +14374,7 @@
       </c>
       <c r="C20" s="20"/>
     </row>
-    <row r="21" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="14.4" customHeight="1">
       <c r="A21" s="23" t="s">
         <v>29</v>
       </c>
@@ -13932,7 +14383,7 @@
       </c>
       <c r="C21" s="20"/>
     </row>
-    <row r="22" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="14.4" customHeight="1">
       <c r="A22" s="23" t="s">
         <v>25</v>
       </c>
@@ -13941,7 +14392,7 @@
       </c>
       <c r="C22" s="20"/>
     </row>
-    <row r="23" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="14.4" customHeight="1">
       <c r="A23" s="23" t="s">
         <v>27</v>
       </c>
@@ -13950,7 +14401,7 @@
       </c>
       <c r="C23" s="20"/>
     </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="14.4" customHeight="1">
       <c r="A24" s="24" t="s">
         <v>22</v>
       </c>
@@ -13959,7 +14410,7 @@
       </c>
       <c r="C24" s="20"/>
     </row>
-    <row r="25" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="14.4">
       <c r="C25" s="20"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dodani podatci u dataset potrebni za dobno spolnu piramidu
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\ProjektR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDF4155-4C2F-457E-B073-CFF6D2AC04BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7A81D5-8DFC-42BC-A1D4-312DB563D0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="10" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="3120" yWindow="3444" windowWidth="17304" windowHeight="8892" firstSheet="7" activeTab="11" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="E-gradani" sheetId="9" r:id="rId9"/>
     <sheet name="Doseljeni" sheetId="10" r:id="rId10"/>
     <sheet name="Odseljeni" sheetId="11" r:id="rId11"/>
+    <sheet name="dobno_spolna" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="112">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -282,6 +283,117 @@
   <si>
     <t>Broj_stanovnika_2021</t>
   </si>
+  <si>
+    <t>Županija</t>
+  </si>
+  <si>
+    <t>Jedinica lokalne samouprave</t>
+  </si>
+  <si>
+    <t>County of</t>
+  </si>
+  <si>
+    <t>Local self-government unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grad/općina  
+Town/Municipality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naselje
+Settlement </t>
+  </si>
+  <si>
+    <t>Spol</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Ukupno
+Total</t>
+  </si>
+  <si>
+    <t>0 – 4</t>
+  </si>
+  <si>
+    <t>5 – 9</t>
+  </si>
+  <si>
+    <t>10 – 14</t>
+  </si>
+  <si>
+    <t>15 – 19</t>
+  </si>
+  <si>
+    <t>20 – 24</t>
+  </si>
+  <si>
+    <t>25 – 29</t>
+  </si>
+  <si>
+    <t>30 – 34</t>
+  </si>
+  <si>
+    <t>35 – 39</t>
+  </si>
+  <si>
+    <t>40 – 44</t>
+  </si>
+  <si>
+    <t>45 – 49</t>
+  </si>
+  <si>
+    <t>50 – 54</t>
+  </si>
+  <si>
+    <t>55 – 59</t>
+  </si>
+  <si>
+    <t>60 – 64</t>
+  </si>
+  <si>
+    <t>65 – 69</t>
+  </si>
+  <si>
+    <t>70 – 74</t>
+  </si>
+  <si>
+    <t>75 – 79</t>
+  </si>
+  <si>
+    <t>80 – 84</t>
+  </si>
+  <si>
+    <t>85 – 89</t>
+  </si>
+  <si>
+    <t>90 – 94</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Republic of Croatia</t>
+  </si>
+  <si>
+    <t>sv.</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ž</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
 </sst>
 </file>
 
@@ -495,7 +607,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -569,6 +681,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3480,7 +3596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F98E4D1-812A-43FC-A5E2-E0E4232BE4B7}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+    <sheetView zoomScale="92" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4457,6 +4573,341 @@
       </c>
       <c r="N22">
         <v>4830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5311FF31-F4DD-4C20-A6CC-31D396DD68FD}">
+  <dimension ref="A1:AC4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:29" ht="55.8" customHeight="1">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+      <c r="N1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S1" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="28">
+        <v>3871833</v>
+      </c>
+      <c r="J2" s="28">
+        <v>175535</v>
+      </c>
+      <c r="K2" s="28">
+        <v>181445</v>
+      </c>
+      <c r="L2" s="28">
+        <v>195436</v>
+      </c>
+      <c r="M2" s="28">
+        <v>188729</v>
+      </c>
+      <c r="N2" s="28">
+        <v>208852</v>
+      </c>
+      <c r="O2" s="28">
+        <v>214023</v>
+      </c>
+      <c r="P2" s="28">
+        <v>227551</v>
+      </c>
+      <c r="Q2" s="28">
+        <v>255617</v>
+      </c>
+      <c r="R2" s="28">
+        <v>267349</v>
+      </c>
+      <c r="S2" s="28">
+        <v>260146</v>
+      </c>
+      <c r="T2" s="28">
+        <v>260056</v>
+      </c>
+      <c r="U2" s="28">
+        <v>279504</v>
+      </c>
+      <c r="V2" s="28">
+        <v>288351</v>
+      </c>
+      <c r="W2" s="28">
+        <v>279106</v>
+      </c>
+      <c r="X2" s="28">
+        <v>228612</v>
+      </c>
+      <c r="Y2" s="28">
+        <v>146855</v>
+      </c>
+      <c r="Z2" s="28">
+        <v>122719</v>
+      </c>
+      <c r="AA2" s="28">
+        <v>67249</v>
+      </c>
+      <c r="AB2" s="28">
+        <v>21019</v>
+      </c>
+      <c r="AC2" s="28">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="28">
+        <v>1865129</v>
+      </c>
+      <c r="J3" s="28">
+        <v>90245</v>
+      </c>
+      <c r="K3" s="28">
+        <v>93311</v>
+      </c>
+      <c r="L3" s="28">
+        <v>100216</v>
+      </c>
+      <c r="M3" s="28">
+        <v>97228</v>
+      </c>
+      <c r="N3" s="28">
+        <v>107102</v>
+      </c>
+      <c r="O3" s="28">
+        <v>109139</v>
+      </c>
+      <c r="P3" s="28">
+        <v>114778</v>
+      </c>
+      <c r="Q3" s="28">
+        <v>128398</v>
+      </c>
+      <c r="R3" s="28">
+        <v>134213</v>
+      </c>
+      <c r="S3" s="28">
+        <v>130035</v>
+      </c>
+      <c r="T3" s="28">
+        <v>127953</v>
+      </c>
+      <c r="U3" s="28">
+        <v>134655</v>
+      </c>
+      <c r="V3" s="28">
+        <v>136338</v>
+      </c>
+      <c r="W3" s="28">
+        <v>129728</v>
+      </c>
+      <c r="X3" s="28">
+        <v>100506</v>
+      </c>
+      <c r="Y3" s="28">
+        <v>59065</v>
+      </c>
+      <c r="Z3" s="28">
+        <v>44672</v>
+      </c>
+      <c r="AA3" s="28">
+        <v>21206</v>
+      </c>
+      <c r="AB3" s="28">
+        <v>5604</v>
+      </c>
+      <c r="AC3">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I4" s="28">
+        <v>2006704</v>
+      </c>
+      <c r="J4" s="28">
+        <v>85290</v>
+      </c>
+      <c r="K4" s="28">
+        <v>88134</v>
+      </c>
+      <c r="L4" s="28">
+        <v>95220</v>
+      </c>
+      <c r="M4" s="28">
+        <v>91501</v>
+      </c>
+      <c r="N4" s="28">
+        <v>101750</v>
+      </c>
+      <c r="O4" s="28">
+        <v>104884</v>
+      </c>
+      <c r="P4" s="28">
+        <v>112773</v>
+      </c>
+      <c r="Q4" s="28">
+        <v>127219</v>
+      </c>
+      <c r="R4" s="28">
+        <v>133136</v>
+      </c>
+      <c r="S4" s="28">
+        <v>130111</v>
+      </c>
+      <c r="T4" s="28">
+        <v>132103</v>
+      </c>
+      <c r="U4" s="28">
+        <v>144849</v>
+      </c>
+      <c r="V4" s="28">
+        <v>152013</v>
+      </c>
+      <c r="W4" s="28">
+        <v>149378</v>
+      </c>
+      <c r="X4" s="28">
+        <v>128106</v>
+      </c>
+      <c r="Y4" s="28">
+        <v>87790</v>
+      </c>
+      <c r="Z4" s="28">
+        <v>78047</v>
+      </c>
+      <c r="AA4" s="28">
+        <v>46043</v>
+      </c>
+      <c r="AB4" s="28">
+        <v>15415</v>
+      </c>
+      <c r="AC4" s="28">
+        <v>2942</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Evo belce fun factovi
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maks\Desktop\ProjektR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7A81D5-8DFC-42BC-A1D4-312DB563D0A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B450268-835D-4493-8682-09774C93DDCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3444" windowWidth="17304" windowHeight="8892" firstSheet="7" activeTab="11" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15720" firstSheet="7" activeTab="12" xr2:uid="{A58E9493-977D-4296-9BB5-F9B5EFAF25FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Stanovnistvo" sheetId="7" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="Doseljeni" sheetId="10" r:id="rId10"/>
     <sheet name="Odseljeni" sheetId="11" r:id="rId11"/>
     <sheet name="dobno_spolna" sheetId="12" r:id="rId12"/>
+    <sheet name="Stat" sheetId="13" r:id="rId13"/>
+    <sheet name="FunFacts" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Brakovi!$A:$A,Brakovi!$1:$1</definedName>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="209">
   <si>
     <t>Republika Hrvatska</t>
   </si>
@@ -393,6 +395,297 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>Grad Zagreb je svoj vrhunac stanovništva doživio 2020. godine, do te brojke je došao sporim i kontinuiranim rastom dok je već sljedeće godine izgubio više od 40 tisuća stanovnika i dosegao svoju najlošiju godinu 21. stoljeća.</t>
+  </si>
+  <si>
+    <t>Grad Zagreb je najmanji broj rođenih bilježio 2001. i 2002. godine, upravo godine kada su rođeni kreatori ove stranice. :)</t>
+  </si>
+  <si>
+    <t>Međimurska županija 2006. godine ostvaruje svoj maksimum po broju stanovnika, a od tada je u padu i 2021. doživljava svoje najniže brojke.</t>
+  </si>
+  <si>
+    <t>Međimurska županije ima najveću brojku rođenih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Krapinsko-zagorska u zadnjih 20 godina ima kontinuirani pad i novim popisom je doživjela najnižu razinu sa malo iznad 120 tisuća stanovnika.</t>
+  </si>
+  <si>
+    <t>Varaždinska županija od 2001. doživljava kontinuirani, ali svom srećom, blagi pad u broju stanovnika.</t>
+  </si>
+  <si>
+    <t>U Varaždinskoj županiji, najveći broj stanovnika ima raspon godina 55-59 što je jedna od najstarijih skupina gledajući sve županije.</t>
+  </si>
+  <si>
+    <t>Virovitičko-podravska je jedna od samo tri županije koja imaju manje od 100 tisuća stanovnika</t>
+  </si>
+  <si>
+    <t>Virovitičko-podravska županija ima najmanji broj brakova na 1000 stanovnika u protekloj godini.</t>
+  </si>
+  <si>
+    <t>Požeško-slavonska je jedna od samo tri županije koja imaju manje od 100 tisuća stanovnika</t>
+  </si>
+  <si>
+    <t>Iako ima godišnji prosjek od preko 760 i maksimum sa više od 1000 rođenih, Požeško-slavonska je u 2021. godini imala samo 572 rođene djece.</t>
+  </si>
+  <si>
+    <t>Požeško-slavonska županija osvaja 1. mjesto po broju odseljenih ljudi u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Bjelovarsko-bilogorska županija zauzima mjesto u top 3 po najvećem broju umrlih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t>U Vukovarsko-srijemskoj, najveći broj stanovnika bilježi između 60 i 64 godine.</t>
+  </si>
+  <si>
+    <t>U Brodsko-posavskoj, najveći broj stanovnika bilježi između 60 i 64 godine.</t>
+  </si>
+  <si>
+    <t>Karlovačka županija ima jedan od najgorih odnosa rođenih i umrlih od svih županija.</t>
+  </si>
+  <si>
+    <t>Karlovačka županija ima kontinuirani rast po broju razvoda na 1000 stanovnika i od jedne od najboljih županija je migrirala u najgoru!</t>
+  </si>
+  <si>
+    <t>Osječko-baranjska je jedna od rijetkih županija koja zadnjih godina doživljava rast po pitanju rođene djece.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka ima jedan od najgorih odnosa rođenih i umrlih od svih županija.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka županija zauzima mjesto u top 5 po najvećem broju umrlih na 1000 stanovnika u 2021. godini.</t>
+  </si>
+  <si>
+    <t>Naša najmanja županija, Ličko-senjska, svakom godinom postaje sve manja...</t>
+  </si>
+  <si>
+    <t>Ličko-senjska je županija sa najmanje rođenih, a brojka već dugo nije prešla 400.</t>
+  </si>
+  <si>
+    <t>Iako ima najmanje umrlih, Ličko-senjska broji dva puta više umrlih od rođenih.</t>
+  </si>
+  <si>
+    <t>Po prvi puta u zadnjih 20 godina, Istarska županija pala je ispod 200 tisuća stanovnika.</t>
+  </si>
+  <si>
+    <t>Istarska županija ima najviše brakova na 1000 stanovnika u 2021. godini!</t>
+  </si>
+  <si>
+    <t>Istarska županija je rekorder po broju doseljenih na 1000 stanovnika!</t>
+  </si>
+  <si>
+    <t>Zagrebačka je jedna od samo dvije županije koja u prošloj godini nije doživjela najnižu brojku u zadnjih 20 godina.</t>
+  </si>
+  <si>
+    <t>U Šibensko-kninskoj, najveći broj stanovnika bilježi između 65 i 69 godina.</t>
+  </si>
+  <si>
+    <t>Dubrovačko-neretvanska županija krasi se jednom od najmanjih oscilacija u proteklih 20 godina.</t>
+  </si>
+  <si>
+    <t>U proteklih 20 godina, Dubrovačko-neretvanska je rekorder po broju rođenih na 1000 stanovnika u jednoj godini, a vrhunac je doživjela 2008. godine.</t>
+  </si>
+  <si>
+    <t>Druga najveća županija naše države je ponos Dalmacije, Splitsko-dalmatinska!</t>
+  </si>
+  <si>
+    <t>Splitsko-dalmatinska ima duplo više umrlih od rođenih.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primorsko-goranska županija je, kao i ostale, doživjela veliki pad u broju stanovnika 2021. godine. </t>
+  </si>
+  <si>
+    <t>U Primorsko-goranskoj županiji se ljudi vole! Županija sa najmanje razvoda na 1000 stanovnika u protekloj godini!</t>
+  </si>
+  <si>
+    <t>Druga po broju odseljenih na 1000 stanovnika u prošloj godini - Primorsko-goranska!</t>
+  </si>
+  <si>
+    <t>Zadarska je jedna od samo dvije županije koja u prošloj godini nije doživjela najnižu brojku u zadnjih 20 godina.</t>
+  </si>
+  <si>
+    <t>U centru Zagreba nalazi se najmanja žičana željeznica na svijetu, a povezuje Donji i Gornji grad.</t>
+  </si>
+  <si>
+    <t>Lenucijeva potkova, kompleks od 7 trgova i parkova u centru Zagreba, prepuna je zelenila i može biti put za predivnu šetnju gradom!</t>
+  </si>
+  <si>
+    <t>Grad Zagreb dom je najvećeg i najuspješnijeg hrvatskog nogometnog kluba, Dinama.</t>
+  </si>
+  <si>
+    <t>U Međimurskoj županiji nalazi se najsjevernija točka naše države.</t>
+  </si>
+  <si>
+    <t>Prvo nalazište nafte u Hrvatskoj pronađeno je upravo u Međimurju, u mjestu Peklenica.</t>
+  </si>
+  <si>
+    <t>Međimurci su ispleli najveću košaru od šibe koja je priznata u cijelome svijetu!</t>
+  </si>
+  <si>
+    <t>U Krapinskoj-zagorskoj županiji nalazi se Marija Bistrica, najveće hrvatsko svetište Majke Božje.</t>
+  </si>
+  <si>
+    <t>Na Hušnjakovu brijegu u Krapinsko-zagorskoj županiji nalazi se jedno od najstarijih nalazišta pračovjeka u Europi te ima i muzej posvećen tome.</t>
+  </si>
+  <si>
+    <t>Krapinsko-zagorska županija odlikuje se nejvećim brojem dvoraca po četvornom kilometru u Hrvatskoj.</t>
+  </si>
+  <si>
+    <t>Sjedište Varaždinske županije, Varaždin, je bivši hrvatski glavni grad, a Ludbreg je poznat kao centar svijeta!</t>
+  </si>
+  <si>
+    <t>U Varaždinskoj županiji nalazi se špilja Vindija u kojoj su otkriveni ostaci neandertalskog pračovjeka.</t>
+  </si>
+  <si>
+    <t>U Varaždinu će se 2023. godine održati svjetsko seniorsko kuglačko prvenstvo!</t>
+  </si>
+  <si>
+    <t>Dvorac Trakošćan jedan je od najljepših dvoraca u Hrvatskoj i nalazi se u Varaždinskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Slatini je proizveden prvi hrvatski pjenušac i na ponos je Virovitičko-podravske županije.</t>
+  </si>
+  <si>
+    <t>Park prirode Papuk odlično je mjesto za ljubitelje prirode, a nalazi se u Virovitičko-podravskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Virovitici je 1242. godine hrvatsko-ugarski kralj Bela IV. Izdao Zlatnu bulu kojem je Gradec (današnji Zagreb) stekao status grada!</t>
+  </si>
+  <si>
+    <t>Iako se dio njega nalazi u Virovitičko-podravskoj županiji, Park prirode Papuk prirodna je atrakcija i Požeško-slavonske županije.</t>
+  </si>
+  <si>
+    <t>U Požeško-slavonskoj županiji nalazi se Kutjevo, poznato pod Kutjevu d.d., jednom od naših najvećih proizvođača vina.</t>
+  </si>
+  <si>
+    <t>U Požegi se nalazi velebni Spomenik 123. brigadi Hrvatske vojske.</t>
+  </si>
+  <si>
+    <t>U Koprivnici se nalazi povijesni Franjevački samostan i crkva Sv. Antuna Padovanskog.</t>
+  </si>
+  <si>
+    <t>Gradska palača, izgrađena u 18. stoljeću, vrijedan je dio povijesti koji se isplati vidjeti, a nalazi se u sjedištu županije.</t>
+  </si>
+  <si>
+    <t>Koprivničko-križevačka županija ima sjedište najveće farmaceutske firme u hrvatskom vlasništvu - Belupo!</t>
+  </si>
+  <si>
+    <t>Bjelovarsko-bilogorska županija dom je mnogih poznatih manifestacija koje se rastežu kroz cijelu godinu i uvijek vrijedi otići.</t>
+  </si>
+  <si>
+    <t>Za ljude željne prirode, Bjelovarsko-bilogorska županija nudi opcije kao što su Moslavačka gora, Papuk i Bilogora!</t>
+  </si>
+  <si>
+    <t>Tko se odluči posjetiti Daruvar, može uživati u toplim kupeljima koje sežu još od rimskih vremena.</t>
+  </si>
+  <si>
+    <t>U Vukovarskoj-srijemskoj se nalazi Vučedol, jedan od najznačajnijih lokaliteta neolitika i Vučedolske kulture.</t>
+  </si>
+  <si>
+    <t>Vukovarski vodotoranj jedan je od najvećih spomenika i obilježava velik dio hrvatske povijesti!</t>
+  </si>
+  <si>
+    <t>Najistočnija županija Republike Hrvatske.</t>
+  </si>
+  <si>
+    <t>U Karlovačkoj županiji može se posjetiti Rastoke, poznate i kao "Plitvice u malom", predivan prirodni krajolik sa slapovima i adrenalinskim atrakcijama.</t>
+  </si>
+  <si>
+    <t>Karlovac, grad na 4 rijeke, povijesna je atrakcija koju vrijedi obići.</t>
+  </si>
+  <si>
+    <t>Tko voli stare zidine i dvorce, a nalazi se u Karlovačkoj županiji, ne smije zaobići Stari grad Dubovac.</t>
+  </si>
+  <si>
+    <t>U Đakovu se nalazi predivna katedrala, po kojoj je i grad poznat, a samim time i Osječko-baranjska županija.</t>
+  </si>
+  <si>
+    <t>U Osječko-baranjskoj županiji nalazi se najstariji park prirode u Hrvatskoj - Kopački rit.</t>
+  </si>
+  <si>
+    <t>Baranja je poznato vinsko središte Hrvatske i nezaobilazna postaja za sve vinoljupce!</t>
+  </si>
+  <si>
+    <t>Sisački stari grad dio je povijesti kojim se Sisak ponosi i isplati se posjetiti ga.</t>
+  </si>
+  <si>
+    <t>Lonjsko polje je park prirode Hrvatske i nalazi se u Sisačko-moslavačkoj županiji.</t>
+  </si>
+  <si>
+    <t>Sisačko-moslavačka županija bivše je industrijsko središte Hrvatske, sa sisačkom naftnom rafinerijom i željezarom te kutinskom petrokemijom kao njihovim najvećim pokretačima</t>
+  </si>
+  <si>
+    <t>Plitvička jezera su nezaobilazna atrakcija Ličko-senjske županije, kao i preostala dva nacionalna parka: Paklenica i Sjeverni Velebit!</t>
+  </si>
+  <si>
+    <t>Poznata Kula Nehaj simbol je grada Senja, najstarijeg grada na gornjem Jadranu i ponosa Ličko-senjske županije.</t>
+  </si>
+  <si>
+    <t>Mi Hrvati se ponosimo Nikolom Teslom, a u Ličko-senjskoj županiji možete posjetiti "Memorijalni centar Nikola Tesla"</t>
+  </si>
+  <si>
+    <t>Nacionalni park Brijuni jedan je od najljepših naših parkova, a nalazi se u Istarskoj županiji.</t>
+  </si>
+  <si>
+    <t>U Istri se nalazi najmanji grad na svijetu - Hum!</t>
+  </si>
+  <si>
+    <t>Za gurmane, u Istri je pronađen najveći tartuf na svijetu.</t>
+  </si>
+  <si>
+    <t>Ljubitelji prirode mogu posjetiti Stari grad Samobor i Samoborsko gorje, uz predivnu prirodu može se vidjeti i dvorac iz 13. stoljeća.</t>
+  </si>
+  <si>
+    <t>Tradicionalne kremšnite potječu iz Samobora, delicija poznata diljem svijeta. Gdje bolje probati tako nešto, ako ne u gradu gdje je nastala.</t>
+  </si>
+  <si>
+    <t>U Zagrebačkoj županiji nalazi se najveća hrvatska zračna luka - Zračna luka doktora Franje Tuđmana.</t>
+  </si>
+  <si>
+    <t>Dražen Petrović ili "košarkaški Mozart", najveći i neprežaljeni talent hrvatske košarke, potječe iz Šibenika!</t>
+  </si>
+  <si>
+    <t>Šibenik je prvi grad na svijetu koji je dobio javnu rasvjetu na izmjeničnu električnu struju.</t>
+  </si>
+  <si>
+    <t>Četvrt Varoš u Šibeniku poznata je jer su u njoj stasali velikani hrvatske glazbene scene: Arsen Dedić, Vice Vukov i Mate Mišo Kovač.</t>
+  </si>
+  <si>
+    <t>Dubrovnik je prije bio republika za sebe i to zauzima velik dio njegove povijesti!</t>
+  </si>
+  <si>
+    <t>Dubrovačke zidine su velebna atrakcija i predivan dio povijesti. Na istim tim zidinama snimane su i scene jedne od najpoznatijih svjetskih serija - Game of Thrones.</t>
+  </si>
+  <si>
+    <t>Arboretum Trsteno u blizini Dubrovnika, osnovan je u 15. stoljeću i najstariji je arboretum na svijetu!</t>
+  </si>
+  <si>
+    <t>Grijeh je otići u Split, a ne posjetiti Dioklecijanovu palaču - jednu od najbolje očuvanih rimskih građevina u svijetu!</t>
+  </si>
+  <si>
+    <t>Modra špilja kod mjesta Komiže svjetska je turistička atrakcija i vrijedna obilaska!</t>
+  </si>
+  <si>
+    <t>Na otoku Braču koji je smješten u Splitsko-dalmatinskoj županiji, nalazi se plaža Zlatni rat u mjestu Bol, koja spada u jedne od najljepših plaža na svijetu.</t>
+  </si>
+  <si>
+    <t>Ljubitelji prirode, ako ste u Primorsko-goranskoj županiji, nemojte zaobići njihov nacionalni park Risnjak, nećete požaliti! U obilasku možete navratiti i do Bijelih i Samarskih stijena.</t>
+  </si>
+  <si>
+    <t>Sjedište Primorsko-goranske županije, Rijeka, predivan je grad na obali Jadranskog mora. Ako ju poželite posjetiti u proljetnim ili jesenskim mjesecima, ponesite kišobran!</t>
+  </si>
+  <si>
+    <t>Na otoku Cresu nalazi se prirodni rezervat bjeloglavih supova, ugrožene životinjske vrste.</t>
+  </si>
+  <si>
+    <t>Šetnja obalom može postati posebna ako ste u Zadru! Uz melodične zvukove morskih orgulja i Pozdrav suncu, šetnja će postati lijepa uspomena.</t>
+  </si>
+  <si>
+    <t>U zaleđu Zadra može se posjetiti park prirode Vransko jezero, koji spaja močvaru s raznovrsnim ekosustavom, razvedenu obalu Jadrana i ruralni ambijent Ravnih kotara!</t>
+  </si>
+  <si>
+    <t>Rijeka Zrmanja stvorila je poseban geomorfološki spomenik prirode koji se nalazi prije ušća Zrmanje u Novigradsko more.</t>
   </si>
 </sst>
 </file>
@@ -404,7 +697,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1041A]#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -481,6 +774,14 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -607,7 +908,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
@@ -685,6 +986,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4584,7 +4890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5311FF31-F4DD-4C20-A6CC-31D396DD68FD}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -4908,6 +5214,989 @@
       </c>
       <c r="AC4" s="28">
         <v>2942</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FD651A-1D52-4CBF-BC31-878C268DCCB8}">
+  <dimension ref="A1:B63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.8">
+      <c r="A1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.8">
+      <c r="A2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="31"/>
+    </row>
+    <row r="4" spans="1:2" ht="13.8">
+      <c r="A4" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.8">
+      <c r="A5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="31"/>
+    </row>
+    <row r="7" spans="1:2" ht="13.8">
+      <c r="A7" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="31"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="31"/>
+    </row>
+    <row r="10" spans="1:2" ht="13.8">
+      <c r="A10" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="13.8">
+      <c r="A11" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="31"/>
+    </row>
+    <row r="13" spans="1:2" ht="13.8">
+      <c r="A13" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="13.8">
+      <c r="A14" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="31"/>
+    </row>
+    <row r="16" spans="1:2" ht="13.8">
+      <c r="A16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13.8">
+      <c r="A17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="13.8">
+      <c r="A18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="31"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="31"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="31"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="31"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="31"/>
+    </row>
+    <row r="25" spans="1:2" ht="13.8">
+      <c r="A25" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="31"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="31"/>
+    </row>
+    <row r="28" spans="1:2" ht="13.8">
+      <c r="A28" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="31"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="31"/>
+    </row>
+    <row r="31" spans="1:2" ht="13.8">
+      <c r="A31" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="31"/>
+    </row>
+    <row r="34" spans="1:2" ht="13.8">
+      <c r="A34" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="31"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="31"/>
+    </row>
+    <row r="37" spans="1:2" ht="13.8">
+      <c r="A37" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="31"/>
+    </row>
+    <row r="40" spans="1:2" ht="13.8">
+      <c r="A40" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="13.8">
+      <c r="A41" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="13.8">
+      <c r="A42" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="13.8">
+      <c r="A43" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="30" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="13.8">
+      <c r="A44" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="13.8">
+      <c r="A45" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="13.8">
+      <c r="A46" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="31"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="31"/>
+    </row>
+    <row r="49" spans="1:2" ht="13.8">
+      <c r="A49" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="31"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="31"/>
+    </row>
+    <row r="52" spans="1:2" ht="13.8">
+      <c r="A52" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="31"/>
+    </row>
+    <row r="55" spans="1:2" ht="13.8">
+      <c r="A55" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" s="30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="13.8">
+      <c r="A56" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="31"/>
+    </row>
+    <row r="58" spans="1:2" ht="13.8">
+      <c r="A58" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="30" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="31" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="13.8">
+      <c r="A60" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="13.8">
+      <c r="A61" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" s="31"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40137D81-047E-4C61-9E88-59E0523B9DFE}">
+  <dimension ref="A1:B64"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -14194,7 +15483,7 @@
     <col min="2" max="2" width="23.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4">
+    <row r="1" spans="1:3" ht="28.8">
       <c r="A1" s="26" t="s">
         <v>54</v>
       </c>

</xml_diff>